<commit_message>
Update theo nội dung yêu cầu
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat dia diem/CF0142_Cap nhat dia diem.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat dia diem/CF0142_Cap nhat dia diem.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Update History" sheetId="4" r:id="rId1"/>
@@ -1389,7 +1389,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="304">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2308,19 +2308,10 @@
     <t>Click</t>
   </si>
   <si>
-    <t>CFML000002</t>
-  </si>
-  <si>
     <t>Click Lưu -&gt; Yes -&gt; Mã trùng</t>
   </si>
   <si>
-    <t>CFML000003</t>
-  </si>
-  <si>
     <t>Click Lưu -&gt; Yes</t>
-  </si>
-  <si>
-    <t>CFML000007</t>
   </si>
   <si>
     <t>Change</t>
@@ -2542,9 +2533,6 @@
     <t>Combo</t>
   </si>
   <si>
-    <t>CFML000026</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mục đổ Combobox </t>
   </si>
   <si>
@@ -2559,15 +2547,27 @@
     <t>Tham khảo luồng nghiệp vụ 2</t>
   </si>
   <si>
+    <t>CustomizeIndex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CustomizeIndex </t>
+  </si>
+  <si>
+    <t>00ML000016</t>
+  </si>
+  <si>
+    <t>00ML000053</t>
+  </si>
+  <si>
+    <t>00ML000001</t>
+  </si>
+  <si>
+    <t>00ML000015</t>
+  </si>
+  <si>
     <t>- Thực thi @SQL0002 Kiểm tra điều kiện trước khi lưu 
-  + Nếu =1, cảnh bảo message CFML000003 và không cho lưu
-  + Nếu =0, thực thi câu @SQL0003 để Insert dữ liệu, Confirm message CFML000007 và @SQL0004 để Load dữ liệu lên Form CF0141</t>
-  </si>
-  <si>
-    <t>CustomizeIndex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CustomizeIndex </t>
+  + Nếu =1, cảnh bảo message 00ML000053 và không cho lưu
+  + Nếu =0, thực thi câu @SQL0003 để Insert dữ liệu, Confirm message 00ML000015 và @SQL0004 để Load dữ liệu lên Form CF0141</t>
   </si>
 </sst>
 </file>
@@ -3364,6 +3364,9 @@
     <xf numFmtId="6" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3528,9 +3531,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3915,10 +3915,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
+      <c r="B1" s="146"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -3945,8 +3945,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -3985,14 +3985,14 @@
       <c r="D4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="146" t="s">
+      <c r="E4" s="147" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
-      <c r="J4" s="146"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="147"/>
+      <c r="H4" s="147"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
     </row>
     <row r="5" spans="1:10" s="25" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="116">
@@ -4008,14 +4008,14 @@
         <f>H1</f>
         <v>Thị Phượng</v>
       </c>
-      <c r="E5" s="147" t="s">
+      <c r="E5" s="148" t="s">
         <v>226</v>
       </c>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
-      <c r="H5" s="148"/>
-      <c r="I5" s="148"/>
-      <c r="J5" s="148"/>
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
+      <c r="H5" s="149"/>
+      <c r="I5" s="149"/>
+      <c r="J5" s="149"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="87">
@@ -4026,12 +4026,12 @@
       </c>
       <c r="C6" s="77"/>
       <c r="D6" s="64"/>
-      <c r="E6" s="149"/>
-      <c r="F6" s="150"/>
-      <c r="G6" s="150"/>
-      <c r="H6" s="150"/>
-      <c r="I6" s="150"/>
-      <c r="J6" s="151"/>
+      <c r="E6" s="150"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="151"/>
+      <c r="J6" s="152"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="88">
@@ -4042,12 +4042,12 @@
       </c>
       <c r="C7" s="78"/>
       <c r="D7" s="40"/>
-      <c r="E7" s="139"/>
-      <c r="F7" s="140"/>
-      <c r="G7" s="140"/>
-      <c r="H7" s="140"/>
-      <c r="I7" s="140"/>
-      <c r="J7" s="141"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="141"/>
+      <c r="G7" s="141"/>
+      <c r="H7" s="141"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="142"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="89">
@@ -4058,12 +4058,12 @@
       </c>
       <c r="C8" s="78"/>
       <c r="D8" s="40"/>
-      <c r="E8" s="142"/>
-      <c r="F8" s="143"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="143"/>
-      <c r="I8" s="143"/>
-      <c r="J8" s="144"/>
+      <c r="E8" s="143"/>
+      <c r="F8" s="144"/>
+      <c r="G8" s="144"/>
+      <c r="H8" s="144"/>
+      <c r="I8" s="144"/>
+      <c r="J8" s="145"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="90">
@@ -4074,12 +4074,12 @@
       </c>
       <c r="C9" s="78"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="139"/>
-      <c r="F9" s="140"/>
-      <c r="G9" s="140"/>
-      <c r="H9" s="140"/>
-      <c r="I9" s="140"/>
-      <c r="J9" s="141"/>
+      <c r="E9" s="140"/>
+      <c r="F9" s="141"/>
+      <c r="G9" s="141"/>
+      <c r="H9" s="141"/>
+      <c r="I9" s="141"/>
+      <c r="J9" s="142"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="91">
@@ -4090,12 +4090,12 @@
       </c>
       <c r="C10" s="78"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="139"/>
-      <c r="F10" s="140"/>
-      <c r="G10" s="140"/>
-      <c r="H10" s="140"/>
-      <c r="I10" s="140"/>
-      <c r="J10" s="141"/>
+      <c r="E10" s="140"/>
+      <c r="F10" s="141"/>
+      <c r="G10" s="141"/>
+      <c r="H10" s="141"/>
+      <c r="I10" s="141"/>
+      <c r="J10" s="142"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="92">
@@ -4106,12 +4106,12 @@
       </c>
       <c r="C11" s="78"/>
       <c r="D11" s="40"/>
-      <c r="E11" s="139"/>
-      <c r="F11" s="140"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="140"/>
-      <c r="I11" s="140"/>
-      <c r="J11" s="141"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="141"/>
+      <c r="G11" s="141"/>
+      <c r="H11" s="141"/>
+      <c r="I11" s="141"/>
+      <c r="J11" s="142"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="93">
@@ -4122,12 +4122,12 @@
       </c>
       <c r="C12" s="78"/>
       <c r="D12" s="40"/>
-      <c r="E12" s="139"/>
-      <c r="F12" s="140"/>
-      <c r="G12" s="140"/>
-      <c r="H12" s="140"/>
-      <c r="I12" s="140"/>
-      <c r="J12" s="141"/>
+      <c r="E12" s="140"/>
+      <c r="F12" s="141"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="141"/>
+      <c r="J12" s="142"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="94">
@@ -4138,12 +4138,12 @@
       </c>
       <c r="C13" s="78"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="139"/>
-      <c r="F13" s="140"/>
-      <c r="G13" s="140"/>
-      <c r="H13" s="140"/>
-      <c r="I13" s="140"/>
-      <c r="J13" s="141"/>
+      <c r="E13" s="140"/>
+      <c r="F13" s="141"/>
+      <c r="G13" s="141"/>
+      <c r="H13" s="141"/>
+      <c r="I13" s="141"/>
+      <c r="J13" s="142"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="95">
@@ -4154,12 +4154,12 @@
       </c>
       <c r="C14" s="78"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="139"/>
-      <c r="F14" s="140"/>
-      <c r="G14" s="140"/>
-      <c r="H14" s="140"/>
-      <c r="I14" s="140"/>
-      <c r="J14" s="141"/>
+      <c r="E14" s="140"/>
+      <c r="F14" s="141"/>
+      <c r="G14" s="141"/>
+      <c r="H14" s="141"/>
+      <c r="I14" s="141"/>
+      <c r="J14" s="142"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="40">
@@ -4170,12 +4170,12 @@
       </c>
       <c r="C15" s="78"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="152"/>
-      <c r="F15" s="152"/>
-      <c r="G15" s="152"/>
-      <c r="H15" s="152"/>
-      <c r="I15" s="152"/>
-      <c r="J15" s="152"/>
+      <c r="E15" s="153"/>
+      <c r="F15" s="153"/>
+      <c r="G15" s="153"/>
+      <c r="H15" s="153"/>
+      <c r="I15" s="153"/>
+      <c r="J15" s="153"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="87">
@@ -4186,12 +4186,12 @@
       </c>
       <c r="C16" s="78"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="152"/>
-      <c r="F16" s="152"/>
-      <c r="G16" s="152"/>
-      <c r="H16" s="152"/>
-      <c r="I16" s="152"/>
-      <c r="J16" s="152"/>
+      <c r="E16" s="153"/>
+      <c r="F16" s="153"/>
+      <c r="G16" s="153"/>
+      <c r="H16" s="153"/>
+      <c r="I16" s="153"/>
+      <c r="J16" s="153"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="88">
@@ -4202,12 +4202,12 @@
       </c>
       <c r="C17" s="78"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="152"/>
-      <c r="F17" s="152"/>
-      <c r="G17" s="152"/>
-      <c r="H17" s="152"/>
-      <c r="I17" s="152"/>
-      <c r="J17" s="152"/>
+      <c r="E17" s="153"/>
+      <c r="F17" s="153"/>
+      <c r="G17" s="153"/>
+      <c r="H17" s="153"/>
+      <c r="I17" s="153"/>
+      <c r="J17" s="153"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="89">
@@ -4218,12 +4218,12 @@
       </c>
       <c r="C18" s="78"/>
       <c r="D18" s="40"/>
-      <c r="E18" s="152"/>
-      <c r="F18" s="152"/>
-      <c r="G18" s="152"/>
-      <c r="H18" s="152"/>
-      <c r="I18" s="152"/>
-      <c r="J18" s="152"/>
+      <c r="E18" s="153"/>
+      <c r="F18" s="153"/>
+      <c r="G18" s="153"/>
+      <c r="H18" s="153"/>
+      <c r="I18" s="153"/>
+      <c r="J18" s="153"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="90">
@@ -4234,12 +4234,12 @@
       </c>
       <c r="C19" s="78"/>
       <c r="D19" s="40"/>
-      <c r="E19" s="152"/>
-      <c r="F19" s="152"/>
-      <c r="G19" s="152"/>
-      <c r="H19" s="152"/>
-      <c r="I19" s="152"/>
-      <c r="J19" s="152"/>
+      <c r="E19" s="153"/>
+      <c r="F19" s="153"/>
+      <c r="G19" s="153"/>
+      <c r="H19" s="153"/>
+      <c r="I19" s="153"/>
+      <c r="J19" s="153"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="91">
@@ -4250,12 +4250,12 @@
       </c>
       <c r="C20" s="78"/>
       <c r="D20" s="40"/>
-      <c r="E20" s="152"/>
-      <c r="F20" s="152"/>
-      <c r="G20" s="152"/>
-      <c r="H20" s="152"/>
-      <c r="I20" s="152"/>
-      <c r="J20" s="152"/>
+      <c r="E20" s="153"/>
+      <c r="F20" s="153"/>
+      <c r="G20" s="153"/>
+      <c r="H20" s="153"/>
+      <c r="I20" s="153"/>
+      <c r="J20" s="153"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="92">
@@ -4266,12 +4266,12 @@
       </c>
       <c r="C21" s="78"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="152"/>
-      <c r="F21" s="152"/>
-      <c r="G21" s="152"/>
-      <c r="H21" s="152"/>
-      <c r="I21" s="152"/>
-      <c r="J21" s="152"/>
+      <c r="E21" s="153"/>
+      <c r="F21" s="153"/>
+      <c r="G21" s="153"/>
+      <c r="H21" s="153"/>
+      <c r="I21" s="153"/>
+      <c r="J21" s="153"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="93">
@@ -4282,12 +4282,12 @@
       </c>
       <c r="C22" s="78"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="152"/>
-      <c r="F22" s="152"/>
-      <c r="G22" s="152"/>
-      <c r="H22" s="152"/>
-      <c r="I22" s="152"/>
-      <c r="J22" s="152"/>
+      <c r="E22" s="153"/>
+      <c r="F22" s="153"/>
+      <c r="G22" s="153"/>
+      <c r="H22" s="153"/>
+      <c r="I22" s="153"/>
+      <c r="J22" s="153"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="94">
@@ -4298,12 +4298,12 @@
       </c>
       <c r="C23" s="78"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="152"/>
-      <c r="F23" s="152"/>
-      <c r="G23" s="152"/>
-      <c r="H23" s="152"/>
-      <c r="I23" s="152"/>
-      <c r="J23" s="152"/>
+      <c r="E23" s="153"/>
+      <c r="F23" s="153"/>
+      <c r="G23" s="153"/>
+      <c r="H23" s="153"/>
+      <c r="I23" s="153"/>
+      <c r="J23" s="153"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="95">
@@ -4314,12 +4314,12 @@
       </c>
       <c r="C24" s="78"/>
       <c r="D24" s="40"/>
-      <c r="E24" s="152"/>
-      <c r="F24" s="152"/>
-      <c r="G24" s="152"/>
-      <c r="H24" s="152"/>
-      <c r="I24" s="152"/>
-      <c r="J24" s="152"/>
+      <c r="E24" s="153"/>
+      <c r="F24" s="153"/>
+      <c r="G24" s="153"/>
+      <c r="H24" s="153"/>
+      <c r="I24" s="153"/>
+      <c r="J24" s="153"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="40">
@@ -4330,12 +4330,12 @@
       </c>
       <c r="C25" s="78"/>
       <c r="D25" s="40"/>
-      <c r="E25" s="152"/>
-      <c r="F25" s="152"/>
-      <c r="G25" s="152"/>
-      <c r="H25" s="152"/>
-      <c r="I25" s="152"/>
-      <c r="J25" s="152"/>
+      <c r="E25" s="153"/>
+      <c r="F25" s="153"/>
+      <c r="G25" s="153"/>
+      <c r="H25" s="153"/>
+      <c r="I25" s="153"/>
+      <c r="J25" s="153"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="87">
@@ -4346,12 +4346,12 @@
       </c>
       <c r="C26" s="78"/>
       <c r="D26" s="40"/>
-      <c r="E26" s="152"/>
-      <c r="F26" s="152"/>
-      <c r="G26" s="152"/>
-      <c r="H26" s="152"/>
-      <c r="I26" s="152"/>
-      <c r="J26" s="152"/>
+      <c r="E26" s="153"/>
+      <c r="F26" s="153"/>
+      <c r="G26" s="153"/>
+      <c r="H26" s="153"/>
+      <c r="I26" s="153"/>
+      <c r="J26" s="153"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="88">
@@ -4362,12 +4362,12 @@
       </c>
       <c r="C27" s="78"/>
       <c r="D27" s="40"/>
-      <c r="E27" s="152"/>
-      <c r="F27" s="152"/>
-      <c r="G27" s="152"/>
-      <c r="H27" s="152"/>
-      <c r="I27" s="152"/>
-      <c r="J27" s="152"/>
+      <c r="E27" s="153"/>
+      <c r="F27" s="153"/>
+      <c r="G27" s="153"/>
+      <c r="H27" s="153"/>
+      <c r="I27" s="153"/>
+      <c r="J27" s="153"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="89">
@@ -4378,12 +4378,12 @@
       </c>
       <c r="C28" s="78"/>
       <c r="D28" s="40"/>
-      <c r="E28" s="152"/>
-      <c r="F28" s="152"/>
-      <c r="G28" s="152"/>
-      <c r="H28" s="152"/>
-      <c r="I28" s="152"/>
-      <c r="J28" s="152"/>
+      <c r="E28" s="153"/>
+      <c r="F28" s="153"/>
+      <c r="G28" s="153"/>
+      <c r="H28" s="153"/>
+      <c r="I28" s="153"/>
+      <c r="J28" s="153"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="90">
@@ -4394,12 +4394,12 @@
       </c>
       <c r="C29" s="78"/>
       <c r="D29" s="40"/>
-      <c r="E29" s="152"/>
-      <c r="F29" s="152"/>
-      <c r="G29" s="152"/>
-      <c r="H29" s="152"/>
-      <c r="I29" s="152"/>
-      <c r="J29" s="152"/>
+      <c r="E29" s="153"/>
+      <c r="F29" s="153"/>
+      <c r="G29" s="153"/>
+      <c r="H29" s="153"/>
+      <c r="I29" s="153"/>
+      <c r="J29" s="153"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="91">
@@ -4410,12 +4410,12 @@
       </c>
       <c r="C30" s="78"/>
       <c r="D30" s="40"/>
-      <c r="E30" s="152"/>
-      <c r="F30" s="152"/>
-      <c r="G30" s="152"/>
-      <c r="H30" s="152"/>
-      <c r="I30" s="152"/>
-      <c r="J30" s="152"/>
+      <c r="E30" s="153"/>
+      <c r="F30" s="153"/>
+      <c r="G30" s="153"/>
+      <c r="H30" s="153"/>
+      <c r="I30" s="153"/>
+      <c r="J30" s="153"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="92">
@@ -4426,12 +4426,12 @@
       </c>
       <c r="C31" s="78"/>
       <c r="D31" s="40"/>
-      <c r="E31" s="152"/>
-      <c r="F31" s="152"/>
-      <c r="G31" s="152"/>
-      <c r="H31" s="152"/>
-      <c r="I31" s="152"/>
-      <c r="J31" s="152"/>
+      <c r="E31" s="153"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="153"/>
+      <c r="H31" s="153"/>
+      <c r="I31" s="153"/>
+      <c r="J31" s="153"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="93">
@@ -4442,12 +4442,12 @@
       </c>
       <c r="C32" s="78"/>
       <c r="D32" s="40"/>
-      <c r="E32" s="152"/>
-      <c r="F32" s="152"/>
-      <c r="G32" s="152"/>
-      <c r="H32" s="152"/>
-      <c r="I32" s="152"/>
-      <c r="J32" s="152"/>
+      <c r="E32" s="153"/>
+      <c r="F32" s="153"/>
+      <c r="G32" s="153"/>
+      <c r="H32" s="153"/>
+      <c r="I32" s="153"/>
+      <c r="J32" s="153"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="94">
@@ -4458,12 +4458,12 @@
       </c>
       <c r="C33" s="78"/>
       <c r="D33" s="40"/>
-      <c r="E33" s="152"/>
-      <c r="F33" s="152"/>
-      <c r="G33" s="152"/>
-      <c r="H33" s="152"/>
-      <c r="I33" s="152"/>
-      <c r="J33" s="152"/>
+      <c r="E33" s="153"/>
+      <c r="F33" s="153"/>
+      <c r="G33" s="153"/>
+      <c r="H33" s="153"/>
+      <c r="I33" s="153"/>
+      <c r="J33" s="153"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="95">
@@ -4474,12 +4474,12 @@
       </c>
       <c r="C34" s="78"/>
       <c r="D34" s="40"/>
-      <c r="E34" s="152"/>
-      <c r="F34" s="152"/>
-      <c r="G34" s="152"/>
-      <c r="H34" s="152"/>
-      <c r="I34" s="152"/>
-      <c r="J34" s="152"/>
+      <c r="E34" s="153"/>
+      <c r="F34" s="153"/>
+      <c r="G34" s="153"/>
+      <c r="H34" s="153"/>
+      <c r="I34" s="153"/>
+      <c r="J34" s="153"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="40">
@@ -4490,12 +4490,12 @@
       </c>
       <c r="C35" s="78"/>
       <c r="D35" s="40"/>
-      <c r="E35" s="152"/>
-      <c r="F35" s="152"/>
-      <c r="G35" s="152"/>
-      <c r="H35" s="152"/>
-      <c r="I35" s="152"/>
-      <c r="J35" s="152"/>
+      <c r="E35" s="153"/>
+      <c r="F35" s="153"/>
+      <c r="G35" s="153"/>
+      <c r="H35" s="153"/>
+      <c r="I35" s="153"/>
+      <c r="J35" s="153"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="87">
@@ -4506,12 +4506,12 @@
       </c>
       <c r="C36" s="78"/>
       <c r="D36" s="40"/>
-      <c r="E36" s="152"/>
-      <c r="F36" s="152"/>
-      <c r="G36" s="152"/>
-      <c r="H36" s="152"/>
-      <c r="I36" s="152"/>
-      <c r="J36" s="152"/>
+      <c r="E36" s="153"/>
+      <c r="F36" s="153"/>
+      <c r="G36" s="153"/>
+      <c r="H36" s="153"/>
+      <c r="I36" s="153"/>
+      <c r="J36" s="153"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="88">
@@ -4522,12 +4522,12 @@
       </c>
       <c r="C37" s="78"/>
       <c r="D37" s="40"/>
-      <c r="E37" s="152"/>
-      <c r="F37" s="152"/>
-      <c r="G37" s="152"/>
-      <c r="H37" s="152"/>
-      <c r="I37" s="152"/>
-      <c r="J37" s="152"/>
+      <c r="E37" s="153"/>
+      <c r="F37" s="153"/>
+      <c r="G37" s="153"/>
+      <c r="H37" s="153"/>
+      <c r="I37" s="153"/>
+      <c r="J37" s="153"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="89">
@@ -4538,12 +4538,12 @@
       </c>
       <c r="C38" s="78"/>
       <c r="D38" s="40"/>
-      <c r="E38" s="152"/>
-      <c r="F38" s="152"/>
-      <c r="G38" s="152"/>
-      <c r="H38" s="152"/>
-      <c r="I38" s="152"/>
-      <c r="J38" s="152"/>
+      <c r="E38" s="153"/>
+      <c r="F38" s="153"/>
+      <c r="G38" s="153"/>
+      <c r="H38" s="153"/>
+      <c r="I38" s="153"/>
+      <c r="J38" s="153"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="90">
@@ -4554,12 +4554,12 @@
       </c>
       <c r="C39" s="78"/>
       <c r="D39" s="40"/>
-      <c r="E39" s="152"/>
-      <c r="F39" s="152"/>
-      <c r="G39" s="152"/>
-      <c r="H39" s="152"/>
-      <c r="I39" s="152"/>
-      <c r="J39" s="152"/>
+      <c r="E39" s="153"/>
+      <c r="F39" s="153"/>
+      <c r="G39" s="153"/>
+      <c r="H39" s="153"/>
+      <c r="I39" s="153"/>
+      <c r="J39" s="153"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="91">
@@ -4570,12 +4570,12 @@
       </c>
       <c r="C40" s="78"/>
       <c r="D40" s="40"/>
-      <c r="E40" s="152"/>
-      <c r="F40" s="152"/>
-      <c r="G40" s="152"/>
-      <c r="H40" s="152"/>
-      <c r="I40" s="152"/>
-      <c r="J40" s="152"/>
+      <c r="E40" s="153"/>
+      <c r="F40" s="153"/>
+      <c r="G40" s="153"/>
+      <c r="H40" s="153"/>
+      <c r="I40" s="153"/>
+      <c r="J40" s="153"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="92">
@@ -4586,12 +4586,12 @@
       </c>
       <c r="C41" s="78"/>
       <c r="D41" s="40"/>
-      <c r="E41" s="152"/>
-      <c r="F41" s="152"/>
-      <c r="G41" s="152"/>
-      <c r="H41" s="152"/>
-      <c r="I41" s="152"/>
-      <c r="J41" s="152"/>
+      <c r="E41" s="153"/>
+      <c r="F41" s="153"/>
+      <c r="G41" s="153"/>
+      <c r="H41" s="153"/>
+      <c r="I41" s="153"/>
+      <c r="J41" s="153"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="93">
@@ -4602,12 +4602,12 @@
       </c>
       <c r="C42" s="78"/>
       <c r="D42" s="40"/>
-      <c r="E42" s="152"/>
-      <c r="F42" s="152"/>
-      <c r="G42" s="152"/>
-      <c r="H42" s="152"/>
-      <c r="I42" s="152"/>
-      <c r="J42" s="152"/>
+      <c r="E42" s="153"/>
+      <c r="F42" s="153"/>
+      <c r="G42" s="153"/>
+      <c r="H42" s="153"/>
+      <c r="I42" s="153"/>
+      <c r="J42" s="153"/>
     </row>
   </sheetData>
   <mergeCells count="40">
@@ -4865,10 +4865,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
+      <c r="B1" s="146"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -4898,8 +4898,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -4929,20 +4929,20 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="153" t="s">
+      <c r="A4" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="155"/>
-      <c r="C4" s="155"/>
-      <c r="D4" s="155"/>
-      <c r="E4" s="155"/>
-      <c r="F4" s="155"/>
-      <c r="G4" s="155"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="153" t="s">
+      <c r="B4" s="156"/>
+      <c r="C4" s="156"/>
+      <c r="D4" s="156"/>
+      <c r="E4" s="156"/>
+      <c r="F4" s="156"/>
+      <c r="G4" s="156"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="154"/>
+      <c r="J4" s="155"/>
     </row>
     <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="42"/>
@@ -4953,10 +4953,10 @@
       <c r="F5" s="43"/>
       <c r="G5" s="43"/>
       <c r="H5" s="44"/>
-      <c r="I5" s="162" t="s">
+      <c r="I5" s="163" t="s">
         <v>174</v>
       </c>
-      <c r="J5" s="163"/>
+      <c r="J5" s="164"/>
     </row>
     <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="42"/>
@@ -4967,8 +4967,8 @@
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
       <c r="H6" s="45"/>
-      <c r="I6" s="164"/>
-      <c r="J6" s="165"/>
+      <c r="I6" s="165"/>
+      <c r="J6" s="166"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="42"/>
@@ -4979,8 +4979,8 @@
       <c r="F7" s="43"/>
       <c r="G7" s="43"/>
       <c r="H7" s="45"/>
-      <c r="I7" s="164"/>
-      <c r="J7" s="165"/>
+      <c r="I7" s="165"/>
+      <c r="J7" s="166"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="42"/>
@@ -4991,8 +4991,8 @@
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
       <c r="H8" s="45"/>
-      <c r="I8" s="164"/>
-      <c r="J8" s="165"/>
+      <c r="I8" s="165"/>
+      <c r="J8" s="166"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="42"/>
@@ -5003,8 +5003,8 @@
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
       <c r="H9" s="45"/>
-      <c r="I9" s="164"/>
-      <c r="J9" s="165"/>
+      <c r="I9" s="165"/>
+      <c r="J9" s="166"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="42"/>
@@ -5015,8 +5015,8 @@
       <c r="F10" s="43"/>
       <c r="G10" s="43"/>
       <c r="H10" s="45"/>
-      <c r="I10" s="166"/>
-      <c r="J10" s="167"/>
+      <c r="I10" s="167"/>
+      <c r="J10" s="168"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="42"/>
@@ -5027,10 +5027,10 @@
       <c r="F11" s="43"/>
       <c r="G11" s="43"/>
       <c r="H11" s="46"/>
-      <c r="I11" s="153" t="s">
+      <c r="I11" s="154" t="s">
         <v>40</v>
       </c>
-      <c r="J11" s="154"/>
+      <c r="J11" s="155"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="42"/>
@@ -5041,10 +5041,10 @@
       <c r="F12" s="43"/>
       <c r="G12" s="43"/>
       <c r="H12" s="45"/>
-      <c r="I12" s="156" t="s">
+      <c r="I12" s="157" t="s">
         <v>227</v>
       </c>
-      <c r="J12" s="157"/>
+      <c r="J12" s="158"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="42"/>
@@ -5055,8 +5055,8 @@
       <c r="F13" s="43"/>
       <c r="G13" s="43"/>
       <c r="H13" s="45"/>
-      <c r="I13" s="158"/>
-      <c r="J13" s="159"/>
+      <c r="I13" s="159"/>
+      <c r="J13" s="160"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="42"/>
@@ -5067,8 +5067,8 @@
       <c r="F14" s="43"/>
       <c r="G14" s="43"/>
       <c r="H14" s="45"/>
-      <c r="I14" s="158"/>
-      <c r="J14" s="159"/>
+      <c r="I14" s="159"/>
+      <c r="J14" s="160"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="42"/>
@@ -5079,8 +5079,8 @@
       <c r="F15" s="43"/>
       <c r="G15" s="43"/>
       <c r="H15" s="45"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="159"/>
+      <c r="I15" s="159"/>
+      <c r="J15" s="160"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="42"/>
@@ -5091,8 +5091,8 @@
       <c r="F16" s="43"/>
       <c r="G16" s="43"/>
       <c r="H16" s="45"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="160"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="42"/>
@@ -5103,8 +5103,8 @@
       <c r="F17" s="43"/>
       <c r="G17" s="43"/>
       <c r="H17" s="45"/>
-      <c r="I17" s="158"/>
-      <c r="J17" s="159"/>
+      <c r="I17" s="159"/>
+      <c r="J17" s="160"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="42"/>
@@ -5115,8 +5115,8 @@
       <c r="F18" s="43"/>
       <c r="G18" s="43"/>
       <c r="H18" s="45"/>
-      <c r="I18" s="158"/>
-      <c r="J18" s="159"/>
+      <c r="I18" s="159"/>
+      <c r="J18" s="160"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="42"/>
@@ -5127,8 +5127,8 @@
       <c r="F19" s="43"/>
       <c r="G19" s="43"/>
       <c r="H19" s="45"/>
-      <c r="I19" s="158"/>
-      <c r="J19" s="159"/>
+      <c r="I19" s="159"/>
+      <c r="J19" s="160"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="42"/>
@@ -5139,8 +5139,8 @@
       <c r="F20" s="43"/>
       <c r="G20" s="43"/>
       <c r="H20" s="45"/>
-      <c r="I20" s="158"/>
-      <c r="J20" s="159"/>
+      <c r="I20" s="159"/>
+      <c r="J20" s="160"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="42"/>
@@ -5151,8 +5151,8 @@
       <c r="F21" s="43"/>
       <c r="G21" s="43"/>
       <c r="H21" s="45"/>
-      <c r="I21" s="158"/>
-      <c r="J21" s="159"/>
+      <c r="I21" s="159"/>
+      <c r="J21" s="160"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="42"/>
@@ -5163,8 +5163,8 @@
       <c r="F22" s="43"/>
       <c r="G22" s="43"/>
       <c r="H22" s="45"/>
-      <c r="I22" s="158"/>
-      <c r="J22" s="159"/>
+      <c r="I22" s="159"/>
+      <c r="J22" s="160"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="42"/>
@@ -5175,8 +5175,8 @@
       <c r="F23" s="43"/>
       <c r="G23" s="43"/>
       <c r="H23" s="45"/>
-      <c r="I23" s="158"/>
-      <c r="J23" s="159"/>
+      <c r="I23" s="159"/>
+      <c r="J23" s="160"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="42"/>
@@ -5187,8 +5187,8 @@
       <c r="F24" s="43"/>
       <c r="G24" s="43"/>
       <c r="H24" s="45"/>
-      <c r="I24" s="158"/>
-      <c r="J24" s="159"/>
+      <c r="I24" s="159"/>
+      <c r="J24" s="160"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="42"/>
@@ -5199,8 +5199,8 @@
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
       <c r="H25" s="45"/>
-      <c r="I25" s="158"/>
-      <c r="J25" s="159"/>
+      <c r="I25" s="159"/>
+      <c r="J25" s="160"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="42"/>
@@ -5211,8 +5211,8 @@
       <c r="F26" s="43"/>
       <c r="G26" s="43"/>
       <c r="H26" s="45"/>
-      <c r="I26" s="158"/>
-      <c r="J26" s="159"/>
+      <c r="I26" s="159"/>
+      <c r="J26" s="160"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="42"/>
@@ -5223,8 +5223,8 @@
       <c r="F27" s="43"/>
       <c r="G27" s="43"/>
       <c r="H27" s="45"/>
-      <c r="I27" s="158"/>
-      <c r="J27" s="159"/>
+      <c r="I27" s="159"/>
+      <c r="J27" s="160"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="42"/>
@@ -5235,8 +5235,8 @@
       <c r="F28" s="43"/>
       <c r="G28" s="43"/>
       <c r="H28" s="45"/>
-      <c r="I28" s="158"/>
-      <c r="J28" s="159"/>
+      <c r="I28" s="159"/>
+      <c r="J28" s="160"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="42"/>
@@ -5247,8 +5247,8 @@
       <c r="F29" s="43"/>
       <c r="G29" s="43"/>
       <c r="H29" s="45"/>
-      <c r="I29" s="158"/>
-      <c r="J29" s="159"/>
+      <c r="I29" s="159"/>
+      <c r="J29" s="160"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="42"/>
@@ -5259,8 +5259,8 @@
       <c r="F30" s="43"/>
       <c r="G30" s="43"/>
       <c r="H30" s="45"/>
-      <c r="I30" s="158"/>
-      <c r="J30" s="159"/>
+      <c r="I30" s="159"/>
+      <c r="J30" s="160"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="42"/>
@@ -5271,8 +5271,8 @@
       <c r="F31" s="43"/>
       <c r="G31" s="43"/>
       <c r="H31" s="45"/>
-      <c r="I31" s="158"/>
-      <c r="J31" s="159"/>
+      <c r="I31" s="159"/>
+      <c r="J31" s="160"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="42"/>
@@ -5283,8 +5283,8 @@
       <c r="F32" s="43"/>
       <c r="G32" s="43"/>
       <c r="H32" s="45"/>
-      <c r="I32" s="158"/>
-      <c r="J32" s="159"/>
+      <c r="I32" s="159"/>
+      <c r="J32" s="160"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="42"/>
@@ -5295,8 +5295,8 @@
       <c r="F33" s="43"/>
       <c r="G33" s="43"/>
       <c r="H33" s="45"/>
-      <c r="I33" s="158"/>
-      <c r="J33" s="159"/>
+      <c r="I33" s="159"/>
+      <c r="J33" s="160"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="42"/>
@@ -5307,8 +5307,8 @@
       <c r="F34" s="43"/>
       <c r="G34" s="43"/>
       <c r="H34" s="45"/>
-      <c r="I34" s="158"/>
-      <c r="J34" s="159"/>
+      <c r="I34" s="159"/>
+      <c r="J34" s="160"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="42"/>
@@ -5319,8 +5319,8 @@
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
       <c r="H35" s="45"/>
-      <c r="I35" s="158"/>
-      <c r="J35" s="159"/>
+      <c r="I35" s="159"/>
+      <c r="J35" s="160"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="42"/>
@@ -5331,8 +5331,8 @@
       <c r="F36" s="43"/>
       <c r="G36" s="43"/>
       <c r="H36" s="45"/>
-      <c r="I36" s="158"/>
-      <c r="J36" s="159"/>
+      <c r="I36" s="159"/>
+      <c r="J36" s="160"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="42"/>
@@ -5343,8 +5343,8 @@
       <c r="F37" s="43"/>
       <c r="G37" s="43"/>
       <c r="H37" s="45"/>
-      <c r="I37" s="158"/>
-      <c r="J37" s="159"/>
+      <c r="I37" s="159"/>
+      <c r="J37" s="160"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="42"/>
@@ -5355,8 +5355,8 @@
       <c r="F38" s="43"/>
       <c r="G38" s="43"/>
       <c r="H38" s="45"/>
-      <c r="I38" s="158"/>
-      <c r="J38" s="159"/>
+      <c r="I38" s="159"/>
+      <c r="J38" s="160"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="42"/>
@@ -5367,8 +5367,8 @@
       <c r="F39" s="43"/>
       <c r="G39" s="43"/>
       <c r="H39" s="45"/>
-      <c r="I39" s="158"/>
-      <c r="J39" s="159"/>
+      <c r="I39" s="159"/>
+      <c r="J39" s="160"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="42"/>
@@ -5379,8 +5379,8 @@
       <c r="F40" s="43"/>
       <c r="G40" s="43"/>
       <c r="H40" s="45"/>
-      <c r="I40" s="158"/>
-      <c r="J40" s="159"/>
+      <c r="I40" s="159"/>
+      <c r="J40" s="160"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="42"/>
@@ -5391,8 +5391,8 @@
       <c r="F41" s="43"/>
       <c r="G41" s="43"/>
       <c r="H41" s="45"/>
-      <c r="I41" s="158"/>
-      <c r="J41" s="159"/>
+      <c r="I41" s="159"/>
+      <c r="J41" s="160"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="42"/>
@@ -5403,8 +5403,8 @@
       <c r="F42" s="43"/>
       <c r="G42" s="43"/>
       <c r="H42" s="45"/>
-      <c r="I42" s="158"/>
-      <c r="J42" s="159"/>
+      <c r="I42" s="159"/>
+      <c r="J42" s="160"/>
     </row>
     <row r="43" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="47"/>
@@ -5415,8 +5415,8 @@
       <c r="F43" s="48"/>
       <c r="G43" s="48"/>
       <c r="H43" s="49"/>
-      <c r="I43" s="160"/>
-      <c r="J43" s="161"/>
+      <c r="I43" s="161"/>
+      <c r="J43" s="162"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5450,7 +5450,7 @@
       <pane xSplit="7" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5475,13 +5475,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
       <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
@@ -5489,16 +5489,16 @@
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="H1" s="168" t="s">
+      <c r="H1" s="169" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="169"/>
-      <c r="J1" s="170" t="str">
+      <c r="I1" s="170"/>
+      <c r="J1" s="171" t="str">
         <f>'Update History'!F1</f>
         <v>CF0142</v>
       </c>
-      <c r="K1" s="171"/>
-      <c r="L1" s="172"/>
+      <c r="K1" s="172"/>
+      <c r="L1" s="173"/>
       <c r="M1" s="31" t="s">
         <v>5</v>
       </c>
@@ -5515,11 +5515,11 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
       <c r="F2" s="30" t="s">
         <v>2</v>
       </c>
@@ -5527,16 +5527,16 @@
         <f>'Update History'!D2</f>
         <v>ASOFT - CI</v>
       </c>
-      <c r="H2" s="168" t="s">
+      <c r="H2" s="169" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="169"/>
-      <c r="J2" s="170" t="str">
+      <c r="I2" s="170"/>
+      <c r="J2" s="171" t="str">
         <f>'Update History'!F2</f>
         <v>Cập nhật địa điểm</v>
       </c>
-      <c r="K2" s="171"/>
-      <c r="L2" s="172"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="173"/>
       <c r="M2" s="31" t="s">
         <v>6</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>45</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C4" s="119" t="s">
         <v>233</v>
@@ -6942,8 +6942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6968,11 +6968,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="174" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="194"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="139"/>
       <c r="D1" s="101" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
@@ -7001,11 +7001,11 @@
       <c r="K1" s="65"/>
     </row>
     <row r="2" spans="1:17" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="173" t="s">
+      <c r="A2" s="174" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="174"/>
-      <c r="C2" s="194"/>
+      <c r="B2" s="175"/>
+      <c r="C2" s="139"/>
       <c r="D2" s="101" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT - CI</v>
@@ -7041,7 +7041,7 @@
         <v>233</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>104</v>
@@ -7098,7 +7098,7 @@
         <v>239</v>
       </c>
       <c r="J5" s="62" t="s">
-        <v>240</v>
+        <v>299</v>
       </c>
       <c r="K5" s="68"/>
     </row>
@@ -7118,16 +7118,18 @@
       <c r="E6" s="122" t="s">
         <v>237</v>
       </c>
-      <c r="F6" s="133"/>
+      <c r="F6" s="133" t="s">
+        <v>221</v>
+      </c>
       <c r="G6" s="61"/>
       <c r="H6" s="122" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I6" s="122" t="s">
         <v>239</v>
       </c>
       <c r="J6" s="62" t="s">
-        <v>242</v>
+        <v>300</v>
       </c>
       <c r="K6" s="68"/>
     </row>
@@ -7150,13 +7152,13 @@
       <c r="F7" s="40"/>
       <c r="G7" s="61"/>
       <c r="H7" s="122" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I7" s="122" t="s">
         <v>239</v>
       </c>
       <c r="J7" s="62" t="s">
-        <v>244</v>
+        <v>302</v>
       </c>
       <c r="K7" s="85"/>
     </row>
@@ -7181,13 +7183,13 @@
       </c>
       <c r="G8" s="61"/>
       <c r="H8" s="122" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="I8" s="122" t="s">
+        <v>242</v>
+      </c>
+      <c r="J8" s="62" t="s">
         <v>245</v>
-      </c>
-      <c r="J8" s="62" t="s">
-        <v>248</v>
       </c>
       <c r="K8" s="85"/>
     </row>
@@ -7208,17 +7210,17 @@
         <v>237</v>
       </c>
       <c r="F9" s="133" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G9" s="61"/>
       <c r="H9" s="122" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="I9" s="122" t="s">
+        <v>242</v>
+      </c>
+      <c r="J9" s="62" t="s">
         <v>245</v>
-      </c>
-      <c r="J9" s="62" t="s">
-        <v>248</v>
       </c>
       <c r="K9" s="82"/>
     </row>
@@ -7233,7 +7235,7 @@
         <v>51</v>
       </c>
       <c r="D10" s="122" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E10" s="122" t="s">
         <v>237</v>
@@ -7241,13 +7243,13 @@
       <c r="F10" s="138"/>
       <c r="G10" s="61"/>
       <c r="H10" s="122" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="I10" s="122" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="J10" s="62" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="K10" s="82"/>
     </row>
@@ -8056,7 +8058,7 @@
   <dimension ref="A1:S56"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27:H27"/>
+      <selection activeCell="B5" sqref="B5:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8081,10 +8083,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="180" t="s">
+      <c r="A1" s="181" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="181"/>
+      <c r="B1" s="182"/>
       <c r="C1" s="134"/>
       <c r="D1" s="31" t="s">
         <v>1</v>
@@ -8118,8 +8120,8 @@
       <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:13" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="182"/>
-      <c r="B2" s="183"/>
+      <c r="A2" s="183"/>
+      <c r="B2" s="184"/>
       <c r="C2" s="135"/>
       <c r="D2" s="31" t="s">
         <v>2</v>
@@ -8160,7 +8162,7 @@
         <v>233</v>
       </c>
       <c r="C4" s="124" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>130</v>
@@ -8171,15 +8173,15 @@
       <c r="F4" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="145" t="s">
+      <c r="G4" s="146" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="145"/>
-      <c r="I4" s="145" t="s">
+      <c r="H4" s="146"/>
+      <c r="I4" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="145"/>
-      <c r="K4" s="145"/>
+      <c r="J4" s="146"/>
+      <c r="K4" s="146"/>
     </row>
     <row r="5" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
@@ -8192,7 +8194,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E5" s="136" t="s">
         <v>135</v>
@@ -8200,13 +8202,13 @@
       <c r="F5" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="G5" s="178" t="s">
-        <v>254</v>
-      </c>
-      <c r="H5" s="179"/>
-      <c r="I5" s="175"/>
-      <c r="J5" s="176"/>
-      <c r="K5" s="177"/>
+      <c r="G5" s="179" t="s">
+        <v>251</v>
+      </c>
+      <c r="H5" s="180"/>
+      <c r="I5" s="176"/>
+      <c r="J5" s="177"/>
+      <c r="K5" s="178"/>
     </row>
     <row r="6" spans="1:13" s="34" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33">
@@ -8219,21 +8221,21 @@
         <v>51</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E6" s="133" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F6" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="G6" s="178" t="s">
-        <v>255</v>
-      </c>
-      <c r="H6" s="179"/>
-      <c r="I6" s="175"/>
-      <c r="J6" s="176"/>
-      <c r="K6" s="177"/>
+      <c r="G6" s="179" t="s">
+        <v>252</v>
+      </c>
+      <c r="H6" s="180"/>
+      <c r="I6" s="176"/>
+      <c r="J6" s="177"/>
+      <c r="K6" s="178"/>
     </row>
     <row r="7" spans="1:13" s="34" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
@@ -8246,21 +8248,21 @@
         <v>51</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E7" s="133" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F7" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="G7" s="178" t="s">
-        <v>255</v>
-      </c>
-      <c r="H7" s="179"/>
-      <c r="I7" s="175"/>
-      <c r="J7" s="176"/>
-      <c r="K7" s="177"/>
+      <c r="G7" s="179" t="s">
+        <v>252</v>
+      </c>
+      <c r="H7" s="180"/>
+      <c r="I7" s="176"/>
+      <c r="J7" s="177"/>
+      <c r="K7" s="178"/>
     </row>
     <row r="8" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
@@ -8271,11 +8273,11 @@
       <c r="D8" s="33"/>
       <c r="E8" s="33"/>
       <c r="F8" s="32"/>
-      <c r="G8" s="178"/>
-      <c r="H8" s="179"/>
-      <c r="I8" s="175"/>
-      <c r="J8" s="176"/>
-      <c r="K8" s="177"/>
+      <c r="G8" s="179"/>
+      <c r="H8" s="180"/>
+      <c r="I8" s="176"/>
+      <c r="J8" s="177"/>
+      <c r="K8" s="178"/>
     </row>
     <row r="9" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33">
@@ -8286,11 +8288,11 @@
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
       <c r="F9" s="32"/>
-      <c r="G9" s="178"/>
-      <c r="H9" s="179"/>
-      <c r="I9" s="175"/>
-      <c r="J9" s="176"/>
-      <c r="K9" s="177"/>
+      <c r="G9" s="179"/>
+      <c r="H9" s="180"/>
+      <c r="I9" s="176"/>
+      <c r="J9" s="177"/>
+      <c r="K9" s="178"/>
     </row>
     <row r="10" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="33">
@@ -8301,11 +8303,11 @@
       <c r="D10" s="33"/>
       <c r="E10" s="33"/>
       <c r="F10" s="32"/>
-      <c r="G10" s="178"/>
-      <c r="H10" s="179"/>
-      <c r="I10" s="175"/>
-      <c r="J10" s="176"/>
-      <c r="K10" s="177"/>
+      <c r="G10" s="179"/>
+      <c r="H10" s="180"/>
+      <c r="I10" s="176"/>
+      <c r="J10" s="177"/>
+      <c r="K10" s="178"/>
     </row>
     <row r="11" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33">
@@ -8316,11 +8318,11 @@
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
       <c r="F11" s="32"/>
-      <c r="G11" s="178"/>
-      <c r="H11" s="179"/>
-      <c r="I11" s="175"/>
-      <c r="J11" s="176"/>
-      <c r="K11" s="177"/>
+      <c r="G11" s="179"/>
+      <c r="H11" s="180"/>
+      <c r="I11" s="176"/>
+      <c r="J11" s="177"/>
+      <c r="K11" s="178"/>
     </row>
     <row r="12" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="33">
@@ -8331,11 +8333,11 @@
       <c r="D12" s="33"/>
       <c r="E12" s="33"/>
       <c r="F12" s="32"/>
-      <c r="G12" s="178"/>
-      <c r="H12" s="179"/>
-      <c r="I12" s="175"/>
-      <c r="J12" s="176"/>
-      <c r="K12" s="177"/>
+      <c r="G12" s="179"/>
+      <c r="H12" s="180"/>
+      <c r="I12" s="176"/>
+      <c r="J12" s="177"/>
+      <c r="K12" s="178"/>
     </row>
     <row r="13" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33">
@@ -8346,11 +8348,11 @@
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
       <c r="F13" s="32"/>
-      <c r="G13" s="178"/>
-      <c r="H13" s="179"/>
-      <c r="I13" s="175"/>
-      <c r="J13" s="176"/>
-      <c r="K13" s="177"/>
+      <c r="G13" s="179"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="176"/>
+      <c r="J13" s="177"/>
+      <c r="K13" s="178"/>
     </row>
     <row r="14" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
@@ -8361,11 +8363,11 @@
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
       <c r="F14" s="32"/>
-      <c r="G14" s="178"/>
-      <c r="H14" s="179"/>
-      <c r="I14" s="175"/>
-      <c r="J14" s="176"/>
-      <c r="K14" s="177"/>
+      <c r="G14" s="179"/>
+      <c r="H14" s="180"/>
+      <c r="I14" s="176"/>
+      <c r="J14" s="177"/>
+      <c r="K14" s="178"/>
     </row>
     <row r="15" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33">
@@ -8376,11 +8378,11 @@
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
       <c r="F15" s="32"/>
-      <c r="G15" s="178"/>
-      <c r="H15" s="179"/>
-      <c r="I15" s="175"/>
-      <c r="J15" s="176"/>
-      <c r="K15" s="177"/>
+      <c r="G15" s="179"/>
+      <c r="H15" s="180"/>
+      <c r="I15" s="176"/>
+      <c r="J15" s="177"/>
+      <c r="K15" s="178"/>
     </row>
     <row r="16" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33">
@@ -8391,11 +8393,11 @@
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
       <c r="F16" s="32"/>
-      <c r="G16" s="178"/>
-      <c r="H16" s="179"/>
-      <c r="I16" s="175"/>
-      <c r="J16" s="176"/>
-      <c r="K16" s="177"/>
+      <c r="G16" s="179"/>
+      <c r="H16" s="180"/>
+      <c r="I16" s="176"/>
+      <c r="J16" s="177"/>
+      <c r="K16" s="178"/>
     </row>
     <row r="17" spans="1:19" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A17" s="33">
@@ -8406,11 +8408,11 @@
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
       <c r="F17" s="32"/>
-      <c r="G17" s="178"/>
-      <c r="H17" s="179"/>
-      <c r="I17" s="175"/>
-      <c r="J17" s="176"/>
-      <c r="K17" s="177"/>
+      <c r="G17" s="179"/>
+      <c r="H17" s="180"/>
+      <c r="I17" s="176"/>
+      <c r="J17" s="177"/>
+      <c r="K17" s="178"/>
     </row>
     <row r="18" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33">
@@ -8421,11 +8423,11 @@
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
       <c r="F18" s="32"/>
-      <c r="G18" s="178"/>
-      <c r="H18" s="179"/>
-      <c r="I18" s="175"/>
-      <c r="J18" s="176"/>
-      <c r="K18" s="177"/>
+      <c r="G18" s="179"/>
+      <c r="H18" s="180"/>
+      <c r="I18" s="176"/>
+      <c r="J18" s="177"/>
+      <c r="K18" s="178"/>
     </row>
     <row r="19" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33">
@@ -8436,11 +8438,11 @@
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
       <c r="F19" s="32"/>
-      <c r="G19" s="178"/>
-      <c r="H19" s="179"/>
-      <c r="I19" s="175"/>
-      <c r="J19" s="176"/>
-      <c r="K19" s="177"/>
+      <c r="G19" s="179"/>
+      <c r="H19" s="180"/>
+      <c r="I19" s="176"/>
+      <c r="J19" s="177"/>
+      <c r="K19" s="178"/>
     </row>
     <row r="20" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="33">
@@ -8451,11 +8453,11 @@
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
       <c r="F20" s="32"/>
-      <c r="G20" s="178"/>
-      <c r="H20" s="179"/>
-      <c r="I20" s="175"/>
-      <c r="J20" s="176"/>
-      <c r="K20" s="177"/>
+      <c r="G20" s="179"/>
+      <c r="H20" s="180"/>
+      <c r="I20" s="176"/>
+      <c r="J20" s="177"/>
+      <c r="K20" s="178"/>
     </row>
     <row r="21" spans="1:19" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A21" s="33">
@@ -8466,11 +8468,11 @@
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
       <c r="F21" s="32"/>
-      <c r="G21" s="178"/>
-      <c r="H21" s="179"/>
-      <c r="I21" s="175"/>
-      <c r="J21" s="176"/>
-      <c r="K21" s="177"/>
+      <c r="G21" s="179"/>
+      <c r="H21" s="180"/>
+      <c r="I21" s="176"/>
+      <c r="J21" s="177"/>
+      <c r="K21" s="178"/>
     </row>
     <row r="22" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="33">
@@ -8481,11 +8483,11 @@
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
       <c r="F22" s="32"/>
-      <c r="G22" s="139"/>
-      <c r="H22" s="141"/>
-      <c r="I22" s="175"/>
-      <c r="J22" s="176"/>
-      <c r="K22" s="177"/>
+      <c r="G22" s="140"/>
+      <c r="H22" s="142"/>
+      <c r="I22" s="176"/>
+      <c r="J22" s="177"/>
+      <c r="K22" s="178"/>
     </row>
     <row r="23" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="33">
@@ -8496,11 +8498,11 @@
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
       <c r="F23" s="32"/>
-      <c r="G23" s="139"/>
-      <c r="H23" s="141"/>
-      <c r="I23" s="175"/>
-      <c r="J23" s="176"/>
-      <c r="K23" s="177"/>
+      <c r="G23" s="140"/>
+      <c r="H23" s="142"/>
+      <c r="I23" s="176"/>
+      <c r="J23" s="177"/>
+      <c r="K23" s="178"/>
     </row>
     <row r="24" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="33">
@@ -8511,11 +8513,11 @@
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="32"/>
-      <c r="G24" s="139"/>
-      <c r="H24" s="141"/>
-      <c r="I24" s="175"/>
-      <c r="J24" s="176"/>
-      <c r="K24" s="177"/>
+      <c r="G24" s="140"/>
+      <c r="H24" s="142"/>
+      <c r="I24" s="176"/>
+      <c r="J24" s="177"/>
+      <c r="K24" s="178"/>
     </row>
     <row r="25" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="33">
@@ -8526,11 +8528,11 @@
       <c r="D25" s="33"/>
       <c r="E25" s="33"/>
       <c r="F25" s="32"/>
-      <c r="G25" s="139"/>
-      <c r="H25" s="141"/>
-      <c r="I25" s="175"/>
-      <c r="J25" s="176"/>
-      <c r="K25" s="177"/>
+      <c r="G25" s="140"/>
+      <c r="H25" s="142"/>
+      <c r="I25" s="176"/>
+      <c r="J25" s="177"/>
+      <c r="K25" s="178"/>
     </row>
     <row r="26" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33">
@@ -8541,11 +8543,11 @@
       <c r="D26" s="33"/>
       <c r="E26" s="33"/>
       <c r="F26" s="32"/>
-      <c r="G26" s="139"/>
-      <c r="H26" s="141"/>
-      <c r="I26" s="175"/>
-      <c r="J26" s="176"/>
-      <c r="K26" s="177"/>
+      <c r="G26" s="140"/>
+      <c r="H26" s="142"/>
+      <c r="I26" s="176"/>
+      <c r="J26" s="177"/>
+      <c r="K26" s="178"/>
     </row>
     <row r="27" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33">
@@ -8556,11 +8558,11 @@
       <c r="D27" s="33"/>
       <c r="E27" s="33"/>
       <c r="F27" s="32"/>
-      <c r="G27" s="139"/>
-      <c r="H27" s="141"/>
-      <c r="I27" s="175"/>
-      <c r="J27" s="176"/>
-      <c r="K27" s="177"/>
+      <c r="G27" s="140"/>
+      <c r="H27" s="142"/>
+      <c r="I27" s="176"/>
+      <c r="J27" s="177"/>
+      <c r="K27" s="178"/>
     </row>
     <row r="28" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="33">
@@ -8571,11 +8573,11 @@
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
       <c r="F28" s="32"/>
-      <c r="G28" s="139"/>
-      <c r="H28" s="141"/>
-      <c r="I28" s="175"/>
-      <c r="J28" s="176"/>
-      <c r="K28" s="177"/>
+      <c r="G28" s="140"/>
+      <c r="H28" s="142"/>
+      <c r="I28" s="176"/>
+      <c r="J28" s="177"/>
+      <c r="K28" s="178"/>
     </row>
     <row r="29" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="33">
@@ -8586,11 +8588,11 @@
       <c r="D29" s="33"/>
       <c r="E29" s="33"/>
       <c r="F29" s="32"/>
-      <c r="G29" s="139"/>
-      <c r="H29" s="141"/>
-      <c r="I29" s="175"/>
-      <c r="J29" s="176"/>
-      <c r="K29" s="177"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="142"/>
+      <c r="I29" s="176"/>
+      <c r="J29" s="177"/>
+      <c r="K29" s="178"/>
     </row>
     <row r="30" spans="1:19" s="34" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="33">
@@ -8601,11 +8603,11 @@
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="32"/>
-      <c r="G30" s="139"/>
-      <c r="H30" s="141"/>
-      <c r="I30" s="175"/>
-      <c r="J30" s="176"/>
-      <c r="K30" s="177"/>
+      <c r="G30" s="140"/>
+      <c r="H30" s="142"/>
+      <c r="I30" s="176"/>
+      <c r="J30" s="177"/>
+      <c r="K30" s="178"/>
     </row>
     <row r="31" spans="1:19" s="34" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="33">
@@ -8616,11 +8618,11 @@
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
       <c r="F31" s="32"/>
-      <c r="G31" s="139"/>
-      <c r="H31" s="141"/>
-      <c r="I31" s="175"/>
-      <c r="J31" s="176"/>
-      <c r="K31" s="177"/>
+      <c r="G31" s="140"/>
+      <c r="H31" s="142"/>
+      <c r="I31" s="176"/>
+      <c r="J31" s="177"/>
+      <c r="K31" s="178"/>
     </row>
     <row r="32" spans="1:19" ht="11.25" x14ac:dyDescent="0.15">
       <c r="A32" s="33">
@@ -8631,11 +8633,11 @@
       <c r="D32" s="33"/>
       <c r="E32" s="33"/>
       <c r="F32" s="32"/>
-      <c r="G32" s="139"/>
-      <c r="H32" s="141"/>
-      <c r="I32" s="175"/>
-      <c r="J32" s="176"/>
-      <c r="K32" s="177"/>
+      <c r="G32" s="140"/>
+      <c r="H32" s="142"/>
+      <c r="I32" s="176"/>
+      <c r="J32" s="177"/>
+      <c r="K32" s="178"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
@@ -8653,11 +8655,11 @@
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
       <c r="F33" s="32"/>
-      <c r="G33" s="139"/>
-      <c r="H33" s="141"/>
-      <c r="I33" s="175"/>
-      <c r="J33" s="176"/>
-      <c r="K33" s="177"/>
+      <c r="G33" s="140"/>
+      <c r="H33" s="142"/>
+      <c r="I33" s="176"/>
+      <c r="J33" s="177"/>
+      <c r="K33" s="178"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
       <c r="O33" s="22"/>
@@ -8675,11 +8677,11 @@
       <c r="D34" s="33"/>
       <c r="E34" s="33"/>
       <c r="F34" s="32"/>
-      <c r="G34" s="139"/>
-      <c r="H34" s="141"/>
-      <c r="I34" s="175"/>
-      <c r="J34" s="176"/>
-      <c r="K34" s="177"/>
+      <c r="G34" s="140"/>
+      <c r="H34" s="142"/>
+      <c r="I34" s="176"/>
+      <c r="J34" s="177"/>
+      <c r="K34" s="178"/>
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
       <c r="O34" s="22"/>
@@ -8697,11 +8699,11 @@
       <c r="D35" s="33"/>
       <c r="E35" s="33"/>
       <c r="F35" s="32"/>
-      <c r="G35" s="139"/>
-      <c r="H35" s="141"/>
-      <c r="I35" s="175"/>
-      <c r="J35" s="176"/>
-      <c r="K35" s="177"/>
+      <c r="G35" s="140"/>
+      <c r="H35" s="142"/>
+      <c r="I35" s="176"/>
+      <c r="J35" s="177"/>
+      <c r="K35" s="178"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="22"/>
@@ -8719,11 +8721,11 @@
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
       <c r="F36" s="32"/>
-      <c r="G36" s="139"/>
-      <c r="H36" s="141"/>
-      <c r="I36" s="175"/>
-      <c r="J36" s="176"/>
-      <c r="K36" s="177"/>
+      <c r="G36" s="140"/>
+      <c r="H36" s="142"/>
+      <c r="I36" s="176"/>
+      <c r="J36" s="177"/>
+      <c r="K36" s="178"/>
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
       <c r="O36" s="22"/>
@@ -8741,11 +8743,11 @@
       <c r="D37" s="33"/>
       <c r="E37" s="33"/>
       <c r="F37" s="32"/>
-      <c r="G37" s="139"/>
-      <c r="H37" s="141"/>
-      <c r="I37" s="175"/>
-      <c r="J37" s="176"/>
-      <c r="K37" s="177"/>
+      <c r="G37" s="140"/>
+      <c r="H37" s="142"/>
+      <c r="I37" s="176"/>
+      <c r="J37" s="177"/>
+      <c r="K37" s="178"/>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22"/>
@@ -8763,11 +8765,11 @@
       <c r="D38" s="33"/>
       <c r="E38" s="33"/>
       <c r="F38" s="32"/>
-      <c r="G38" s="139"/>
-      <c r="H38" s="141"/>
-      <c r="I38" s="175"/>
-      <c r="J38" s="176"/>
-      <c r="K38" s="177"/>
+      <c r="G38" s="140"/>
+      <c r="H38" s="142"/>
+      <c r="I38" s="176"/>
+      <c r="J38" s="177"/>
+      <c r="K38" s="178"/>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
       <c r="O38" s="22"/>
@@ -8785,11 +8787,11 @@
       <c r="D39" s="33"/>
       <c r="E39" s="33"/>
       <c r="F39" s="32"/>
-      <c r="G39" s="139"/>
-      <c r="H39" s="141"/>
-      <c r="I39" s="175"/>
-      <c r="J39" s="176"/>
-      <c r="K39" s="177"/>
+      <c r="G39" s="140"/>
+      <c r="H39" s="142"/>
+      <c r="I39" s="176"/>
+      <c r="J39" s="177"/>
+      <c r="K39" s="178"/>
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22"/>
@@ -8807,11 +8809,11 @@
       <c r="D40" s="33"/>
       <c r="E40" s="33"/>
       <c r="F40" s="32"/>
-      <c r="G40" s="139"/>
-      <c r="H40" s="141"/>
-      <c r="I40" s="175"/>
-      <c r="J40" s="176"/>
-      <c r="K40" s="177"/>
+      <c r="G40" s="140"/>
+      <c r="H40" s="142"/>
+      <c r="I40" s="176"/>
+      <c r="J40" s="177"/>
+      <c r="K40" s="178"/>
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
       <c r="O40" s="22"/>
@@ -8829,11 +8831,11 @@
       <c r="D41" s="33"/>
       <c r="E41" s="33"/>
       <c r="F41" s="32"/>
-      <c r="G41" s="139"/>
-      <c r="H41" s="141"/>
-      <c r="I41" s="175"/>
-      <c r="J41" s="176"/>
-      <c r="K41" s="177"/>
+      <c r="G41" s="140"/>
+      <c r="H41" s="142"/>
+      <c r="I41" s="176"/>
+      <c r="J41" s="177"/>
+      <c r="K41" s="178"/>
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22"/>
@@ -8851,11 +8853,11 @@
       <c r="D42" s="33"/>
       <c r="E42" s="33"/>
       <c r="F42" s="32"/>
-      <c r="G42" s="139"/>
-      <c r="H42" s="141"/>
-      <c r="I42" s="175"/>
-      <c r="J42" s="176"/>
-      <c r="K42" s="177"/>
+      <c r="G42" s="140"/>
+      <c r="H42" s="142"/>
+      <c r="I42" s="176"/>
+      <c r="J42" s="177"/>
+      <c r="K42" s="178"/>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
       <c r="O42" s="22"/>
@@ -8873,11 +8875,11 @@
       <c r="D43" s="33"/>
       <c r="E43" s="33"/>
       <c r="F43" s="32"/>
-      <c r="G43" s="139"/>
-      <c r="H43" s="141"/>
-      <c r="I43" s="175"/>
-      <c r="J43" s="176"/>
-      <c r="K43" s="177"/>
+      <c r="G43" s="140"/>
+      <c r="H43" s="142"/>
+      <c r="I43" s="176"/>
+      <c r="J43" s="177"/>
+      <c r="K43" s="178"/>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
       <c r="O43" s="22"/>
@@ -8895,11 +8897,11 @@
       <c r="D44" s="33"/>
       <c r="E44" s="33"/>
       <c r="F44" s="32"/>
-      <c r="G44" s="139"/>
-      <c r="H44" s="141"/>
-      <c r="I44" s="175"/>
-      <c r="J44" s="176"/>
-      <c r="K44" s="177"/>
+      <c r="G44" s="140"/>
+      <c r="H44" s="142"/>
+      <c r="I44" s="176"/>
+      <c r="J44" s="177"/>
+      <c r="K44" s="178"/>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
       <c r="O44" s="22"/>
@@ -8917,11 +8919,11 @@
       <c r="D45" s="33"/>
       <c r="E45" s="33"/>
       <c r="F45" s="32"/>
-      <c r="G45" s="139"/>
-      <c r="H45" s="141"/>
-      <c r="I45" s="175"/>
-      <c r="J45" s="176"/>
-      <c r="K45" s="177"/>
+      <c r="G45" s="140"/>
+      <c r="H45" s="142"/>
+      <c r="I45" s="176"/>
+      <c r="J45" s="177"/>
+      <c r="K45" s="178"/>
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
       <c r="O45" s="22"/>
@@ -8939,11 +8941,11 @@
       <c r="D46" s="33"/>
       <c r="E46" s="33"/>
       <c r="F46" s="32"/>
-      <c r="G46" s="139"/>
-      <c r="H46" s="141"/>
-      <c r="I46" s="175"/>
-      <c r="J46" s="176"/>
-      <c r="K46" s="177"/>
+      <c r="G46" s="140"/>
+      <c r="H46" s="142"/>
+      <c r="I46" s="176"/>
+      <c r="J46" s="177"/>
+      <c r="K46" s="178"/>
       <c r="M46" s="22"/>
       <c r="N46" s="22"/>
       <c r="O46" s="22"/>
@@ -8961,11 +8963,11 @@
       <c r="D47" s="33"/>
       <c r="E47" s="33"/>
       <c r="F47" s="32"/>
-      <c r="G47" s="139"/>
-      <c r="H47" s="141"/>
-      <c r="I47" s="175"/>
-      <c r="J47" s="176"/>
-      <c r="K47" s="177"/>
+      <c r="G47" s="140"/>
+      <c r="H47" s="142"/>
+      <c r="I47" s="176"/>
+      <c r="J47" s="177"/>
+      <c r="K47" s="178"/>
       <c r="M47" s="22"/>
       <c r="N47" s="22"/>
       <c r="O47" s="22"/>
@@ -8983,11 +8985,11 @@
       <c r="D48" s="33"/>
       <c r="E48" s="33"/>
       <c r="F48" s="32"/>
-      <c r="G48" s="139"/>
-      <c r="H48" s="141"/>
-      <c r="I48" s="175"/>
-      <c r="J48" s="176"/>
-      <c r="K48" s="177"/>
+      <c r="G48" s="140"/>
+      <c r="H48" s="142"/>
+      <c r="I48" s="176"/>
+      <c r="J48" s="177"/>
+      <c r="K48" s="178"/>
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
       <c r="O48" s="22"/>
@@ -9005,11 +9007,11 @@
       <c r="D49" s="33"/>
       <c r="E49" s="33"/>
       <c r="F49" s="32"/>
-      <c r="G49" s="139"/>
-      <c r="H49" s="141"/>
-      <c r="I49" s="175"/>
-      <c r="J49" s="176"/>
-      <c r="K49" s="177"/>
+      <c r="G49" s="140"/>
+      <c r="H49" s="142"/>
+      <c r="I49" s="176"/>
+      <c r="J49" s="177"/>
+      <c r="K49" s="178"/>
       <c r="M49" s="22"/>
       <c r="N49" s="22"/>
       <c r="O49" s="22"/>
@@ -9027,11 +9029,11 @@
       <c r="D50" s="33"/>
       <c r="E50" s="33"/>
       <c r="F50" s="32"/>
-      <c r="G50" s="139"/>
-      <c r="H50" s="141"/>
-      <c r="I50" s="175"/>
-      <c r="J50" s="176"/>
-      <c r="K50" s="177"/>
+      <c r="G50" s="140"/>
+      <c r="H50" s="142"/>
+      <c r="I50" s="176"/>
+      <c r="J50" s="177"/>
+      <c r="K50" s="178"/>
       <c r="M50" s="22"/>
       <c r="N50" s="22"/>
       <c r="O50" s="22"/>
@@ -9049,11 +9051,11 @@
       <c r="D51" s="33"/>
       <c r="E51" s="33"/>
       <c r="F51" s="32"/>
-      <c r="G51" s="139"/>
-      <c r="H51" s="141"/>
-      <c r="I51" s="175"/>
-      <c r="J51" s="176"/>
-      <c r="K51" s="177"/>
+      <c r="G51" s="140"/>
+      <c r="H51" s="142"/>
+      <c r="I51" s="176"/>
+      <c r="J51" s="177"/>
+      <c r="K51" s="178"/>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
       <c r="O51" s="22"/>
@@ -9071,11 +9073,11 @@
       <c r="D52" s="33"/>
       <c r="E52" s="33"/>
       <c r="F52" s="32"/>
-      <c r="G52" s="139"/>
-      <c r="H52" s="141"/>
-      <c r="I52" s="175"/>
-      <c r="J52" s="176"/>
-      <c r="K52" s="177"/>
+      <c r="G52" s="140"/>
+      <c r="H52" s="142"/>
+      <c r="I52" s="176"/>
+      <c r="J52" s="177"/>
+      <c r="K52" s="178"/>
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
       <c r="O52" s="22"/>
@@ -9093,11 +9095,11 @@
       <c r="D53" s="33"/>
       <c r="E53" s="33"/>
       <c r="F53" s="32"/>
-      <c r="G53" s="139"/>
-      <c r="H53" s="141"/>
-      <c r="I53" s="175"/>
-      <c r="J53" s="176"/>
-      <c r="K53" s="177"/>
+      <c r="G53" s="140"/>
+      <c r="H53" s="142"/>
+      <c r="I53" s="176"/>
+      <c r="J53" s="177"/>
+      <c r="K53" s="178"/>
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
       <c r="O53" s="22"/>
@@ -9115,11 +9117,11 @@
       <c r="D54" s="33"/>
       <c r="E54" s="33"/>
       <c r="F54" s="32"/>
-      <c r="G54" s="139"/>
-      <c r="H54" s="141"/>
-      <c r="I54" s="175"/>
-      <c r="J54" s="176"/>
-      <c r="K54" s="177"/>
+      <c r="G54" s="140"/>
+      <c r="H54" s="142"/>
+      <c r="I54" s="176"/>
+      <c r="J54" s="177"/>
+      <c r="K54" s="178"/>
       <c r="M54" s="22"/>
       <c r="N54" s="22"/>
       <c r="O54" s="22"/>
@@ -9137,11 +9139,11 @@
       <c r="D55" s="33"/>
       <c r="E55" s="33"/>
       <c r="F55" s="32"/>
-      <c r="G55" s="139"/>
-      <c r="H55" s="141"/>
-      <c r="I55" s="175"/>
-      <c r="J55" s="176"/>
-      <c r="K55" s="177"/>
+      <c r="G55" s="140"/>
+      <c r="H55" s="142"/>
+      <c r="I55" s="176"/>
+      <c r="J55" s="177"/>
+      <c r="K55" s="178"/>
       <c r="M55" s="22"/>
       <c r="N55" s="22"/>
       <c r="O55" s="22"/>
@@ -9159,11 +9161,11 @@
       <c r="D56" s="33"/>
       <c r="E56" s="33"/>
       <c r="F56" s="32"/>
-      <c r="G56" s="139"/>
-      <c r="H56" s="141"/>
-      <c r="I56" s="175"/>
-      <c r="J56" s="176"/>
-      <c r="K56" s="177"/>
+      <c r="G56" s="140"/>
+      <c r="H56" s="142"/>
+      <c r="I56" s="176"/>
+      <c r="J56" s="177"/>
+      <c r="K56" s="178"/>
       <c r="M56" s="22"/>
       <c r="N56" s="22"/>
       <c r="O56" s="22"/>
@@ -9303,8 +9305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1048469"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C10"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9333,24 +9335,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
       <c r="I1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="187" t="str">
+      <c r="J1" s="188" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="K1" s="187"/>
+      <c r="K1" s="188"/>
       <c r="L1" s="26" t="s">
         <v>3</v>
       </c>
@@ -9378,22 +9380,22 @@
       <c r="U1" s="52"/>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="145"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
       <c r="I2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="187" t="str">
+      <c r="J2" s="188" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT - CI</v>
       </c>
-      <c r="K2" s="187"/>
+      <c r="K2" s="188"/>
       <c r="L2" s="26" t="s">
         <v>50</v>
       </c>
@@ -9428,7 +9430,7 @@
         <v>233</v>
       </c>
       <c r="C4" s="125" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D4" s="67" t="s">
         <v>98</v>
@@ -9451,12 +9453,12 @@
       <c r="J4" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="153" t="s">
+      <c r="K4" s="154" t="s">
         <v>56</v>
       </c>
-      <c r="L4" s="155"/>
-      <c r="M4" s="155"/>
-      <c r="N4" s="154"/>
+      <c r="L4" s="156"/>
+      <c r="M4" s="156"/>
+      <c r="N4" s="155"/>
       <c r="O4" s="39" t="s">
         <v>57</v>
       </c>
@@ -9484,7 +9486,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E5" s="33"/>
       <c r="F5" s="32"/>
@@ -9500,22 +9502,22 @@
       <c r="J5" s="117" t="s">
         <v>215</v>
       </c>
-      <c r="K5" s="142" t="s">
-        <v>256</v>
-      </c>
-      <c r="L5" s="143"/>
-      <c r="M5" s="143"/>
-      <c r="N5" s="144"/>
+      <c r="K5" s="143" t="s">
+        <v>253</v>
+      </c>
+      <c r="L5" s="144"/>
+      <c r="M5" s="144"/>
+      <c r="N5" s="145"/>
       <c r="O5" s="85"/>
       <c r="P5" s="86"/>
       <c r="Q5" s="75" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R5" s="74" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="S5" s="85" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="T5" s="63"/>
       <c r="U5" s="63"/>
@@ -9531,7 +9533,7 @@
         <v>51</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E6" s="33"/>
       <c r="F6" s="32"/>
@@ -9543,31 +9545,31 @@
       <c r="J6" s="117" t="s">
         <v>216</v>
       </c>
-      <c r="K6" s="142" t="s">
-        <v>257</v>
-      </c>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="144"/>
+      <c r="K6" s="143" t="s">
+        <v>254</v>
+      </c>
+      <c r="L6" s="144"/>
+      <c r="M6" s="144"/>
+      <c r="N6" s="145"/>
       <c r="O6" s="121" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="P6" s="121" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="Q6" s="75" t="s">
         <v>106</v>
       </c>
       <c r="R6" s="74" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="S6" s="115" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="T6" s="63"/>
       <c r="U6" s="63"/>
     </row>
-    <row r="7" spans="1:21" s="34" customFormat="1" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="34" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
         <v>3</v>
       </c>
@@ -9578,10 +9580,10 @@
         <v>51</v>
       </c>
       <c r="D7" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="E7" s="40" t="s">
         <v>259</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>262</v>
       </c>
       <c r="F7" s="62"/>
       <c r="G7" s="85" t="s">
@@ -9596,26 +9598,26 @@
       <c r="J7" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="K7" s="142" t="s">
+      <c r="K7" s="143" t="s">
+        <v>273</v>
+      </c>
+      <c r="L7" s="144"/>
+      <c r="M7" s="144"/>
+      <c r="N7" s="145"/>
+      <c r="O7" s="121" t="s">
+        <v>274</v>
+      </c>
+      <c r="P7" s="121" t="s">
         <v>276</v>
       </c>
-      <c r="L7" s="143"/>
-      <c r="M7" s="143"/>
-      <c r="N7" s="144"/>
-      <c r="O7" s="121" t="s">
-        <v>277</v>
-      </c>
-      <c r="P7" s="121" t="s">
-        <v>279</v>
-      </c>
       <c r="Q7" s="75" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="R7" s="74" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="S7" s="85" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="T7" s="63"/>
       <c r="U7" s="63"/>
@@ -9631,16 +9633,16 @@
         <v>51</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F8" s="62" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G8" s="122" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H8" s="62" t="s">
         <v>212</v>
@@ -9651,26 +9653,26 @@
       <c r="J8" s="117" t="s">
         <v>218</v>
       </c>
-      <c r="K8" s="142" t="s">
-        <v>275</v>
-      </c>
-      <c r="L8" s="143"/>
-      <c r="M8" s="143"/>
-      <c r="N8" s="144"/>
+      <c r="K8" s="143" t="s">
+        <v>272</v>
+      </c>
+      <c r="L8" s="144"/>
+      <c r="M8" s="144"/>
+      <c r="N8" s="145"/>
       <c r="O8" s="121" t="s">
         <v>135</v>
       </c>
       <c r="P8" s="121" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="Q8" s="75" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="R8" s="74" t="s">
+        <v>283</v>
+      </c>
+      <c r="S8" s="122" t="s">
         <v>286</v>
-      </c>
-      <c r="S8" s="122" t="s">
-        <v>289</v>
       </c>
       <c r="T8" s="63"/>
       <c r="U8" s="63"/>
@@ -9686,14 +9688,14 @@
         <v>51</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="85" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H9" s="62" t="s">
         <v>212</v>
@@ -9704,26 +9706,26 @@
       <c r="J9" s="117" t="s">
         <v>220</v>
       </c>
-      <c r="K9" s="142" t="s">
-        <v>272</v>
-      </c>
-      <c r="L9" s="143"/>
-      <c r="M9" s="143"/>
-      <c r="N9" s="144"/>
+      <c r="K9" s="143" t="s">
+        <v>269</v>
+      </c>
+      <c r="L9" s="144"/>
+      <c r="M9" s="144"/>
+      <c r="N9" s="145"/>
       <c r="O9" s="121" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="P9" s="121" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="Q9" s="75" t="s">
         <v>106</v>
       </c>
       <c r="R9" s="74" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="S9" s="81" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="T9" s="63"/>
       <c r="U9" s="63"/>
@@ -9739,10 +9741,10 @@
         <v>51</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E10" s="121" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="85" t="s">
@@ -9755,28 +9757,28 @@
         <v>56</v>
       </c>
       <c r="J10" s="117" t="s">
-        <v>293</v>
-      </c>
-      <c r="K10" s="142" t="s">
-        <v>268</v>
-      </c>
-      <c r="L10" s="143"/>
-      <c r="M10" s="143"/>
-      <c r="N10" s="144"/>
+        <v>290</v>
+      </c>
+      <c r="K10" s="143" t="s">
+        <v>265</v>
+      </c>
+      <c r="L10" s="144"/>
+      <c r="M10" s="144"/>
+      <c r="N10" s="145"/>
       <c r="O10" s="121" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="P10" s="121" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="Q10" s="75" t="s">
+        <v>285</v>
+      </c>
+      <c r="R10" s="74" t="s">
+        <v>242</v>
+      </c>
+      <c r="S10" s="81" t="s">
         <v>288</v>
-      </c>
-      <c r="R10" s="74" t="s">
-        <v>245</v>
-      </c>
-      <c r="S10" s="81" t="s">
-        <v>291</v>
       </c>
       <c r="T10" s="63"/>
       <c r="U10" s="63"/>
@@ -9794,10 +9796,10 @@
       <c r="H11" s="62"/>
       <c r="I11" s="62"/>
       <c r="J11" s="81"/>
-      <c r="K11" s="184"/>
-      <c r="L11" s="185"/>
-      <c r="M11" s="185"/>
-      <c r="N11" s="186"/>
+      <c r="K11" s="185"/>
+      <c r="L11" s="186"/>
+      <c r="M11" s="186"/>
+      <c r="N11" s="187"/>
       <c r="O11" s="86"/>
       <c r="P11" s="86"/>
       <c r="Q11" s="75"/>
@@ -9819,10 +9821,10 @@
       <c r="H12" s="62"/>
       <c r="I12" s="62"/>
       <c r="J12" s="81"/>
-      <c r="K12" s="184"/>
-      <c r="L12" s="185"/>
-      <c r="M12" s="185"/>
-      <c r="N12" s="186"/>
+      <c r="K12" s="185"/>
+      <c r="L12" s="186"/>
+      <c r="M12" s="186"/>
+      <c r="N12" s="187"/>
       <c r="O12" s="86"/>
       <c r="P12" s="86"/>
       <c r="Q12" s="75"/>
@@ -9844,10 +9846,10 @@
       <c r="H13" s="62"/>
       <c r="I13" s="62"/>
       <c r="J13" s="81"/>
-      <c r="K13" s="184"/>
-      <c r="L13" s="185"/>
-      <c r="M13" s="185"/>
-      <c r="N13" s="186"/>
+      <c r="K13" s="185"/>
+      <c r="L13" s="186"/>
+      <c r="M13" s="186"/>
+      <c r="N13" s="187"/>
       <c r="O13" s="86"/>
       <c r="P13" s="86"/>
       <c r="Q13" s="75"/>
@@ -9869,10 +9871,10 @@
       <c r="H14" s="62"/>
       <c r="I14" s="62"/>
       <c r="J14" s="81"/>
-      <c r="K14" s="184"/>
-      <c r="L14" s="185"/>
-      <c r="M14" s="185"/>
-      <c r="N14" s="186"/>
+      <c r="K14" s="185"/>
+      <c r="L14" s="186"/>
+      <c r="M14" s="186"/>
+      <c r="N14" s="187"/>
       <c r="O14" s="83"/>
       <c r="P14" s="83"/>
       <c r="Q14" s="75"/>
@@ -9894,10 +9896,10 @@
       <c r="H15" s="62"/>
       <c r="I15" s="62"/>
       <c r="J15" s="81"/>
-      <c r="K15" s="184"/>
-      <c r="L15" s="185"/>
-      <c r="M15" s="185"/>
-      <c r="N15" s="186"/>
+      <c r="K15" s="185"/>
+      <c r="L15" s="186"/>
+      <c r="M15" s="186"/>
+      <c r="N15" s="187"/>
       <c r="O15" s="83"/>
       <c r="P15" s="83"/>
       <c r="Q15" s="75"/>
@@ -9919,10 +9921,10 @@
       <c r="H16" s="62"/>
       <c r="I16" s="62"/>
       <c r="J16" s="81"/>
-      <c r="K16" s="184"/>
-      <c r="L16" s="185"/>
-      <c r="M16" s="185"/>
-      <c r="N16" s="186"/>
+      <c r="K16" s="185"/>
+      <c r="L16" s="186"/>
+      <c r="M16" s="186"/>
+      <c r="N16" s="187"/>
       <c r="O16" s="80"/>
       <c r="P16" s="80"/>
       <c r="Q16" s="75"/>
@@ -9944,10 +9946,10 @@
       <c r="H17" s="62"/>
       <c r="I17" s="62"/>
       <c r="J17" s="81"/>
-      <c r="K17" s="184"/>
-      <c r="L17" s="185"/>
-      <c r="M17" s="185"/>
-      <c r="N17" s="186"/>
+      <c r="K17" s="185"/>
+      <c r="L17" s="186"/>
+      <c r="M17" s="186"/>
+      <c r="N17" s="187"/>
       <c r="O17" s="80"/>
       <c r="P17" s="80"/>
       <c r="Q17" s="75"/>
@@ -9969,10 +9971,10 @@
       <c r="H18" s="62"/>
       <c r="I18" s="62"/>
       <c r="J18" s="40"/>
-      <c r="K18" s="184"/>
-      <c r="L18" s="185"/>
-      <c r="M18" s="185"/>
-      <c r="N18" s="186"/>
+      <c r="K18" s="185"/>
+      <c r="L18" s="186"/>
+      <c r="M18" s="186"/>
+      <c r="N18" s="187"/>
       <c r="O18" s="71"/>
       <c r="P18" s="59"/>
       <c r="Q18" s="75"/>
@@ -9994,10 +9996,10 @@
       <c r="H19" s="62"/>
       <c r="I19" s="62"/>
       <c r="J19" s="40"/>
-      <c r="K19" s="184"/>
-      <c r="L19" s="185"/>
-      <c r="M19" s="185"/>
-      <c r="N19" s="186"/>
+      <c r="K19" s="185"/>
+      <c r="L19" s="186"/>
+      <c r="M19" s="186"/>
+      <c r="N19" s="187"/>
       <c r="O19" s="59"/>
       <c r="P19" s="59"/>
       <c r="Q19" s="75"/>
@@ -10019,10 +10021,10 @@
       <c r="H20" s="62"/>
       <c r="I20" s="62"/>
       <c r="J20" s="40"/>
-      <c r="K20" s="184"/>
-      <c r="L20" s="185"/>
-      <c r="M20" s="185"/>
-      <c r="N20" s="186"/>
+      <c r="K20" s="185"/>
+      <c r="L20" s="186"/>
+      <c r="M20" s="186"/>
+      <c r="N20" s="187"/>
       <c r="O20" s="59"/>
       <c r="P20" s="59"/>
       <c r="Q20" s="75"/>
@@ -10044,10 +10046,10 @@
       <c r="H21" s="62"/>
       <c r="I21" s="62"/>
       <c r="J21" s="40"/>
-      <c r="K21" s="184"/>
-      <c r="L21" s="185"/>
-      <c r="M21" s="185"/>
-      <c r="N21" s="186"/>
+      <c r="K21" s="185"/>
+      <c r="L21" s="186"/>
+      <c r="M21" s="186"/>
+      <c r="N21" s="187"/>
       <c r="O21" s="59"/>
       <c r="P21" s="59"/>
       <c r="Q21" s="75"/>
@@ -10069,10 +10071,10 @@
       <c r="H22" s="62"/>
       <c r="I22" s="62"/>
       <c r="J22" s="40"/>
-      <c r="K22" s="184"/>
-      <c r="L22" s="185"/>
-      <c r="M22" s="185"/>
-      <c r="N22" s="186"/>
+      <c r="K22" s="185"/>
+      <c r="L22" s="186"/>
+      <c r="M22" s="186"/>
+      <c r="N22" s="187"/>
       <c r="O22" s="59"/>
       <c r="P22" s="59"/>
       <c r="Q22" s="75"/>
@@ -10094,10 +10096,10 @@
       <c r="H23" s="62"/>
       <c r="I23" s="62"/>
       <c r="J23" s="40"/>
-      <c r="K23" s="184"/>
-      <c r="L23" s="185"/>
-      <c r="M23" s="185"/>
-      <c r="N23" s="186"/>
+      <c r="K23" s="185"/>
+      <c r="L23" s="186"/>
+      <c r="M23" s="186"/>
+      <c r="N23" s="187"/>
       <c r="O23" s="59"/>
       <c r="P23" s="59"/>
       <c r="Q23" s="75"/>
@@ -10119,10 +10121,10 @@
       <c r="H24" s="62"/>
       <c r="I24" s="62"/>
       <c r="J24" s="40"/>
-      <c r="K24" s="184"/>
-      <c r="L24" s="185"/>
-      <c r="M24" s="185"/>
-      <c r="N24" s="186"/>
+      <c r="K24" s="185"/>
+      <c r="L24" s="186"/>
+      <c r="M24" s="186"/>
+      <c r="N24" s="187"/>
       <c r="O24" s="59"/>
       <c r="P24" s="59"/>
       <c r="Q24" s="75"/>
@@ -10144,10 +10146,10 @@
       <c r="H25" s="62"/>
       <c r="I25" s="62"/>
       <c r="J25" s="40"/>
-      <c r="K25" s="184"/>
-      <c r="L25" s="185"/>
-      <c r="M25" s="185"/>
-      <c r="N25" s="186"/>
+      <c r="K25" s="185"/>
+      <c r="L25" s="186"/>
+      <c r="M25" s="186"/>
+      <c r="N25" s="187"/>
       <c r="O25" s="59"/>
       <c r="P25" s="59"/>
       <c r="Q25" s="75"/>
@@ -10169,10 +10171,10 @@
       <c r="H26" s="62"/>
       <c r="I26" s="62"/>
       <c r="J26" s="40"/>
-      <c r="K26" s="184"/>
-      <c r="L26" s="185"/>
-      <c r="M26" s="185"/>
-      <c r="N26" s="186"/>
+      <c r="K26" s="185"/>
+      <c r="L26" s="186"/>
+      <c r="M26" s="186"/>
+      <c r="N26" s="187"/>
       <c r="O26" s="59"/>
       <c r="P26" s="59"/>
       <c r="Q26" s="75"/>
@@ -10194,10 +10196,10 @@
       <c r="H27" s="62"/>
       <c r="I27" s="62"/>
       <c r="J27" s="40"/>
-      <c r="K27" s="184"/>
-      <c r="L27" s="185"/>
-      <c r="M27" s="185"/>
-      <c r="N27" s="186"/>
+      <c r="K27" s="185"/>
+      <c r="L27" s="186"/>
+      <c r="M27" s="186"/>
+      <c r="N27" s="187"/>
       <c r="O27" s="59"/>
       <c r="P27" s="59"/>
       <c r="Q27" s="75"/>
@@ -10219,10 +10221,10 @@
       <c r="H28" s="62"/>
       <c r="I28" s="62"/>
       <c r="J28" s="40"/>
-      <c r="K28" s="184"/>
-      <c r="L28" s="185"/>
-      <c r="M28" s="185"/>
-      <c r="N28" s="186"/>
+      <c r="K28" s="185"/>
+      <c r="L28" s="186"/>
+      <c r="M28" s="186"/>
+      <c r="N28" s="187"/>
       <c r="O28" s="59"/>
       <c r="P28" s="59"/>
       <c r="Q28" s="75"/>
@@ -10244,10 +10246,10 @@
       <c r="H29" s="62"/>
       <c r="I29" s="62"/>
       <c r="J29" s="40"/>
-      <c r="K29" s="184"/>
-      <c r="L29" s="185"/>
-      <c r="M29" s="185"/>
-      <c r="N29" s="186"/>
+      <c r="K29" s="185"/>
+      <c r="L29" s="186"/>
+      <c r="M29" s="186"/>
+      <c r="N29" s="187"/>
       <c r="O29" s="59"/>
       <c r="P29" s="59"/>
       <c r="Q29" s="75"/>
@@ -10269,10 +10271,10 @@
       <c r="H30" s="62"/>
       <c r="I30" s="62"/>
       <c r="J30" s="40"/>
-      <c r="K30" s="184"/>
-      <c r="L30" s="185"/>
-      <c r="M30" s="185"/>
-      <c r="N30" s="186"/>
+      <c r="K30" s="185"/>
+      <c r="L30" s="186"/>
+      <c r="M30" s="186"/>
+      <c r="N30" s="187"/>
       <c r="O30" s="59"/>
       <c r="P30" s="59"/>
       <c r="Q30" s="75"/>
@@ -10294,10 +10296,10 @@
       <c r="H31" s="62"/>
       <c r="I31" s="62"/>
       <c r="J31" s="40"/>
-      <c r="K31" s="184"/>
-      <c r="L31" s="185"/>
-      <c r="M31" s="185"/>
-      <c r="N31" s="186"/>
+      <c r="K31" s="185"/>
+      <c r="L31" s="186"/>
+      <c r="M31" s="186"/>
+      <c r="N31" s="187"/>
       <c r="O31" s="59"/>
       <c r="P31" s="59"/>
       <c r="Q31" s="75"/>
@@ -10319,10 +10321,10 @@
       <c r="H32" s="62"/>
       <c r="I32" s="62"/>
       <c r="J32" s="40"/>
-      <c r="K32" s="184"/>
-      <c r="L32" s="185"/>
-      <c r="M32" s="185"/>
-      <c r="N32" s="186"/>
+      <c r="K32" s="185"/>
+      <c r="L32" s="186"/>
+      <c r="M32" s="186"/>
+      <c r="N32" s="187"/>
       <c r="O32" s="59"/>
       <c r="P32" s="59"/>
       <c r="Q32" s="75"/>
@@ -10344,10 +10346,10 @@
       <c r="H33" s="62"/>
       <c r="I33" s="62"/>
       <c r="J33" s="40"/>
-      <c r="K33" s="184"/>
-      <c r="L33" s="185"/>
-      <c r="M33" s="185"/>
-      <c r="N33" s="186"/>
+      <c r="K33" s="185"/>
+      <c r="L33" s="186"/>
+      <c r="M33" s="186"/>
+      <c r="N33" s="187"/>
       <c r="O33" s="59"/>
       <c r="P33" s="59"/>
       <c r="Q33" s="75"/>
@@ -10369,10 +10371,10 @@
       <c r="H34" s="62"/>
       <c r="I34" s="62"/>
       <c r="J34" s="40"/>
-      <c r="K34" s="184"/>
-      <c r="L34" s="185"/>
-      <c r="M34" s="185"/>
-      <c r="N34" s="186"/>
+      <c r="K34" s="185"/>
+      <c r="L34" s="186"/>
+      <c r="M34" s="186"/>
+      <c r="N34" s="187"/>
       <c r="O34" s="59"/>
       <c r="P34" s="59"/>
       <c r="Q34" s="75"/>
@@ -10394,10 +10396,10 @@
       <c r="H35" s="62"/>
       <c r="I35" s="62"/>
       <c r="J35" s="40"/>
-      <c r="K35" s="184"/>
-      <c r="L35" s="185"/>
-      <c r="M35" s="185"/>
-      <c r="N35" s="186"/>
+      <c r="K35" s="185"/>
+      <c r="L35" s="186"/>
+      <c r="M35" s="186"/>
+      <c r="N35" s="187"/>
       <c r="O35" s="59"/>
       <c r="P35" s="59"/>
       <c r="Q35" s="75"/>
@@ -10419,10 +10421,10 @@
       <c r="H36" s="62"/>
       <c r="I36" s="62"/>
       <c r="J36" s="81"/>
-      <c r="K36" s="184"/>
-      <c r="L36" s="185"/>
-      <c r="M36" s="185"/>
-      <c r="N36" s="186"/>
+      <c r="K36" s="185"/>
+      <c r="L36" s="186"/>
+      <c r="M36" s="186"/>
+      <c r="N36" s="187"/>
       <c r="O36" s="83"/>
       <c r="P36" s="83"/>
       <c r="Q36" s="75"/>
@@ -10444,10 +10446,10 @@
       <c r="H37" s="62"/>
       <c r="I37" s="62"/>
       <c r="J37" s="40"/>
-      <c r="K37" s="184"/>
-      <c r="L37" s="185"/>
-      <c r="M37" s="185"/>
-      <c r="N37" s="186"/>
+      <c r="K37" s="185"/>
+      <c r="L37" s="186"/>
+      <c r="M37" s="186"/>
+      <c r="N37" s="187"/>
       <c r="O37" s="59"/>
       <c r="P37" s="59"/>
       <c r="Q37" s="75"/>
@@ -10469,10 +10471,10 @@
       <c r="H38" s="62"/>
       <c r="I38" s="62"/>
       <c r="J38" s="40"/>
-      <c r="K38" s="184"/>
-      <c r="L38" s="185"/>
-      <c r="M38" s="185"/>
-      <c r="N38" s="186"/>
+      <c r="K38" s="185"/>
+      <c r="L38" s="186"/>
+      <c r="M38" s="186"/>
+      <c r="N38" s="187"/>
       <c r="O38" s="59"/>
       <c r="P38" s="59"/>
       <c r="Q38" s="75"/>
@@ -10494,10 +10496,10 @@
       <c r="H39" s="62"/>
       <c r="I39" s="62"/>
       <c r="J39" s="40"/>
-      <c r="K39" s="184"/>
-      <c r="L39" s="185"/>
-      <c r="M39" s="185"/>
-      <c r="N39" s="186"/>
+      <c r="K39" s="185"/>
+      <c r="L39" s="186"/>
+      <c r="M39" s="186"/>
+      <c r="N39" s="187"/>
       <c r="O39" s="59"/>
       <c r="P39" s="59"/>
       <c r="Q39" s="75"/>
@@ -10519,10 +10521,10 @@
       <c r="H40" s="62"/>
       <c r="I40" s="62"/>
       <c r="J40" s="40"/>
-      <c r="K40" s="184"/>
-      <c r="L40" s="185"/>
-      <c r="M40" s="185"/>
-      <c r="N40" s="186"/>
+      <c r="K40" s="185"/>
+      <c r="L40" s="186"/>
+      <c r="M40" s="186"/>
+      <c r="N40" s="187"/>
       <c r="O40" s="59"/>
       <c r="P40" s="59"/>
       <c r="Q40" s="75"/>
@@ -10544,10 +10546,10 @@
       <c r="H41" s="62"/>
       <c r="I41" s="62"/>
       <c r="J41" s="40"/>
-      <c r="K41" s="184"/>
-      <c r="L41" s="185"/>
-      <c r="M41" s="185"/>
-      <c r="N41" s="186"/>
+      <c r="K41" s="185"/>
+      <c r="L41" s="186"/>
+      <c r="M41" s="186"/>
+      <c r="N41" s="187"/>
       <c r="O41" s="59"/>
       <c r="P41" s="59"/>
       <c r="Q41" s="75"/>
@@ -10569,10 +10571,10 @@
       <c r="H42" s="62"/>
       <c r="I42" s="62"/>
       <c r="J42" s="40"/>
-      <c r="K42" s="184"/>
-      <c r="L42" s="185"/>
-      <c r="M42" s="185"/>
-      <c r="N42" s="186"/>
+      <c r="K42" s="185"/>
+      <c r="L42" s="186"/>
+      <c r="M42" s="186"/>
+      <c r="N42" s="187"/>
       <c r="O42" s="73"/>
       <c r="P42" s="73"/>
       <c r="Q42" s="75"/>
@@ -10594,10 +10596,10 @@
       <c r="H43" s="62"/>
       <c r="I43" s="62"/>
       <c r="J43" s="40"/>
-      <c r="K43" s="184"/>
-      <c r="L43" s="185"/>
-      <c r="M43" s="185"/>
-      <c r="N43" s="186"/>
+      <c r="K43" s="185"/>
+      <c r="L43" s="186"/>
+      <c r="M43" s="186"/>
+      <c r="N43" s="187"/>
       <c r="O43" s="73"/>
       <c r="P43" s="73"/>
       <c r="Q43" s="75"/>
@@ -10619,10 +10621,10 @@
       <c r="H44" s="62"/>
       <c r="I44" s="62"/>
       <c r="J44" s="40"/>
-      <c r="K44" s="184"/>
-      <c r="L44" s="185"/>
-      <c r="M44" s="185"/>
-      <c r="N44" s="186"/>
+      <c r="K44" s="185"/>
+      <c r="L44" s="186"/>
+      <c r="M44" s="186"/>
+      <c r="N44" s="187"/>
       <c r="O44" s="73"/>
       <c r="P44" s="73"/>
       <c r="Q44" s="75"/>
@@ -10644,10 +10646,10 @@
       <c r="H45" s="62"/>
       <c r="I45" s="62"/>
       <c r="J45" s="40"/>
-      <c r="K45" s="184"/>
-      <c r="L45" s="185"/>
-      <c r="M45" s="185"/>
-      <c r="N45" s="186"/>
+      <c r="K45" s="185"/>
+      <c r="L45" s="186"/>
+      <c r="M45" s="186"/>
+      <c r="N45" s="187"/>
       <c r="O45" s="73"/>
       <c r="P45" s="73"/>
       <c r="Q45" s="75"/>
@@ -10669,10 +10671,10 @@
       <c r="H46" s="62"/>
       <c r="I46" s="62"/>
       <c r="J46" s="40"/>
-      <c r="K46" s="184"/>
-      <c r="L46" s="185"/>
-      <c r="M46" s="185"/>
-      <c r="N46" s="186"/>
+      <c r="K46" s="185"/>
+      <c r="L46" s="186"/>
+      <c r="M46" s="186"/>
+      <c r="N46" s="187"/>
       <c r="O46" s="73"/>
       <c r="P46" s="73"/>
       <c r="Q46" s="75"/>
@@ -10694,10 +10696,10 @@
       <c r="H47" s="62"/>
       <c r="I47" s="62"/>
       <c r="J47" s="40"/>
-      <c r="K47" s="184"/>
-      <c r="L47" s="185"/>
-      <c r="M47" s="185"/>
-      <c r="N47" s="186"/>
+      <c r="K47" s="185"/>
+      <c r="L47" s="186"/>
+      <c r="M47" s="186"/>
+      <c r="N47" s="187"/>
       <c r="O47" s="73"/>
       <c r="P47" s="73"/>
       <c r="Q47" s="75"/>
@@ -10719,10 +10721,10 @@
       <c r="H48" s="62"/>
       <c r="I48" s="62"/>
       <c r="J48" s="40"/>
-      <c r="K48" s="184"/>
-      <c r="L48" s="185"/>
-      <c r="M48" s="185"/>
-      <c r="N48" s="186"/>
+      <c r="K48" s="185"/>
+      <c r="L48" s="186"/>
+      <c r="M48" s="186"/>
+      <c r="N48" s="187"/>
       <c r="O48" s="73"/>
       <c r="P48" s="73"/>
       <c r="Q48" s="75"/>
@@ -10744,10 +10746,10 @@
       <c r="H49" s="62"/>
       <c r="I49" s="62"/>
       <c r="J49" s="40"/>
-      <c r="K49" s="184"/>
-      <c r="L49" s="185"/>
-      <c r="M49" s="185"/>
-      <c r="N49" s="186"/>
+      <c r="K49" s="185"/>
+      <c r="L49" s="186"/>
+      <c r="M49" s="186"/>
+      <c r="N49" s="187"/>
       <c r="O49" s="73"/>
       <c r="P49" s="73"/>
       <c r="Q49" s="75"/>
@@ -10769,10 +10771,10 @@
       <c r="H50" s="62"/>
       <c r="I50" s="62"/>
       <c r="J50" s="40"/>
-      <c r="K50" s="184"/>
-      <c r="L50" s="185"/>
-      <c r="M50" s="185"/>
-      <c r="N50" s="186"/>
+      <c r="K50" s="185"/>
+      <c r="L50" s="186"/>
+      <c r="M50" s="186"/>
+      <c r="N50" s="187"/>
       <c r="O50" s="73"/>
       <c r="P50" s="73"/>
       <c r="Q50" s="75"/>
@@ -10794,10 +10796,10 @@
       <c r="H51" s="62"/>
       <c r="I51" s="62"/>
       <c r="J51" s="40"/>
-      <c r="K51" s="184"/>
-      <c r="L51" s="185"/>
-      <c r="M51" s="185"/>
-      <c r="N51" s="186"/>
+      <c r="K51" s="185"/>
+      <c r="L51" s="186"/>
+      <c r="M51" s="186"/>
+      <c r="N51" s="187"/>
       <c r="O51" s="73"/>
       <c r="P51" s="73"/>
       <c r="Q51" s="75"/>
@@ -10819,10 +10821,10 @@
       <c r="H52" s="62"/>
       <c r="I52" s="62"/>
       <c r="J52" s="40"/>
-      <c r="K52" s="184"/>
-      <c r="L52" s="185"/>
-      <c r="M52" s="185"/>
-      <c r="N52" s="186"/>
+      <c r="K52" s="185"/>
+      <c r="L52" s="186"/>
+      <c r="M52" s="186"/>
+      <c r="N52" s="187"/>
       <c r="O52" s="73"/>
       <c r="P52" s="73"/>
       <c r="Q52" s="75"/>
@@ -10844,10 +10846,10 @@
       <c r="H53" s="62"/>
       <c r="I53" s="62"/>
       <c r="J53" s="40"/>
-      <c r="K53" s="184"/>
-      <c r="L53" s="185"/>
-      <c r="M53" s="185"/>
-      <c r="N53" s="186"/>
+      <c r="K53" s="185"/>
+      <c r="L53" s="186"/>
+      <c r="M53" s="186"/>
+      <c r="N53" s="187"/>
       <c r="O53" s="73"/>
       <c r="P53" s="73"/>
       <c r="Q53" s="75"/>
@@ -10869,10 +10871,10 @@
       <c r="H54" s="62"/>
       <c r="I54" s="62"/>
       <c r="J54" s="40"/>
-      <c r="K54" s="184"/>
-      <c r="L54" s="185"/>
-      <c r="M54" s="185"/>
-      <c r="N54" s="186"/>
+      <c r="K54" s="185"/>
+      <c r="L54" s="186"/>
+      <c r="M54" s="186"/>
+      <c r="N54" s="187"/>
       <c r="O54" s="73"/>
       <c r="P54" s="73"/>
       <c r="Q54" s="75"/>
@@ -10894,10 +10896,10 @@
       <c r="H55" s="62"/>
       <c r="I55" s="62"/>
       <c r="J55" s="40"/>
-      <c r="K55" s="184"/>
-      <c r="L55" s="185"/>
-      <c r="M55" s="185"/>
-      <c r="N55" s="186"/>
+      <c r="K55" s="185"/>
+      <c r="L55" s="186"/>
+      <c r="M55" s="186"/>
+      <c r="N55" s="187"/>
       <c r="O55" s="73"/>
       <c r="P55" s="73"/>
       <c r="Q55" s="75"/>
@@ -10919,10 +10921,10 @@
       <c r="H56" s="62"/>
       <c r="I56" s="62"/>
       <c r="J56" s="40"/>
-      <c r="K56" s="184"/>
-      <c r="L56" s="185"/>
-      <c r="M56" s="185"/>
-      <c r="N56" s="186"/>
+      <c r="K56" s="185"/>
+      <c r="L56" s="186"/>
+      <c r="M56" s="186"/>
+      <c r="N56" s="187"/>
       <c r="O56" s="73"/>
       <c r="P56" s="73"/>
       <c r="Q56" s="75"/>
@@ -10944,10 +10946,10 @@
       <c r="H57" s="62"/>
       <c r="I57" s="62"/>
       <c r="J57" s="40"/>
-      <c r="K57" s="184"/>
-      <c r="L57" s="185"/>
-      <c r="M57" s="185"/>
-      <c r="N57" s="186"/>
+      <c r="K57" s="185"/>
+      <c r="L57" s="186"/>
+      <c r="M57" s="186"/>
+      <c r="N57" s="187"/>
       <c r="O57" s="73"/>
       <c r="P57" s="73"/>
       <c r="Q57" s="75"/>
@@ -10969,10 +10971,10 @@
       <c r="H58" s="62"/>
       <c r="I58" s="62"/>
       <c r="J58" s="40"/>
-      <c r="K58" s="184"/>
-      <c r="L58" s="185"/>
-      <c r="M58" s="185"/>
-      <c r="N58" s="186"/>
+      <c r="K58" s="185"/>
+      <c r="L58" s="186"/>
+      <c r="M58" s="186"/>
+      <c r="N58" s="187"/>
       <c r="O58" s="73"/>
       <c r="P58" s="73"/>
       <c r="Q58" s="75"/>
@@ -10994,10 +10996,10 @@
       <c r="H59" s="62"/>
       <c r="I59" s="62"/>
       <c r="J59" s="40"/>
-      <c r="K59" s="184"/>
-      <c r="L59" s="185"/>
-      <c r="M59" s="185"/>
-      <c r="N59" s="186"/>
+      <c r="K59" s="185"/>
+      <c r="L59" s="186"/>
+      <c r="M59" s="186"/>
+      <c r="N59" s="187"/>
       <c r="O59" s="73"/>
       <c r="P59" s="73"/>
       <c r="Q59" s="75"/>
@@ -11019,10 +11021,10 @@
       <c r="H60" s="62"/>
       <c r="I60" s="62"/>
       <c r="J60" s="40"/>
-      <c r="K60" s="184"/>
-      <c r="L60" s="185"/>
-      <c r="M60" s="185"/>
-      <c r="N60" s="186"/>
+      <c r="K60" s="185"/>
+      <c r="L60" s="186"/>
+      <c r="M60" s="186"/>
+      <c r="N60" s="187"/>
       <c r="O60" s="73"/>
       <c r="P60" s="73"/>
       <c r="Q60" s="75"/>
@@ -11044,10 +11046,10 @@
       <c r="H61" s="62"/>
       <c r="I61" s="62"/>
       <c r="J61" s="40"/>
-      <c r="K61" s="184"/>
-      <c r="L61" s="185"/>
-      <c r="M61" s="185"/>
-      <c r="N61" s="186"/>
+      <c r="K61" s="185"/>
+      <c r="L61" s="186"/>
+      <c r="M61" s="186"/>
+      <c r="N61" s="187"/>
       <c r="O61" s="73"/>
       <c r="P61" s="73"/>
       <c r="Q61" s="75"/>
@@ -11069,10 +11071,10 @@
       <c r="H62" s="62"/>
       <c r="I62" s="62"/>
       <c r="J62" s="40"/>
-      <c r="K62" s="184"/>
-      <c r="L62" s="185"/>
-      <c r="M62" s="185"/>
-      <c r="N62" s="186"/>
+      <c r="K62" s="185"/>
+      <c r="L62" s="186"/>
+      <c r="M62" s="186"/>
+      <c r="N62" s="187"/>
       <c r="O62" s="73"/>
       <c r="P62" s="73"/>
       <c r="Q62" s="75"/>
@@ -11094,10 +11096,10 @@
       <c r="H63" s="62"/>
       <c r="I63" s="62"/>
       <c r="J63" s="40"/>
-      <c r="K63" s="184"/>
-      <c r="L63" s="185"/>
-      <c r="M63" s="185"/>
-      <c r="N63" s="186"/>
+      <c r="K63" s="185"/>
+      <c r="L63" s="186"/>
+      <c r="M63" s="186"/>
+      <c r="N63" s="187"/>
       <c r="O63" s="73"/>
       <c r="P63" s="73"/>
       <c r="Q63" s="75"/>
@@ -11119,10 +11121,10 @@
       <c r="H64" s="62"/>
       <c r="I64" s="62"/>
       <c r="J64" s="40"/>
-      <c r="K64" s="184"/>
-      <c r="L64" s="185"/>
-      <c r="M64" s="185"/>
-      <c r="N64" s="186"/>
+      <c r="K64" s="185"/>
+      <c r="L64" s="186"/>
+      <c r="M64" s="186"/>
+      <c r="N64" s="187"/>
       <c r="O64" s="82"/>
       <c r="P64" s="82"/>
       <c r="Q64" s="75"/>
@@ -11144,10 +11146,10 @@
       <c r="H65" s="62"/>
       <c r="I65" s="62"/>
       <c r="J65" s="40"/>
-      <c r="K65" s="184"/>
-      <c r="L65" s="185"/>
-      <c r="M65" s="185"/>
-      <c r="N65" s="186"/>
+      <c r="K65" s="185"/>
+      <c r="L65" s="186"/>
+      <c r="M65" s="186"/>
+      <c r="N65" s="187"/>
       <c r="O65" s="82"/>
       <c r="P65" s="82"/>
       <c r="Q65" s="75"/>
@@ -11169,10 +11171,10 @@
       <c r="H66" s="62"/>
       <c r="I66" s="62"/>
       <c r="J66" s="40"/>
-      <c r="K66" s="184"/>
-      <c r="L66" s="185"/>
-      <c r="M66" s="185"/>
-      <c r="N66" s="186"/>
+      <c r="K66" s="185"/>
+      <c r="L66" s="186"/>
+      <c r="M66" s="186"/>
+      <c r="N66" s="187"/>
       <c r="O66" s="82"/>
       <c r="P66" s="82"/>
       <c r="Q66" s="75"/>
@@ -11192,10 +11194,10 @@
       <c r="H67" s="62"/>
       <c r="I67" s="62"/>
       <c r="J67" s="40"/>
-      <c r="K67" s="184"/>
-      <c r="L67" s="185"/>
-      <c r="M67" s="185"/>
-      <c r="N67" s="186"/>
+      <c r="K67" s="185"/>
+      <c r="L67" s="186"/>
+      <c r="M67" s="186"/>
+      <c r="N67" s="187"/>
       <c r="O67" s="82"/>
       <c r="P67" s="82"/>
       <c r="Q67" s="75"/>
@@ -11215,10 +11217,10 @@
       <c r="H68" s="62"/>
       <c r="I68" s="62"/>
       <c r="J68" s="40"/>
-      <c r="K68" s="184"/>
-      <c r="L68" s="185"/>
-      <c r="M68" s="185"/>
-      <c r="N68" s="186"/>
+      <c r="K68" s="185"/>
+      <c r="L68" s="186"/>
+      <c r="M68" s="186"/>
+      <c r="N68" s="187"/>
       <c r="O68" s="82"/>
       <c r="P68" s="82"/>
       <c r="Q68" s="75"/>
@@ -11238,10 +11240,10 @@
       <c r="H69" s="62"/>
       <c r="I69" s="62"/>
       <c r="J69" s="40"/>
-      <c r="K69" s="184"/>
-      <c r="L69" s="185"/>
-      <c r="M69" s="185"/>
-      <c r="N69" s="186"/>
+      <c r="K69" s="185"/>
+      <c r="L69" s="186"/>
+      <c r="M69" s="186"/>
+      <c r="N69" s="187"/>
       <c r="O69" s="82"/>
       <c r="P69" s="82"/>
       <c r="Q69" s="75"/>
@@ -11261,10 +11263,10 @@
       <c r="H70" s="62"/>
       <c r="I70" s="62"/>
       <c r="J70" s="40"/>
-      <c r="K70" s="184"/>
-      <c r="L70" s="185"/>
-      <c r="M70" s="185"/>
-      <c r="N70" s="186"/>
+      <c r="K70" s="185"/>
+      <c r="L70" s="186"/>
+      <c r="M70" s="186"/>
+      <c r="N70" s="187"/>
       <c r="O70" s="82"/>
       <c r="P70" s="82"/>
       <c r="Q70" s="75"/>
@@ -11284,10 +11286,10 @@
       <c r="H71" s="62"/>
       <c r="I71" s="62"/>
       <c r="J71" s="40"/>
-      <c r="K71" s="184"/>
-      <c r="L71" s="185"/>
-      <c r="M71" s="185"/>
-      <c r="N71" s="186"/>
+      <c r="K71" s="185"/>
+      <c r="L71" s="186"/>
+      <c r="M71" s="186"/>
+      <c r="N71" s="187"/>
       <c r="O71" s="82"/>
       <c r="P71" s="82"/>
       <c r="Q71" s="75"/>
@@ -11307,10 +11309,10 @@
       <c r="H72" s="62"/>
       <c r="I72" s="62"/>
       <c r="J72" s="40"/>
-      <c r="K72" s="184"/>
-      <c r="L72" s="185"/>
-      <c r="M72" s="185"/>
-      <c r="N72" s="186"/>
+      <c r="K72" s="185"/>
+      <c r="L72" s="186"/>
+      <c r="M72" s="186"/>
+      <c r="N72" s="187"/>
       <c r="O72" s="82"/>
       <c r="P72" s="82"/>
       <c r="Q72" s="75"/>
@@ -11330,10 +11332,10 @@
       <c r="H73" s="62"/>
       <c r="I73" s="62"/>
       <c r="J73" s="40"/>
-      <c r="K73" s="184"/>
-      <c r="L73" s="185"/>
-      <c r="M73" s="185"/>
-      <c r="N73" s="186"/>
+      <c r="K73" s="185"/>
+      <c r="L73" s="186"/>
+      <c r="M73" s="186"/>
+      <c r="N73" s="187"/>
       <c r="O73" s="82"/>
       <c r="P73" s="82"/>
       <c r="Q73" s="75"/>
@@ -11353,10 +11355,10 @@
       <c r="H74" s="62"/>
       <c r="I74" s="62"/>
       <c r="J74" s="40"/>
-      <c r="K74" s="184"/>
-      <c r="L74" s="185"/>
-      <c r="M74" s="185"/>
-      <c r="N74" s="186"/>
+      <c r="K74" s="185"/>
+      <c r="L74" s="186"/>
+      <c r="M74" s="186"/>
+      <c r="N74" s="187"/>
       <c r="O74" s="82"/>
       <c r="P74" s="82"/>
       <c r="Q74" s="75"/>
@@ -11376,10 +11378,10 @@
       <c r="H75" s="62"/>
       <c r="I75" s="62"/>
       <c r="J75" s="40"/>
-      <c r="K75" s="184"/>
-      <c r="L75" s="185"/>
-      <c r="M75" s="185"/>
-      <c r="N75" s="186"/>
+      <c r="K75" s="185"/>
+      <c r="L75" s="186"/>
+      <c r="M75" s="186"/>
+      <c r="N75" s="187"/>
       <c r="O75" s="82"/>
       <c r="P75" s="82"/>
       <c r="Q75" s="75"/>
@@ -11399,10 +11401,10 @@
       <c r="H76" s="62"/>
       <c r="I76" s="62"/>
       <c r="J76" s="40"/>
-      <c r="K76" s="184"/>
-      <c r="L76" s="185"/>
-      <c r="M76" s="185"/>
-      <c r="N76" s="186"/>
+      <c r="K76" s="185"/>
+      <c r="L76" s="186"/>
+      <c r="M76" s="186"/>
+      <c r="N76" s="187"/>
       <c r="O76" s="82"/>
       <c r="P76" s="82"/>
       <c r="Q76" s="75"/>
@@ -11422,10 +11424,10 @@
       <c r="H77" s="62"/>
       <c r="I77" s="62"/>
       <c r="J77" s="40"/>
-      <c r="K77" s="184"/>
-      <c r="L77" s="185"/>
-      <c r="M77" s="185"/>
-      <c r="N77" s="186"/>
+      <c r="K77" s="185"/>
+      <c r="L77" s="186"/>
+      <c r="M77" s="186"/>
+      <c r="N77" s="187"/>
       <c r="O77" s="82"/>
       <c r="P77" s="82"/>
       <c r="Q77" s="75"/>
@@ -11445,10 +11447,10 @@
       <c r="H78" s="62"/>
       <c r="I78" s="62"/>
       <c r="J78" s="40"/>
-      <c r="K78" s="184"/>
-      <c r="L78" s="185"/>
-      <c r="M78" s="185"/>
-      <c r="N78" s="186"/>
+      <c r="K78" s="185"/>
+      <c r="L78" s="186"/>
+      <c r="M78" s="186"/>
+      <c r="N78" s="187"/>
       <c r="O78" s="82"/>
       <c r="P78" s="82"/>
       <c r="Q78" s="75"/>
@@ -11468,10 +11470,10 @@
       <c r="H79" s="62"/>
       <c r="I79" s="62"/>
       <c r="J79" s="40"/>
-      <c r="K79" s="184"/>
-      <c r="L79" s="185"/>
-      <c r="M79" s="185"/>
-      <c r="N79" s="186"/>
+      <c r="K79" s="185"/>
+      <c r="L79" s="186"/>
+      <c r="M79" s="186"/>
+      <c r="N79" s="187"/>
       <c r="O79" s="82"/>
       <c r="P79" s="82"/>
       <c r="Q79" s="75"/>
@@ -11491,10 +11493,10 @@
       <c r="H80" s="62"/>
       <c r="I80" s="62"/>
       <c r="J80" s="40"/>
-      <c r="K80" s="184"/>
-      <c r="L80" s="185"/>
-      <c r="M80" s="185"/>
-      <c r="N80" s="186"/>
+      <c r="K80" s="185"/>
+      <c r="L80" s="186"/>
+      <c r="M80" s="186"/>
+      <c r="N80" s="187"/>
       <c r="O80" s="82"/>
       <c r="P80" s="82"/>
       <c r="Q80" s="75"/>
@@ -11514,10 +11516,10 @@
       <c r="H81" s="62"/>
       <c r="I81" s="62"/>
       <c r="J81" s="40"/>
-      <c r="K81" s="184"/>
-      <c r="L81" s="185"/>
-      <c r="M81" s="185"/>
-      <c r="N81" s="186"/>
+      <c r="K81" s="185"/>
+      <c r="L81" s="186"/>
+      <c r="M81" s="186"/>
+      <c r="N81" s="187"/>
       <c r="O81" s="82"/>
       <c r="P81" s="82"/>
       <c r="Q81" s="75"/>
@@ -11537,10 +11539,10 @@
       <c r="H82" s="62"/>
       <c r="I82" s="62"/>
       <c r="J82" s="40"/>
-      <c r="K82" s="184"/>
-      <c r="L82" s="185"/>
-      <c r="M82" s="185"/>
-      <c r="N82" s="186"/>
+      <c r="K82" s="185"/>
+      <c r="L82" s="186"/>
+      <c r="M82" s="186"/>
+      <c r="N82" s="187"/>
       <c r="O82" s="82"/>
       <c r="P82" s="82"/>
       <c r="Q82" s="75"/>
@@ -11560,10 +11562,10 @@
       <c r="H83" s="62"/>
       <c r="I83" s="62"/>
       <c r="J83" s="40"/>
-      <c r="K83" s="184"/>
-      <c r="L83" s="185"/>
-      <c r="M83" s="185"/>
-      <c r="N83" s="186"/>
+      <c r="K83" s="185"/>
+      <c r="L83" s="186"/>
+      <c r="M83" s="186"/>
+      <c r="N83" s="187"/>
       <c r="O83" s="82"/>
       <c r="P83" s="82"/>
       <c r="Q83" s="75"/>
@@ -11583,10 +11585,10 @@
       <c r="H84" s="62"/>
       <c r="I84" s="62"/>
       <c r="J84" s="40"/>
-      <c r="K84" s="184"/>
-      <c r="L84" s="185"/>
-      <c r="M84" s="185"/>
-      <c r="N84" s="186"/>
+      <c r="K84" s="185"/>
+      <c r="L84" s="186"/>
+      <c r="M84" s="186"/>
+      <c r="N84" s="187"/>
       <c r="O84" s="82"/>
       <c r="P84" s="82"/>
       <c r="Q84" s="75"/>
@@ -11606,10 +11608,10 @@
       <c r="H85" s="62"/>
       <c r="I85" s="62"/>
       <c r="J85" s="40"/>
-      <c r="K85" s="184"/>
-      <c r="L85" s="185"/>
-      <c r="M85" s="185"/>
-      <c r="N85" s="186"/>
+      <c r="K85" s="185"/>
+      <c r="L85" s="186"/>
+      <c r="M85" s="186"/>
+      <c r="N85" s="187"/>
       <c r="O85" s="82"/>
       <c r="P85" s="82"/>
       <c r="Q85" s="75"/>
@@ -11629,10 +11631,10 @@
       <c r="H86" s="62"/>
       <c r="I86" s="62"/>
       <c r="J86" s="40"/>
-      <c r="K86" s="184"/>
-      <c r="L86" s="185"/>
-      <c r="M86" s="185"/>
-      <c r="N86" s="186"/>
+      <c r="K86" s="185"/>
+      <c r="L86" s="186"/>
+      <c r="M86" s="186"/>
+      <c r="N86" s="187"/>
       <c r="O86" s="82"/>
       <c r="P86" s="82"/>
       <c r="Q86" s="75"/>
@@ -11652,10 +11654,10 @@
       <c r="H87" s="62"/>
       <c r="I87" s="62"/>
       <c r="J87" s="40"/>
-      <c r="K87" s="184"/>
-      <c r="L87" s="185"/>
-      <c r="M87" s="185"/>
-      <c r="N87" s="186"/>
+      <c r="K87" s="185"/>
+      <c r="L87" s="186"/>
+      <c r="M87" s="186"/>
+      <c r="N87" s="187"/>
       <c r="O87" s="82"/>
       <c r="P87" s="82"/>
       <c r="Q87" s="75"/>
@@ -11675,10 +11677,10 @@
       <c r="H88" s="62"/>
       <c r="I88" s="62"/>
       <c r="J88" s="40"/>
-      <c r="K88" s="184"/>
-      <c r="L88" s="185"/>
-      <c r="M88" s="185"/>
-      <c r="N88" s="186"/>
+      <c r="K88" s="185"/>
+      <c r="L88" s="186"/>
+      <c r="M88" s="186"/>
+      <c r="N88" s="187"/>
       <c r="O88" s="82"/>
       <c r="P88" s="82"/>
       <c r="Q88" s="75"/>
@@ -11698,10 +11700,10 @@
       <c r="H89" s="62"/>
       <c r="I89" s="62"/>
       <c r="J89" s="40"/>
-      <c r="K89" s="184"/>
-      <c r="L89" s="185"/>
-      <c r="M89" s="185"/>
-      <c r="N89" s="186"/>
+      <c r="K89" s="185"/>
+      <c r="L89" s="186"/>
+      <c r="M89" s="186"/>
+      <c r="N89" s="187"/>
       <c r="O89" s="82"/>
       <c r="P89" s="82"/>
       <c r="Q89" s="75"/>
@@ -11721,10 +11723,10 @@
       <c r="H90" s="62"/>
       <c r="I90" s="62"/>
       <c r="J90" s="40"/>
-      <c r="K90" s="184"/>
-      <c r="L90" s="185"/>
-      <c r="M90" s="185"/>
-      <c r="N90" s="186"/>
+      <c r="K90" s="185"/>
+      <c r="L90" s="186"/>
+      <c r="M90" s="186"/>
+      <c r="N90" s="187"/>
       <c r="O90" s="82"/>
       <c r="P90" s="82"/>
       <c r="Q90" s="75"/>
@@ -11744,10 +11746,10 @@
       <c r="H91" s="62"/>
       <c r="I91" s="62"/>
       <c r="J91" s="40"/>
-      <c r="K91" s="184"/>
-      <c r="L91" s="185"/>
-      <c r="M91" s="185"/>
-      <c r="N91" s="186"/>
+      <c r="K91" s="185"/>
+      <c r="L91" s="186"/>
+      <c r="M91" s="186"/>
+      <c r="N91" s="187"/>
       <c r="O91" s="82"/>
       <c r="P91" s="82"/>
       <c r="Q91" s="75"/>
@@ -11767,10 +11769,10 @@
       <c r="H92" s="62"/>
       <c r="I92" s="62"/>
       <c r="J92" s="40"/>
-      <c r="K92" s="184"/>
-      <c r="L92" s="185"/>
-      <c r="M92" s="185"/>
-      <c r="N92" s="186"/>
+      <c r="K92" s="185"/>
+      <c r="L92" s="186"/>
+      <c r="M92" s="186"/>
+      <c r="N92" s="187"/>
       <c r="O92" s="82"/>
       <c r="P92" s="82"/>
       <c r="Q92" s="75"/>
@@ -11790,10 +11792,10 @@
       <c r="H93" s="62"/>
       <c r="I93" s="62"/>
       <c r="J93" s="40"/>
-      <c r="K93" s="184"/>
-      <c r="L93" s="185"/>
-      <c r="M93" s="185"/>
-      <c r="N93" s="186"/>
+      <c r="K93" s="185"/>
+      <c r="L93" s="186"/>
+      <c r="M93" s="186"/>
+      <c r="N93" s="187"/>
       <c r="O93" s="82"/>
       <c r="P93" s="82"/>
       <c r="Q93" s="75"/>
@@ -11813,10 +11815,10 @@
       <c r="H94" s="62"/>
       <c r="I94" s="62"/>
       <c r="J94" s="40"/>
-      <c r="K94" s="184"/>
-      <c r="L94" s="185"/>
-      <c r="M94" s="185"/>
-      <c r="N94" s="186"/>
+      <c r="K94" s="185"/>
+      <c r="L94" s="186"/>
+      <c r="M94" s="186"/>
+      <c r="N94" s="187"/>
       <c r="O94" s="82"/>
       <c r="P94" s="82"/>
       <c r="Q94" s="75"/>
@@ -11836,10 +11838,10 @@
       <c r="H95" s="62"/>
       <c r="I95" s="62"/>
       <c r="J95" s="40"/>
-      <c r="K95" s="184"/>
-      <c r="L95" s="185"/>
-      <c r="M95" s="185"/>
-      <c r="N95" s="186"/>
+      <c r="K95" s="185"/>
+      <c r="L95" s="186"/>
+      <c r="M95" s="186"/>
+      <c r="N95" s="187"/>
       <c r="O95" s="82"/>
       <c r="P95" s="82"/>
       <c r="Q95" s="75"/>
@@ -11859,10 +11861,10 @@
       <c r="H96" s="62"/>
       <c r="I96" s="62"/>
       <c r="J96" s="40"/>
-      <c r="K96" s="184"/>
-      <c r="L96" s="185"/>
-      <c r="M96" s="185"/>
-      <c r="N96" s="186"/>
+      <c r="K96" s="185"/>
+      <c r="L96" s="186"/>
+      <c r="M96" s="186"/>
+      <c r="N96" s="187"/>
       <c r="O96" s="82"/>
       <c r="P96" s="82"/>
       <c r="Q96" s="75"/>
@@ -11894,8 +11896,6 @@
     <mergeCell ref="K76:N76"/>
     <mergeCell ref="K77:N77"/>
     <mergeCell ref="K78:N78"/>
-    <mergeCell ref="K54:N54"/>
-    <mergeCell ref="K55:N55"/>
     <mergeCell ref="K74:N74"/>
     <mergeCell ref="K75:N75"/>
     <mergeCell ref="K61:N61"/>
@@ -11918,42 +11918,49 @@
     <mergeCell ref="K71:N71"/>
     <mergeCell ref="K72:N72"/>
     <mergeCell ref="K73:N73"/>
-    <mergeCell ref="K40:N40"/>
-    <mergeCell ref="K41:N41"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="K45:N45"/>
+    <mergeCell ref="K46:N46"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="K48:N48"/>
     <mergeCell ref="K60:N60"/>
     <mergeCell ref="K49:N49"/>
     <mergeCell ref="K50:N50"/>
     <mergeCell ref="K51:N51"/>
     <mergeCell ref="K52:N52"/>
     <mergeCell ref="K56:N56"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="K45:N45"/>
-    <mergeCell ref="K46:N46"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="K48:N48"/>
     <mergeCell ref="K53:N53"/>
+    <mergeCell ref="K54:N54"/>
+    <mergeCell ref="K55:N55"/>
+    <mergeCell ref="K39:N39"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="K41:N41"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="K34:N34"/>
     <mergeCell ref="K35:N35"/>
     <mergeCell ref="K36:N36"/>
     <mergeCell ref="K37:N37"/>
     <mergeCell ref="K38:N38"/>
-    <mergeCell ref="K39:N39"/>
+    <mergeCell ref="K29:N29"/>
     <mergeCell ref="K30:N30"/>
     <mergeCell ref="K31:N31"/>
     <mergeCell ref="K32:N32"/>
     <mergeCell ref="K33:N33"/>
-    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="K24:N24"/>
     <mergeCell ref="K25:N25"/>
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="K27:N27"/>
     <mergeCell ref="K28:N28"/>
-    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="K8:N8"/>
     <mergeCell ref="K20:N20"/>
     <mergeCell ref="K21:N21"/>
     <mergeCell ref="K22:N22"/>
     <mergeCell ref="K23:N23"/>
-    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K18:N18"/>
     <mergeCell ref="K19:N19"/>
     <mergeCell ref="K14:N14"/>
     <mergeCell ref="K15:N15"/>
@@ -11966,11 +11973,6 @@
     <mergeCell ref="K12:N12"/>
     <mergeCell ref="K13:N13"/>
     <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="K18:N18"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="Q1048469:Q1048576 Q5:Q96"/>
@@ -11999,8 +12001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12017,10 +12019,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
+      <c r="B1" s="146"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -12051,8 +12053,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -12111,7 +12113,7 @@
     <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="42"/>
       <c r="B6" s="43" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C6" s="43"/>
       <c r="D6" s="43"/>
@@ -12216,7 +12218,7 @@
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="43" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="43"/>
@@ -12253,7 +12255,7 @@
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="43" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C18" s="43"/>
       <c r="D18" s="43"/>
@@ -12328,7 +12330,7 @@
     <row r="24" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="72"/>
       <c r="B24" s="43" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C24" s="43"/>
       <c r="D24" s="43"/>
@@ -12355,28 +12357,28 @@
     </row>
     <row r="26" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="42"/>
-      <c r="B26" s="188" t="s">
-        <v>301</v>
-      </c>
-      <c r="C26" s="188"/>
-      <c r="D26" s="188"/>
-      <c r="E26" s="188"/>
-      <c r="F26" s="188"/>
-      <c r="G26" s="188"/>
+      <c r="B26" s="189" t="s">
+        <v>303</v>
+      </c>
+      <c r="C26" s="189"/>
+      <c r="D26" s="189"/>
+      <c r="E26" s="189"/>
+      <c r="F26" s="189"/>
+      <c r="G26" s="189"/>
       <c r="H26" s="43"/>
       <c r="I26" s="43"/>
       <c r="J26" s="46"/>
     </row>
     <row r="27" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="42"/>
-      <c r="B27" s="189" t="s">
-        <v>298</v>
-      </c>
-      <c r="C27" s="189"/>
-      <c r="D27" s="189"/>
-      <c r="E27" s="189"/>
-      <c r="F27" s="189"/>
-      <c r="G27" s="189"/>
+      <c r="B27" s="190" t="s">
+        <v>294</v>
+      </c>
+      <c r="C27" s="190"/>
+      <c r="D27" s="190"/>
+      <c r="E27" s="190"/>
+      <c r="F27" s="190"/>
+      <c r="G27" s="190"/>
       <c r="H27" s="43"/>
       <c r="I27" s="43"/>
       <c r="J27" s="46"/>
@@ -12411,7 +12413,7 @@
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="43"/>
       <c r="C30" s="84" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D30" s="43"/>
       <c r="E30" s="43"/>
@@ -12448,7 +12450,7 @@
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="79"/>
       <c r="C33" s="84" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D33" s="43"/>
       <c r="E33" s="43"/>
@@ -12500,7 +12502,7 @@
     <row r="37" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="43"/>
       <c r="C37" s="84" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D37" s="43"/>
       <c r="E37" s="43"/>
@@ -12537,7 +12539,7 @@
     <row r="40" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="79"/>
       <c r="C40" s="84" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D40" s="43"/>
       <c r="E40" s="43"/>
@@ -13129,7 +13131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -13146,10 +13148,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
+      <c r="B1" s="146"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -13177,8 +13179,8 @@
       <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -13589,14 +13591,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B1" s="190" t="s">
+      <c r="B1" s="191" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
     </row>
     <row r="2" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="16"/>
@@ -13789,11 +13791,11 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E27" s="191" t="s">
+      <c r="E27" s="192" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="192"/>
-      <c r="G27" s="193"/>
+      <c r="F27" s="193"/>
+      <c r="G27" s="194"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="19" t="s">

</xml_diff>

<commit_message>
Update dữ liệu sau khi chỉnh sửa the review
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat dia diem/CF0142_Cap nhat dia diem.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat dia diem/CF0142_Cap nhat dia diem.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Update History" sheetId="4" r:id="rId1"/>
@@ -1389,7 +1389,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="305">
   <si>
     <t>Detail Design</t>
   </si>
@@ -3387,6 +3387,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3426,9 +3429,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3496,6 +3496,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3503,12 +3509,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3938,10 +3938,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
+      <c r="B1" s="152"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -3968,8 +3968,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -4008,14 +4008,14 @@
       <c r="D4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="152" t="s">
+      <c r="E4" s="153" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
+      <c r="F4" s="153"/>
+      <c r="G4" s="153"/>
+      <c r="H4" s="153"/>
+      <c r="I4" s="153"/>
+      <c r="J4" s="153"/>
     </row>
     <row r="5" spans="1:10" s="25" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="114">
@@ -4031,14 +4031,14 @@
         <f>H1</f>
         <v>Thị Phượng</v>
       </c>
-      <c r="E5" s="153" t="s">
+      <c r="E5" s="154" t="s">
         <v>290</v>
       </c>
-      <c r="F5" s="154"/>
-      <c r="G5" s="154"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
+      <c r="F5" s="155"/>
+      <c r="G5" s="155"/>
+      <c r="H5" s="155"/>
+      <c r="I5" s="155"/>
+      <c r="J5" s="155"/>
     </row>
     <row r="6" spans="1:10" s="144" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="140">
@@ -4049,12 +4049,12 @@
       </c>
       <c r="C6" s="142"/>
       <c r="D6" s="143"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="156"/>
-      <c r="G6" s="156"/>
-      <c r="H6" s="156"/>
-      <c r="I6" s="156"/>
-      <c r="J6" s="157"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="157"/>
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="158"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="86">
@@ -4065,12 +4065,12 @@
       </c>
       <c r="C7" s="76"/>
       <c r="D7" s="40"/>
-      <c r="E7" s="145"/>
-      <c r="F7" s="146"/>
-      <c r="G7" s="146"/>
-      <c r="H7" s="146"/>
-      <c r="I7" s="146"/>
-      <c r="J7" s="147"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="147"/>
+      <c r="I7" s="147"/>
+      <c r="J7" s="148"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="87">
@@ -4081,12 +4081,12 @@
       </c>
       <c r="C8" s="76"/>
       <c r="D8" s="40"/>
-      <c r="E8" s="148"/>
-      <c r="F8" s="149"/>
-      <c r="G8" s="149"/>
-      <c r="H8" s="149"/>
-      <c r="I8" s="149"/>
-      <c r="J8" s="150"/>
+      <c r="E8" s="149"/>
+      <c r="F8" s="150"/>
+      <c r="G8" s="150"/>
+      <c r="H8" s="150"/>
+      <c r="I8" s="150"/>
+      <c r="J8" s="151"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="88">
@@ -4097,12 +4097,12 @@
       </c>
       <c r="C9" s="76"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="145"/>
-      <c r="F9" s="146"/>
-      <c r="G9" s="146"/>
-      <c r="H9" s="146"/>
-      <c r="I9" s="146"/>
-      <c r="J9" s="147"/>
+      <c r="E9" s="146"/>
+      <c r="F9" s="147"/>
+      <c r="G9" s="147"/>
+      <c r="H9" s="147"/>
+      <c r="I9" s="147"/>
+      <c r="J9" s="148"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="89">
@@ -4113,12 +4113,12 @@
       </c>
       <c r="C10" s="76"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="146"/>
-      <c r="G10" s="146"/>
-      <c r="H10" s="146"/>
-      <c r="I10" s="146"/>
-      <c r="J10" s="147"/>
+      <c r="E10" s="146"/>
+      <c r="F10" s="147"/>
+      <c r="G10" s="147"/>
+      <c r="H10" s="147"/>
+      <c r="I10" s="147"/>
+      <c r="J10" s="148"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="90">
@@ -4129,12 +4129,12 @@
       </c>
       <c r="C11" s="76"/>
       <c r="D11" s="40"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="146"/>
-      <c r="G11" s="146"/>
-      <c r="H11" s="146"/>
-      <c r="I11" s="146"/>
-      <c r="J11" s="147"/>
+      <c r="E11" s="146"/>
+      <c r="F11" s="147"/>
+      <c r="G11" s="147"/>
+      <c r="H11" s="147"/>
+      <c r="I11" s="147"/>
+      <c r="J11" s="148"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="91">
@@ -4145,12 +4145,12 @@
       </c>
       <c r="C12" s="76"/>
       <c r="D12" s="40"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="146"/>
-      <c r="G12" s="146"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="147"/>
+      <c r="E12" s="146"/>
+      <c r="F12" s="147"/>
+      <c r="G12" s="147"/>
+      <c r="H12" s="147"/>
+      <c r="I12" s="147"/>
+      <c r="J12" s="148"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="92">
@@ -4161,12 +4161,12 @@
       </c>
       <c r="C13" s="76"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="145"/>
-      <c r="F13" s="146"/>
-      <c r="G13" s="146"/>
-      <c r="H13" s="146"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="147"/>
+      <c r="E13" s="146"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="147"/>
+      <c r="H13" s="147"/>
+      <c r="I13" s="147"/>
+      <c r="J13" s="148"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="93">
@@ -4177,12 +4177,12 @@
       </c>
       <c r="C14" s="76"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="145"/>
-      <c r="F14" s="146"/>
-      <c r="G14" s="146"/>
-      <c r="H14" s="146"/>
-      <c r="I14" s="146"/>
-      <c r="J14" s="147"/>
+      <c r="E14" s="146"/>
+      <c r="F14" s="147"/>
+      <c r="G14" s="147"/>
+      <c r="H14" s="147"/>
+      <c r="I14" s="147"/>
+      <c r="J14" s="148"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="40">
@@ -4193,12 +4193,12 @@
       </c>
       <c r="C15" s="76"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
-      <c r="H15" s="158"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="158"/>
+      <c r="E15" s="145"/>
+      <c r="F15" s="145"/>
+      <c r="G15" s="145"/>
+      <c r="H15" s="145"/>
+      <c r="I15" s="145"/>
+      <c r="J15" s="145"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="85">
@@ -4209,12 +4209,12 @@
       </c>
       <c r="C16" s="76"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
+      <c r="E16" s="145"/>
+      <c r="F16" s="145"/>
+      <c r="G16" s="145"/>
+      <c r="H16" s="145"/>
+      <c r="I16" s="145"/>
+      <c r="J16" s="145"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="86">
@@ -4225,12 +4225,12 @@
       </c>
       <c r="C17" s="76"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="158"/>
-      <c r="F17" s="158"/>
-      <c r="G17" s="158"/>
-      <c r="H17" s="158"/>
-      <c r="I17" s="158"/>
-      <c r="J17" s="158"/>
+      <c r="E17" s="145"/>
+      <c r="F17" s="145"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="145"/>
+      <c r="I17" s="145"/>
+      <c r="J17" s="145"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="87">
@@ -4241,12 +4241,12 @@
       </c>
       <c r="C18" s="76"/>
       <c r="D18" s="40"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="158"/>
-      <c r="G18" s="158"/>
-      <c r="H18" s="158"/>
-      <c r="I18" s="158"/>
-      <c r="J18" s="158"/>
+      <c r="E18" s="145"/>
+      <c r="F18" s="145"/>
+      <c r="G18" s="145"/>
+      <c r="H18" s="145"/>
+      <c r="I18" s="145"/>
+      <c r="J18" s="145"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="88">
@@ -4257,12 +4257,12 @@
       </c>
       <c r="C19" s="76"/>
       <c r="D19" s="40"/>
-      <c r="E19" s="158"/>
-      <c r="F19" s="158"/>
-      <c r="G19" s="158"/>
-      <c r="H19" s="158"/>
-      <c r="I19" s="158"/>
-      <c r="J19" s="158"/>
+      <c r="E19" s="145"/>
+      <c r="F19" s="145"/>
+      <c r="G19" s="145"/>
+      <c r="H19" s="145"/>
+      <c r="I19" s="145"/>
+      <c r="J19" s="145"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="89">
@@ -4273,12 +4273,12 @@
       </c>
       <c r="C20" s="76"/>
       <c r="D20" s="40"/>
-      <c r="E20" s="158"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158"/>
-      <c r="J20" s="158"/>
+      <c r="E20" s="145"/>
+      <c r="F20" s="145"/>
+      <c r="G20" s="145"/>
+      <c r="H20" s="145"/>
+      <c r="I20" s="145"/>
+      <c r="J20" s="145"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="90">
@@ -4289,12 +4289,12 @@
       </c>
       <c r="C21" s="76"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="158"/>
-      <c r="F21" s="158"/>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158"/>
-      <c r="J21" s="158"/>
+      <c r="E21" s="145"/>
+      <c r="F21" s="145"/>
+      <c r="G21" s="145"/>
+      <c r="H21" s="145"/>
+      <c r="I21" s="145"/>
+      <c r="J21" s="145"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="91">
@@ -4305,12 +4305,12 @@
       </c>
       <c r="C22" s="76"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158"/>
-      <c r="J22" s="158"/>
+      <c r="E22" s="145"/>
+      <c r="F22" s="145"/>
+      <c r="G22" s="145"/>
+      <c r="H22" s="145"/>
+      <c r="I22" s="145"/>
+      <c r="J22" s="145"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="92">
@@ -4321,12 +4321,12 @@
       </c>
       <c r="C23" s="76"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="158"/>
-      <c r="F23" s="158"/>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="158"/>
-      <c r="J23" s="158"/>
+      <c r="E23" s="145"/>
+      <c r="F23" s="145"/>
+      <c r="G23" s="145"/>
+      <c r="H23" s="145"/>
+      <c r="I23" s="145"/>
+      <c r="J23" s="145"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="93">
@@ -4337,12 +4337,12 @@
       </c>
       <c r="C24" s="76"/>
       <c r="D24" s="40"/>
-      <c r="E24" s="158"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="158"/>
-      <c r="H24" s="158"/>
-      <c r="I24" s="158"/>
-      <c r="J24" s="158"/>
+      <c r="E24" s="145"/>
+      <c r="F24" s="145"/>
+      <c r="G24" s="145"/>
+      <c r="H24" s="145"/>
+      <c r="I24" s="145"/>
+      <c r="J24" s="145"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="40">
@@ -4353,12 +4353,12 @@
       </c>
       <c r="C25" s="76"/>
       <c r="D25" s="40"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158"/>
-      <c r="H25" s="158"/>
-      <c r="I25" s="158"/>
-      <c r="J25" s="158"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
+      <c r="H25" s="145"/>
+      <c r="I25" s="145"/>
+      <c r="J25" s="145"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="85">
@@ -4369,12 +4369,12 @@
       </c>
       <c r="C26" s="76"/>
       <c r="D26" s="40"/>
-      <c r="E26" s="158"/>
-      <c r="F26" s="158"/>
-      <c r="G26" s="158"/>
-      <c r="H26" s="158"/>
-      <c r="I26" s="158"/>
-      <c r="J26" s="158"/>
+      <c r="E26" s="145"/>
+      <c r="F26" s="145"/>
+      <c r="G26" s="145"/>
+      <c r="H26" s="145"/>
+      <c r="I26" s="145"/>
+      <c r="J26" s="145"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="86">
@@ -4385,12 +4385,12 @@
       </c>
       <c r="C27" s="76"/>
       <c r="D27" s="40"/>
-      <c r="E27" s="158"/>
-      <c r="F27" s="158"/>
-      <c r="G27" s="158"/>
-      <c r="H27" s="158"/>
-      <c r="I27" s="158"/>
-      <c r="J27" s="158"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
+      <c r="H27" s="145"/>
+      <c r="I27" s="145"/>
+      <c r="J27" s="145"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="87">
@@ -4401,12 +4401,12 @@
       </c>
       <c r="C28" s="76"/>
       <c r="D28" s="40"/>
-      <c r="E28" s="158"/>
-      <c r="F28" s="158"/>
-      <c r="G28" s="158"/>
-      <c r="H28" s="158"/>
-      <c r="I28" s="158"/>
-      <c r="J28" s="158"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="145"/>
+      <c r="H28" s="145"/>
+      <c r="I28" s="145"/>
+      <c r="J28" s="145"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="88">
@@ -4417,12 +4417,12 @@
       </c>
       <c r="C29" s="76"/>
       <c r="D29" s="40"/>
-      <c r="E29" s="158"/>
-      <c r="F29" s="158"/>
-      <c r="G29" s="158"/>
-      <c r="H29" s="158"/>
-      <c r="I29" s="158"/>
-      <c r="J29" s="158"/>
+      <c r="E29" s="145"/>
+      <c r="F29" s="145"/>
+      <c r="G29" s="145"/>
+      <c r="H29" s="145"/>
+      <c r="I29" s="145"/>
+      <c r="J29" s="145"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="89">
@@ -4433,12 +4433,12 @@
       </c>
       <c r="C30" s="76"/>
       <c r="D30" s="40"/>
-      <c r="E30" s="158"/>
-      <c r="F30" s="158"/>
-      <c r="G30" s="158"/>
-      <c r="H30" s="158"/>
-      <c r="I30" s="158"/>
-      <c r="J30" s="158"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
+      <c r="H30" s="145"/>
+      <c r="I30" s="145"/>
+      <c r="J30" s="145"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="90">
@@ -4449,12 +4449,12 @@
       </c>
       <c r="C31" s="76"/>
       <c r="D31" s="40"/>
-      <c r="E31" s="158"/>
-      <c r="F31" s="158"/>
-      <c r="G31" s="158"/>
-      <c r="H31" s="158"/>
-      <c r="I31" s="158"/>
-      <c r="J31" s="158"/>
+      <c r="E31" s="145"/>
+      <c r="F31" s="145"/>
+      <c r="G31" s="145"/>
+      <c r="H31" s="145"/>
+      <c r="I31" s="145"/>
+      <c r="J31" s="145"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="91">
@@ -4465,12 +4465,12 @@
       </c>
       <c r="C32" s="76"/>
       <c r="D32" s="40"/>
-      <c r="E32" s="158"/>
-      <c r="F32" s="158"/>
-      <c r="G32" s="158"/>
-      <c r="H32" s="158"/>
-      <c r="I32" s="158"/>
-      <c r="J32" s="158"/>
+      <c r="E32" s="145"/>
+      <c r="F32" s="145"/>
+      <c r="G32" s="145"/>
+      <c r="H32" s="145"/>
+      <c r="I32" s="145"/>
+      <c r="J32" s="145"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="92">
@@ -4481,12 +4481,12 @@
       </c>
       <c r="C33" s="76"/>
       <c r="D33" s="40"/>
-      <c r="E33" s="158"/>
-      <c r="F33" s="158"/>
-      <c r="G33" s="158"/>
-      <c r="H33" s="158"/>
-      <c r="I33" s="158"/>
-      <c r="J33" s="158"/>
+      <c r="E33" s="145"/>
+      <c r="F33" s="145"/>
+      <c r="G33" s="145"/>
+      <c r="H33" s="145"/>
+      <c r="I33" s="145"/>
+      <c r="J33" s="145"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="93">
@@ -4497,12 +4497,12 @@
       </c>
       <c r="C34" s="76"/>
       <c r="D34" s="40"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="158"/>
-      <c r="H34" s="158"/>
-      <c r="I34" s="158"/>
-      <c r="J34" s="158"/>
+      <c r="E34" s="145"/>
+      <c r="F34" s="145"/>
+      <c r="G34" s="145"/>
+      <c r="H34" s="145"/>
+      <c r="I34" s="145"/>
+      <c r="J34" s="145"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="40">
@@ -4513,12 +4513,12 @@
       </c>
       <c r="C35" s="76"/>
       <c r="D35" s="40"/>
-      <c r="E35" s="158"/>
-      <c r="F35" s="158"/>
-      <c r="G35" s="158"/>
-      <c r="H35" s="158"/>
-      <c r="I35" s="158"/>
-      <c r="J35" s="158"/>
+      <c r="E35" s="145"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="145"/>
+      <c r="H35" s="145"/>
+      <c r="I35" s="145"/>
+      <c r="J35" s="145"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="85">
@@ -4529,12 +4529,12 @@
       </c>
       <c r="C36" s="76"/>
       <c r="D36" s="40"/>
-      <c r="E36" s="158"/>
-      <c r="F36" s="158"/>
-      <c r="G36" s="158"/>
-      <c r="H36" s="158"/>
-      <c r="I36" s="158"/>
-      <c r="J36" s="158"/>
+      <c r="E36" s="145"/>
+      <c r="F36" s="145"/>
+      <c r="G36" s="145"/>
+      <c r="H36" s="145"/>
+      <c r="I36" s="145"/>
+      <c r="J36" s="145"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="86">
@@ -4545,12 +4545,12 @@
       </c>
       <c r="C37" s="76"/>
       <c r="D37" s="40"/>
-      <c r="E37" s="158"/>
-      <c r="F37" s="158"/>
-      <c r="G37" s="158"/>
-      <c r="H37" s="158"/>
-      <c r="I37" s="158"/>
-      <c r="J37" s="158"/>
+      <c r="E37" s="145"/>
+      <c r="F37" s="145"/>
+      <c r="G37" s="145"/>
+      <c r="H37" s="145"/>
+      <c r="I37" s="145"/>
+      <c r="J37" s="145"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="87">
@@ -4561,12 +4561,12 @@
       </c>
       <c r="C38" s="76"/>
       <c r="D38" s="40"/>
-      <c r="E38" s="158"/>
-      <c r="F38" s="158"/>
-      <c r="G38" s="158"/>
-      <c r="H38" s="158"/>
-      <c r="I38" s="158"/>
-      <c r="J38" s="158"/>
+      <c r="E38" s="145"/>
+      <c r="F38" s="145"/>
+      <c r="G38" s="145"/>
+      <c r="H38" s="145"/>
+      <c r="I38" s="145"/>
+      <c r="J38" s="145"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="88">
@@ -4577,12 +4577,12 @@
       </c>
       <c r="C39" s="76"/>
       <c r="D39" s="40"/>
-      <c r="E39" s="158"/>
-      <c r="F39" s="158"/>
-      <c r="G39" s="158"/>
-      <c r="H39" s="158"/>
-      <c r="I39" s="158"/>
-      <c r="J39" s="158"/>
+      <c r="E39" s="145"/>
+      <c r="F39" s="145"/>
+      <c r="G39" s="145"/>
+      <c r="H39" s="145"/>
+      <c r="I39" s="145"/>
+      <c r="J39" s="145"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="89">
@@ -4593,12 +4593,12 @@
       </c>
       <c r="C40" s="76"/>
       <c r="D40" s="40"/>
-      <c r="E40" s="158"/>
-      <c r="F40" s="158"/>
-      <c r="G40" s="158"/>
-      <c r="H40" s="158"/>
-      <c r="I40" s="158"/>
-      <c r="J40" s="158"/>
+      <c r="E40" s="145"/>
+      <c r="F40" s="145"/>
+      <c r="G40" s="145"/>
+      <c r="H40" s="145"/>
+      <c r="I40" s="145"/>
+      <c r="J40" s="145"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="90">
@@ -4609,12 +4609,12 @@
       </c>
       <c r="C41" s="76"/>
       <c r="D41" s="40"/>
-      <c r="E41" s="158"/>
-      <c r="F41" s="158"/>
-      <c r="G41" s="158"/>
-      <c r="H41" s="158"/>
-      <c r="I41" s="158"/>
-      <c r="J41" s="158"/>
+      <c r="E41" s="145"/>
+      <c r="F41" s="145"/>
+      <c r="G41" s="145"/>
+      <c r="H41" s="145"/>
+      <c r="I41" s="145"/>
+      <c r="J41" s="145"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="91">
@@ -4625,32 +4625,23 @@
       </c>
       <c r="C42" s="76"/>
       <c r="D42" s="40"/>
-      <c r="E42" s="158"/>
-      <c r="F42" s="158"/>
-      <c r="G42" s="158"/>
-      <c r="H42" s="158"/>
-      <c r="I42" s="158"/>
-      <c r="J42" s="158"/>
+      <c r="E42" s="145"/>
+      <c r="F42" s="145"/>
+      <c r="G42" s="145"/>
+      <c r="H42" s="145"/>
+      <c r="I42" s="145"/>
+      <c r="J42" s="145"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E25:J25"/>
@@ -4666,14 +4657,23 @@
     <mergeCell ref="E22:J22"/>
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -4888,10 +4888,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
+      <c r="B1" s="152"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -4921,8 +4921,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -5498,13 +5498,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
       <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
@@ -5538,11 +5538,11 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
       <c r="F2" s="30" t="s">
         <v>2</v>
       </c>
@@ -6935,7 +6935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="G13" sqref="G12:G13"/>
     </sheetView>
   </sheetViews>
@@ -7994,8 +7994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8110,15 +8110,15 @@
       <c r="F4" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="151" t="s">
+      <c r="G4" s="152" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="151"/>
-      <c r="I4" s="151" t="s">
+      <c r="H4" s="152"/>
+      <c r="I4" s="152" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="151"/>
-      <c r="K4" s="151"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="152"/>
     </row>
     <row r="5" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
@@ -8132,18 +8132,16 @@
       <c r="E5" s="137" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="G5" s="184" t="s">
+      <c r="F5" s="32"/>
+      <c r="G5" s="181" t="s">
         <v>243</v>
       </c>
-      <c r="H5" s="185"/>
-      <c r="I5" s="181" t="s">
+      <c r="H5" s="182"/>
+      <c r="I5" s="183" t="s">
         <v>298</v>
       </c>
-      <c r="J5" s="182"/>
-      <c r="K5" s="183"/>
+      <c r="J5" s="184"/>
+      <c r="K5" s="185"/>
     </row>
     <row r="6" spans="1:13" s="34" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33">
@@ -8157,18 +8155,16 @@
       <c r="E6" s="138" t="s">
         <v>242</v>
       </c>
-      <c r="F6" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="G6" s="184" t="s">
+      <c r="F6" s="32"/>
+      <c r="G6" s="181" t="s">
         <v>244</v>
       </c>
-      <c r="H6" s="185"/>
-      <c r="I6" s="181" t="s">
+      <c r="H6" s="182"/>
+      <c r="I6" s="183" t="s">
         <v>299</v>
       </c>
-      <c r="J6" s="182"/>
-      <c r="K6" s="183"/>
+      <c r="J6" s="184"/>
+      <c r="K6" s="185"/>
     </row>
     <row r="7" spans="1:13" s="34" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
@@ -8182,18 +8178,16 @@
       <c r="E7" s="138" t="s">
         <v>242</v>
       </c>
-      <c r="F7" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="G7" s="184" t="s">
+      <c r="F7" s="32"/>
+      <c r="G7" s="181" t="s">
         <v>244</v>
       </c>
-      <c r="H7" s="185"/>
-      <c r="I7" s="181" t="s">
+      <c r="H7" s="182"/>
+      <c r="I7" s="183" t="s">
         <v>300</v>
       </c>
-      <c r="J7" s="182"/>
-      <c r="K7" s="183"/>
+      <c r="J7" s="184"/>
+      <c r="K7" s="185"/>
     </row>
     <row r="8" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
@@ -8204,11 +8198,11 @@
       <c r="D8" s="33"/>
       <c r="E8" s="33"/>
       <c r="F8" s="32"/>
-      <c r="G8" s="184"/>
-      <c r="H8" s="185"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="182"/>
-      <c r="K8" s="183"/>
+      <c r="G8" s="181"/>
+      <c r="H8" s="182"/>
+      <c r="I8" s="183"/>
+      <c r="J8" s="184"/>
+      <c r="K8" s="185"/>
     </row>
     <row r="9" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33">
@@ -8219,11 +8213,11 @@
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
       <c r="F9" s="32"/>
-      <c r="G9" s="184"/>
-      <c r="H9" s="185"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="182"/>
-      <c r="K9" s="183"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="182"/>
+      <c r="I9" s="183"/>
+      <c r="J9" s="184"/>
+      <c r="K9" s="185"/>
     </row>
     <row r="10" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="33">
@@ -8234,11 +8228,11 @@
       <c r="D10" s="33"/>
       <c r="E10" s="33"/>
       <c r="F10" s="32"/>
-      <c r="G10" s="184"/>
-      <c r="H10" s="185"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="182"/>
-      <c r="K10" s="183"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="182"/>
+      <c r="I10" s="183"/>
+      <c r="J10" s="184"/>
+      <c r="K10" s="185"/>
     </row>
     <row r="11" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33">
@@ -8249,11 +8243,11 @@
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
       <c r="F11" s="32"/>
-      <c r="G11" s="184"/>
-      <c r="H11" s="185"/>
-      <c r="I11" s="181"/>
-      <c r="J11" s="182"/>
-      <c r="K11" s="183"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="182"/>
+      <c r="I11" s="183"/>
+      <c r="J11" s="184"/>
+      <c r="K11" s="185"/>
     </row>
     <row r="12" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="33">
@@ -8264,11 +8258,11 @@
       <c r="D12" s="33"/>
       <c r="E12" s="33"/>
       <c r="F12" s="32"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="185"/>
-      <c r="I12" s="181"/>
-      <c r="J12" s="182"/>
-      <c r="K12" s="183"/>
+      <c r="G12" s="181"/>
+      <c r="H12" s="182"/>
+      <c r="I12" s="183"/>
+      <c r="J12" s="184"/>
+      <c r="K12" s="185"/>
     </row>
     <row r="13" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33">
@@ -8279,11 +8273,11 @@
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
       <c r="F13" s="32"/>
-      <c r="G13" s="184"/>
-      <c r="H13" s="185"/>
-      <c r="I13" s="181"/>
-      <c r="J13" s="182"/>
-      <c r="K13" s="183"/>
+      <c r="G13" s="181"/>
+      <c r="H13" s="182"/>
+      <c r="I13" s="183"/>
+      <c r="J13" s="184"/>
+      <c r="K13" s="185"/>
     </row>
     <row r="14" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
@@ -8294,11 +8288,11 @@
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
       <c r="F14" s="32"/>
-      <c r="G14" s="184"/>
-      <c r="H14" s="185"/>
-      <c r="I14" s="181"/>
-      <c r="J14" s="182"/>
-      <c r="K14" s="183"/>
+      <c r="G14" s="181"/>
+      <c r="H14" s="182"/>
+      <c r="I14" s="183"/>
+      <c r="J14" s="184"/>
+      <c r="K14" s="185"/>
     </row>
     <row r="15" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33">
@@ -8309,11 +8303,11 @@
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
       <c r="F15" s="32"/>
-      <c r="G15" s="184"/>
-      <c r="H15" s="185"/>
-      <c r="I15" s="181"/>
-      <c r="J15" s="182"/>
-      <c r="K15" s="183"/>
+      <c r="G15" s="181"/>
+      <c r="H15" s="182"/>
+      <c r="I15" s="183"/>
+      <c r="J15" s="184"/>
+      <c r="K15" s="185"/>
     </row>
     <row r="16" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33">
@@ -8324,11 +8318,11 @@
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
       <c r="F16" s="32"/>
-      <c r="G16" s="184"/>
-      <c r="H16" s="185"/>
-      <c r="I16" s="181"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="183"/>
+      <c r="G16" s="181"/>
+      <c r="H16" s="182"/>
+      <c r="I16" s="183"/>
+      <c r="J16" s="184"/>
+      <c r="K16" s="185"/>
     </row>
     <row r="17" spans="1:19" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A17" s="33">
@@ -8339,11 +8333,11 @@
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
       <c r="F17" s="32"/>
-      <c r="G17" s="184"/>
-      <c r="H17" s="185"/>
-      <c r="I17" s="181"/>
-      <c r="J17" s="182"/>
-      <c r="K17" s="183"/>
+      <c r="G17" s="181"/>
+      <c r="H17" s="182"/>
+      <c r="I17" s="183"/>
+      <c r="J17" s="184"/>
+      <c r="K17" s="185"/>
     </row>
     <row r="18" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33">
@@ -8354,11 +8348,11 @@
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
       <c r="F18" s="32"/>
-      <c r="G18" s="184"/>
-      <c r="H18" s="185"/>
-      <c r="I18" s="181"/>
-      <c r="J18" s="182"/>
-      <c r="K18" s="183"/>
+      <c r="G18" s="181"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="183"/>
+      <c r="J18" s="184"/>
+      <c r="K18" s="185"/>
     </row>
     <row r="19" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33">
@@ -8369,11 +8363,11 @@
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
       <c r="F19" s="32"/>
-      <c r="G19" s="184"/>
-      <c r="H19" s="185"/>
-      <c r="I19" s="181"/>
-      <c r="J19" s="182"/>
-      <c r="K19" s="183"/>
+      <c r="G19" s="181"/>
+      <c r="H19" s="182"/>
+      <c r="I19" s="183"/>
+      <c r="J19" s="184"/>
+      <c r="K19" s="185"/>
     </row>
     <row r="20" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="33">
@@ -8384,11 +8378,11 @@
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
       <c r="F20" s="32"/>
-      <c r="G20" s="184"/>
-      <c r="H20" s="185"/>
-      <c r="I20" s="181"/>
-      <c r="J20" s="182"/>
-      <c r="K20" s="183"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="183"/>
+      <c r="J20" s="184"/>
+      <c r="K20" s="185"/>
     </row>
     <row r="21" spans="1:19" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A21" s="33">
@@ -8399,11 +8393,11 @@
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
       <c r="F21" s="32"/>
-      <c r="G21" s="184"/>
-      <c r="H21" s="185"/>
-      <c r="I21" s="181"/>
-      <c r="J21" s="182"/>
-      <c r="K21" s="183"/>
+      <c r="G21" s="181"/>
+      <c r="H21" s="182"/>
+      <c r="I21" s="183"/>
+      <c r="J21" s="184"/>
+      <c r="K21" s="185"/>
     </row>
     <row r="22" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="33">
@@ -8414,11 +8408,11 @@
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
       <c r="F22" s="32"/>
-      <c r="G22" s="145"/>
-      <c r="H22" s="147"/>
-      <c r="I22" s="181"/>
-      <c r="J22" s="182"/>
-      <c r="K22" s="183"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="148"/>
+      <c r="I22" s="183"/>
+      <c r="J22" s="184"/>
+      <c r="K22" s="185"/>
     </row>
     <row r="23" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="33">
@@ -8429,11 +8423,11 @@
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
       <c r="F23" s="32"/>
-      <c r="G23" s="145"/>
-      <c r="H23" s="147"/>
-      <c r="I23" s="181"/>
-      <c r="J23" s="182"/>
-      <c r="K23" s="183"/>
+      <c r="G23" s="146"/>
+      <c r="H23" s="148"/>
+      <c r="I23" s="183"/>
+      <c r="J23" s="184"/>
+      <c r="K23" s="185"/>
     </row>
     <row r="24" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="33">
@@ -8444,11 +8438,11 @@
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="32"/>
-      <c r="G24" s="145"/>
-      <c r="H24" s="147"/>
-      <c r="I24" s="181"/>
-      <c r="J24" s="182"/>
-      <c r="K24" s="183"/>
+      <c r="G24" s="146"/>
+      <c r="H24" s="148"/>
+      <c r="I24" s="183"/>
+      <c r="J24" s="184"/>
+      <c r="K24" s="185"/>
     </row>
     <row r="25" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="33">
@@ -8459,11 +8453,11 @@
       <c r="D25" s="33"/>
       <c r="E25" s="33"/>
       <c r="F25" s="32"/>
-      <c r="G25" s="145"/>
-      <c r="H25" s="147"/>
-      <c r="I25" s="181"/>
-      <c r="J25" s="182"/>
-      <c r="K25" s="183"/>
+      <c r="G25" s="146"/>
+      <c r="H25" s="148"/>
+      <c r="I25" s="183"/>
+      <c r="J25" s="184"/>
+      <c r="K25" s="185"/>
     </row>
     <row r="26" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33">
@@ -8474,11 +8468,11 @@
       <c r="D26" s="33"/>
       <c r="E26" s="33"/>
       <c r="F26" s="32"/>
-      <c r="G26" s="145"/>
-      <c r="H26" s="147"/>
-      <c r="I26" s="181"/>
-      <c r="J26" s="182"/>
-      <c r="K26" s="183"/>
+      <c r="G26" s="146"/>
+      <c r="H26" s="148"/>
+      <c r="I26" s="183"/>
+      <c r="J26" s="184"/>
+      <c r="K26" s="185"/>
     </row>
     <row r="27" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33">
@@ -8489,11 +8483,11 @@
       <c r="D27" s="33"/>
       <c r="E27" s="33"/>
       <c r="F27" s="32"/>
-      <c r="G27" s="145"/>
-      <c r="H27" s="147"/>
-      <c r="I27" s="181"/>
-      <c r="J27" s="182"/>
-      <c r="K27" s="183"/>
+      <c r="G27" s="146"/>
+      <c r="H27" s="148"/>
+      <c r="I27" s="183"/>
+      <c r="J27" s="184"/>
+      <c r="K27" s="185"/>
     </row>
     <row r="28" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="33">
@@ -8504,11 +8498,11 @@
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
       <c r="F28" s="32"/>
-      <c r="G28" s="145"/>
-      <c r="H28" s="147"/>
-      <c r="I28" s="181"/>
-      <c r="J28" s="182"/>
-      <c r="K28" s="183"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="148"/>
+      <c r="I28" s="183"/>
+      <c r="J28" s="184"/>
+      <c r="K28" s="185"/>
     </row>
     <row r="29" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="33">
@@ -8519,11 +8513,11 @@
       <c r="D29" s="33"/>
       <c r="E29" s="33"/>
       <c r="F29" s="32"/>
-      <c r="G29" s="145"/>
-      <c r="H29" s="147"/>
-      <c r="I29" s="181"/>
-      <c r="J29" s="182"/>
-      <c r="K29" s="183"/>
+      <c r="G29" s="146"/>
+      <c r="H29" s="148"/>
+      <c r="I29" s="183"/>
+      <c r="J29" s="184"/>
+      <c r="K29" s="185"/>
     </row>
     <row r="30" spans="1:19" s="34" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="33">
@@ -8534,11 +8528,11 @@
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="32"/>
-      <c r="G30" s="145"/>
-      <c r="H30" s="147"/>
-      <c r="I30" s="181"/>
-      <c r="J30" s="182"/>
-      <c r="K30" s="183"/>
+      <c r="G30" s="146"/>
+      <c r="H30" s="148"/>
+      <c r="I30" s="183"/>
+      <c r="J30" s="184"/>
+      <c r="K30" s="185"/>
     </row>
     <row r="31" spans="1:19" s="34" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="33">
@@ -8549,11 +8543,11 @@
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
       <c r="F31" s="32"/>
-      <c r="G31" s="145"/>
-      <c r="H31" s="147"/>
-      <c r="I31" s="181"/>
-      <c r="J31" s="182"/>
-      <c r="K31" s="183"/>
+      <c r="G31" s="146"/>
+      <c r="H31" s="148"/>
+      <c r="I31" s="183"/>
+      <c r="J31" s="184"/>
+      <c r="K31" s="185"/>
     </row>
     <row r="32" spans="1:19" ht="11.25" x14ac:dyDescent="0.15">
       <c r="A32" s="33">
@@ -8564,11 +8558,11 @@
       <c r="D32" s="33"/>
       <c r="E32" s="33"/>
       <c r="F32" s="32"/>
-      <c r="G32" s="145"/>
-      <c r="H32" s="147"/>
-      <c r="I32" s="181"/>
-      <c r="J32" s="182"/>
-      <c r="K32" s="183"/>
+      <c r="G32" s="146"/>
+      <c r="H32" s="148"/>
+      <c r="I32" s="183"/>
+      <c r="J32" s="184"/>
+      <c r="K32" s="185"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
@@ -8586,11 +8580,11 @@
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
       <c r="F33" s="32"/>
-      <c r="G33" s="145"/>
-      <c r="H33" s="147"/>
-      <c r="I33" s="181"/>
-      <c r="J33" s="182"/>
-      <c r="K33" s="183"/>
+      <c r="G33" s="146"/>
+      <c r="H33" s="148"/>
+      <c r="I33" s="183"/>
+      <c r="J33" s="184"/>
+      <c r="K33" s="185"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
       <c r="O33" s="22"/>
@@ -8608,11 +8602,11 @@
       <c r="D34" s="33"/>
       <c r="E34" s="33"/>
       <c r="F34" s="32"/>
-      <c r="G34" s="145"/>
-      <c r="H34" s="147"/>
-      <c r="I34" s="181"/>
-      <c r="J34" s="182"/>
-      <c r="K34" s="183"/>
+      <c r="G34" s="146"/>
+      <c r="H34" s="148"/>
+      <c r="I34" s="183"/>
+      <c r="J34" s="184"/>
+      <c r="K34" s="185"/>
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
       <c r="O34" s="22"/>
@@ -8630,11 +8624,11 @@
       <c r="D35" s="33"/>
       <c r="E35" s="33"/>
       <c r="F35" s="32"/>
-      <c r="G35" s="145"/>
-      <c r="H35" s="147"/>
-      <c r="I35" s="181"/>
-      <c r="J35" s="182"/>
-      <c r="K35" s="183"/>
+      <c r="G35" s="146"/>
+      <c r="H35" s="148"/>
+      <c r="I35" s="183"/>
+      <c r="J35" s="184"/>
+      <c r="K35" s="185"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="22"/>
@@ -8652,11 +8646,11 @@
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
       <c r="F36" s="32"/>
-      <c r="G36" s="145"/>
-      <c r="H36" s="147"/>
-      <c r="I36" s="181"/>
-      <c r="J36" s="182"/>
-      <c r="K36" s="183"/>
+      <c r="G36" s="146"/>
+      <c r="H36" s="148"/>
+      <c r="I36" s="183"/>
+      <c r="J36" s="184"/>
+      <c r="K36" s="185"/>
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
       <c r="O36" s="22"/>
@@ -8674,11 +8668,11 @@
       <c r="D37" s="33"/>
       <c r="E37" s="33"/>
       <c r="F37" s="32"/>
-      <c r="G37" s="145"/>
-      <c r="H37" s="147"/>
-      <c r="I37" s="181"/>
-      <c r="J37" s="182"/>
-      <c r="K37" s="183"/>
+      <c r="G37" s="146"/>
+      <c r="H37" s="148"/>
+      <c r="I37" s="183"/>
+      <c r="J37" s="184"/>
+      <c r="K37" s="185"/>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22"/>
@@ -8696,11 +8690,11 @@
       <c r="D38" s="33"/>
       <c r="E38" s="33"/>
       <c r="F38" s="32"/>
-      <c r="G38" s="145"/>
-      <c r="H38" s="147"/>
-      <c r="I38" s="181"/>
-      <c r="J38" s="182"/>
-      <c r="K38" s="183"/>
+      <c r="G38" s="146"/>
+      <c r="H38" s="148"/>
+      <c r="I38" s="183"/>
+      <c r="J38" s="184"/>
+      <c r="K38" s="185"/>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
       <c r="O38" s="22"/>
@@ -8718,11 +8712,11 @@
       <c r="D39" s="33"/>
       <c r="E39" s="33"/>
       <c r="F39" s="32"/>
-      <c r="G39" s="145"/>
-      <c r="H39" s="147"/>
-      <c r="I39" s="181"/>
-      <c r="J39" s="182"/>
-      <c r="K39" s="183"/>
+      <c r="G39" s="146"/>
+      <c r="H39" s="148"/>
+      <c r="I39" s="183"/>
+      <c r="J39" s="184"/>
+      <c r="K39" s="185"/>
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22"/>
@@ -8740,11 +8734,11 @@
       <c r="D40" s="33"/>
       <c r="E40" s="33"/>
       <c r="F40" s="32"/>
-      <c r="G40" s="145"/>
-      <c r="H40" s="147"/>
-      <c r="I40" s="181"/>
-      <c r="J40" s="182"/>
-      <c r="K40" s="183"/>
+      <c r="G40" s="146"/>
+      <c r="H40" s="148"/>
+      <c r="I40" s="183"/>
+      <c r="J40" s="184"/>
+      <c r="K40" s="185"/>
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
       <c r="O40" s="22"/>
@@ -8762,11 +8756,11 @@
       <c r="D41" s="33"/>
       <c r="E41" s="33"/>
       <c r="F41" s="32"/>
-      <c r="G41" s="145"/>
-      <c r="H41" s="147"/>
-      <c r="I41" s="181"/>
-      <c r="J41" s="182"/>
-      <c r="K41" s="183"/>
+      <c r="G41" s="146"/>
+      <c r="H41" s="148"/>
+      <c r="I41" s="183"/>
+      <c r="J41" s="184"/>
+      <c r="K41" s="185"/>
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22"/>
@@ -8784,11 +8778,11 @@
       <c r="D42" s="33"/>
       <c r="E42" s="33"/>
       <c r="F42" s="32"/>
-      <c r="G42" s="145"/>
-      <c r="H42" s="147"/>
-      <c r="I42" s="181"/>
-      <c r="J42" s="182"/>
-      <c r="K42" s="183"/>
+      <c r="G42" s="146"/>
+      <c r="H42" s="148"/>
+      <c r="I42" s="183"/>
+      <c r="J42" s="184"/>
+      <c r="K42" s="185"/>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
       <c r="O42" s="22"/>
@@ -8806,11 +8800,11 @@
       <c r="D43" s="33"/>
       <c r="E43" s="33"/>
       <c r="F43" s="32"/>
-      <c r="G43" s="145"/>
-      <c r="H43" s="147"/>
-      <c r="I43" s="181"/>
-      <c r="J43" s="182"/>
-      <c r="K43" s="183"/>
+      <c r="G43" s="146"/>
+      <c r="H43" s="148"/>
+      <c r="I43" s="183"/>
+      <c r="J43" s="184"/>
+      <c r="K43" s="185"/>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
       <c r="O43" s="22"/>
@@ -8828,11 +8822,11 @@
       <c r="D44" s="33"/>
       <c r="E44" s="33"/>
       <c r="F44" s="32"/>
-      <c r="G44" s="145"/>
-      <c r="H44" s="147"/>
-      <c r="I44" s="181"/>
-      <c r="J44" s="182"/>
-      <c r="K44" s="183"/>
+      <c r="G44" s="146"/>
+      <c r="H44" s="148"/>
+      <c r="I44" s="183"/>
+      <c r="J44" s="184"/>
+      <c r="K44" s="185"/>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
       <c r="O44" s="22"/>
@@ -8850,11 +8844,11 @@
       <c r="D45" s="33"/>
       <c r="E45" s="33"/>
       <c r="F45" s="32"/>
-      <c r="G45" s="145"/>
-      <c r="H45" s="147"/>
-      <c r="I45" s="181"/>
-      <c r="J45" s="182"/>
-      <c r="K45" s="183"/>
+      <c r="G45" s="146"/>
+      <c r="H45" s="148"/>
+      <c r="I45" s="183"/>
+      <c r="J45" s="184"/>
+      <c r="K45" s="185"/>
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
       <c r="O45" s="22"/>
@@ -8872,11 +8866,11 @@
       <c r="D46" s="33"/>
       <c r="E46" s="33"/>
       <c r="F46" s="32"/>
-      <c r="G46" s="145"/>
-      <c r="H46" s="147"/>
-      <c r="I46" s="181"/>
-      <c r="J46" s="182"/>
-      <c r="K46" s="183"/>
+      <c r="G46" s="146"/>
+      <c r="H46" s="148"/>
+      <c r="I46" s="183"/>
+      <c r="J46" s="184"/>
+      <c r="K46" s="185"/>
       <c r="M46" s="22"/>
       <c r="N46" s="22"/>
       <c r="O46" s="22"/>
@@ -8894,11 +8888,11 @@
       <c r="D47" s="33"/>
       <c r="E47" s="33"/>
       <c r="F47" s="32"/>
-      <c r="G47" s="145"/>
-      <c r="H47" s="147"/>
-      <c r="I47" s="181"/>
-      <c r="J47" s="182"/>
-      <c r="K47" s="183"/>
+      <c r="G47" s="146"/>
+      <c r="H47" s="148"/>
+      <c r="I47" s="183"/>
+      <c r="J47" s="184"/>
+      <c r="K47" s="185"/>
       <c r="M47" s="22"/>
       <c r="N47" s="22"/>
       <c r="O47" s="22"/>
@@ -8916,11 +8910,11 @@
       <c r="D48" s="33"/>
       <c r="E48" s="33"/>
       <c r="F48" s="32"/>
-      <c r="G48" s="145"/>
-      <c r="H48" s="147"/>
-      <c r="I48" s="181"/>
-      <c r="J48" s="182"/>
-      <c r="K48" s="183"/>
+      <c r="G48" s="146"/>
+      <c r="H48" s="148"/>
+      <c r="I48" s="183"/>
+      <c r="J48" s="184"/>
+      <c r="K48" s="185"/>
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
       <c r="O48" s="22"/>
@@ -8938,11 +8932,11 @@
       <c r="D49" s="33"/>
       <c r="E49" s="33"/>
       <c r="F49" s="32"/>
-      <c r="G49" s="145"/>
-      <c r="H49" s="147"/>
-      <c r="I49" s="181"/>
-      <c r="J49" s="182"/>
-      <c r="K49" s="183"/>
+      <c r="G49" s="146"/>
+      <c r="H49" s="148"/>
+      <c r="I49" s="183"/>
+      <c r="J49" s="184"/>
+      <c r="K49" s="185"/>
       <c r="M49" s="22"/>
       <c r="N49" s="22"/>
       <c r="O49" s="22"/>
@@ -8960,11 +8954,11 @@
       <c r="D50" s="33"/>
       <c r="E50" s="33"/>
       <c r="F50" s="32"/>
-      <c r="G50" s="145"/>
-      <c r="H50" s="147"/>
-      <c r="I50" s="181"/>
-      <c r="J50" s="182"/>
-      <c r="K50" s="183"/>
+      <c r="G50" s="146"/>
+      <c r="H50" s="148"/>
+      <c r="I50" s="183"/>
+      <c r="J50" s="184"/>
+      <c r="K50" s="185"/>
       <c r="M50" s="22"/>
       <c r="N50" s="22"/>
       <c r="O50" s="22"/>
@@ -8982,11 +8976,11 @@
       <c r="D51" s="33"/>
       <c r="E51" s="33"/>
       <c r="F51" s="32"/>
-      <c r="G51" s="145"/>
-      <c r="H51" s="147"/>
-      <c r="I51" s="181"/>
-      <c r="J51" s="182"/>
-      <c r="K51" s="183"/>
+      <c r="G51" s="146"/>
+      <c r="H51" s="148"/>
+      <c r="I51" s="183"/>
+      <c r="J51" s="184"/>
+      <c r="K51" s="185"/>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
       <c r="O51" s="22"/>
@@ -9004,11 +8998,11 @@
       <c r="D52" s="33"/>
       <c r="E52" s="33"/>
       <c r="F52" s="32"/>
-      <c r="G52" s="145"/>
-      <c r="H52" s="147"/>
-      <c r="I52" s="181"/>
-      <c r="J52" s="182"/>
-      <c r="K52" s="183"/>
+      <c r="G52" s="146"/>
+      <c r="H52" s="148"/>
+      <c r="I52" s="183"/>
+      <c r="J52" s="184"/>
+      <c r="K52" s="185"/>
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
       <c r="O52" s="22"/>
@@ -9026,11 +9020,11 @@
       <c r="D53" s="33"/>
       <c r="E53" s="33"/>
       <c r="F53" s="32"/>
-      <c r="G53" s="145"/>
-      <c r="H53" s="147"/>
-      <c r="I53" s="181"/>
-      <c r="J53" s="182"/>
-      <c r="K53" s="183"/>
+      <c r="G53" s="146"/>
+      <c r="H53" s="148"/>
+      <c r="I53" s="183"/>
+      <c r="J53" s="184"/>
+      <c r="K53" s="185"/>
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
       <c r="O53" s="22"/>
@@ -9048,11 +9042,11 @@
       <c r="D54" s="33"/>
       <c r="E54" s="33"/>
       <c r="F54" s="32"/>
-      <c r="G54" s="145"/>
-      <c r="H54" s="147"/>
-      <c r="I54" s="181"/>
-      <c r="J54" s="182"/>
-      <c r="K54" s="183"/>
+      <c r="G54" s="146"/>
+      <c r="H54" s="148"/>
+      <c r="I54" s="183"/>
+      <c r="J54" s="184"/>
+      <c r="K54" s="185"/>
       <c r="M54" s="22"/>
       <c r="N54" s="22"/>
       <c r="O54" s="22"/>
@@ -9070,11 +9064,11 @@
       <c r="D55" s="33"/>
       <c r="E55" s="33"/>
       <c r="F55" s="32"/>
-      <c r="G55" s="145"/>
-      <c r="H55" s="147"/>
-      <c r="I55" s="181"/>
-      <c r="J55" s="182"/>
-      <c r="K55" s="183"/>
+      <c r="G55" s="146"/>
+      <c r="H55" s="148"/>
+      <c r="I55" s="183"/>
+      <c r="J55" s="184"/>
+      <c r="K55" s="185"/>
       <c r="M55" s="22"/>
       <c r="N55" s="22"/>
       <c r="O55" s="22"/>
@@ -9092,11 +9086,11 @@
       <c r="D56" s="33"/>
       <c r="E56" s="33"/>
       <c r="F56" s="32"/>
-      <c r="G56" s="145"/>
-      <c r="H56" s="147"/>
-      <c r="I56" s="181"/>
-      <c r="J56" s="182"/>
-      <c r="K56" s="183"/>
+      <c r="G56" s="146"/>
+      <c r="H56" s="148"/>
+      <c r="I56" s="183"/>
+      <c r="J56" s="184"/>
+      <c r="K56" s="185"/>
       <c r="M56" s="22"/>
       <c r="N56" s="22"/>
       <c r="O56" s="22"/>
@@ -9108,25 +9102,80 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="107">
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="I53:K53"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -9141,80 +9190,25 @@
     <mergeCell ref="I17:K17"/>
     <mergeCell ref="I18:K18"/>
     <mergeCell ref="I19:K19"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I49:K49"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="I53:K53"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A1:B2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F56">
@@ -9266,16 +9260,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
+      <c r="H1" s="152"/>
       <c r="I1" s="31" t="s">
         <v>1</v>
       </c>
@@ -9311,14 +9305,14 @@
       <c r="U1" s="52"/>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
       <c r="I2" s="31" t="s">
         <v>2</v>
       </c>
@@ -9431,12 +9425,12 @@
       <c r="J5" s="115" t="s">
         <v>214</v>
       </c>
-      <c r="K5" s="148" t="s">
+      <c r="K5" s="149" t="s">
         <v>294</v>
       </c>
-      <c r="L5" s="149"/>
-      <c r="M5" s="149"/>
-      <c r="N5" s="150"/>
+      <c r="L5" s="150"/>
+      <c r="M5" s="150"/>
+      <c r="N5" s="151"/>
       <c r="O5" s="119" t="s">
         <v>292</v>
       </c>
@@ -9476,12 +9470,12 @@
       <c r="J6" s="115" t="s">
         <v>215</v>
       </c>
-      <c r="K6" s="148" t="s">
+      <c r="K6" s="149" t="s">
         <v>245</v>
       </c>
-      <c r="L6" s="149"/>
-      <c r="M6" s="149"/>
-      <c r="N6" s="150"/>
+      <c r="L6" s="150"/>
+      <c r="M6" s="150"/>
+      <c r="N6" s="151"/>
       <c r="O6" s="119" t="s">
         <v>257</v>
       </c>
@@ -9527,12 +9521,12 @@
       <c r="J7" s="115" t="s">
         <v>216</v>
       </c>
-      <c r="K7" s="148" t="s">
+      <c r="K7" s="149" t="s">
         <v>262</v>
       </c>
-      <c r="L7" s="149"/>
-      <c r="M7" s="149"/>
-      <c r="N7" s="150"/>
+      <c r="L7" s="150"/>
+      <c r="M7" s="150"/>
+      <c r="N7" s="151"/>
       <c r="O7" s="119" t="s">
         <v>263</v>
       </c>
@@ -9580,12 +9574,12 @@
       <c r="J8" s="115" t="s">
         <v>217</v>
       </c>
-      <c r="K8" s="148" t="s">
+      <c r="K8" s="149" t="s">
         <v>261</v>
       </c>
-      <c r="L8" s="149"/>
-      <c r="M8" s="149"/>
-      <c r="N8" s="150"/>
+      <c r="L8" s="150"/>
+      <c r="M8" s="150"/>
+      <c r="N8" s="151"/>
       <c r="O8" s="119" t="s">
         <v>135</v>
       </c>
@@ -9633,12 +9627,12 @@
       <c r="J9" s="115" t="s">
         <v>219</v>
       </c>
-      <c r="K9" s="148" t="s">
+      <c r="K9" s="149" t="s">
         <v>295</v>
       </c>
-      <c r="L9" s="149"/>
-      <c r="M9" s="149"/>
-      <c r="N9" s="150"/>
+      <c r="L9" s="150"/>
+      <c r="M9" s="150"/>
+      <c r="N9" s="151"/>
       <c r="O9" s="119" t="s">
         <v>256</v>
       </c>
@@ -9684,12 +9678,12 @@
       <c r="J10" s="115" t="s">
         <v>279</v>
       </c>
-      <c r="K10" s="148" t="s">
+      <c r="K10" s="149" t="s">
         <v>255</v>
       </c>
-      <c r="L10" s="149"/>
-      <c r="M10" s="149"/>
-      <c r="N10" s="150"/>
+      <c r="L10" s="150"/>
+      <c r="M10" s="150"/>
+      <c r="N10" s="151"/>
       <c r="O10" s="119" t="s">
         <v>267</v>
       </c>
@@ -11802,16 +11796,76 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="96">
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="K91:N91"/>
-    <mergeCell ref="K92:N92"/>
-    <mergeCell ref="K93:N93"/>
-    <mergeCell ref="K94:N94"/>
-    <mergeCell ref="K76:N76"/>
-    <mergeCell ref="K77:N77"/>
-    <mergeCell ref="K78:N78"/>
-    <mergeCell ref="K74:N74"/>
-    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="K31:N31"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="K33:N33"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="K36:N36"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="K38:N38"/>
+    <mergeCell ref="K39:N39"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="K41:N41"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="K45:N45"/>
+    <mergeCell ref="K46:N46"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="K48:N48"/>
+    <mergeCell ref="K60:N60"/>
+    <mergeCell ref="K49:N49"/>
+    <mergeCell ref="K50:N50"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="K52:N52"/>
+    <mergeCell ref="K56:N56"/>
+    <mergeCell ref="K53:N53"/>
+    <mergeCell ref="K54:N54"/>
+    <mergeCell ref="K55:N55"/>
+    <mergeCell ref="K96:N96"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K80:N80"/>
+    <mergeCell ref="K81:N81"/>
+    <mergeCell ref="K82:N82"/>
+    <mergeCell ref="K83:N83"/>
+    <mergeCell ref="K84:N84"/>
+    <mergeCell ref="K85:N85"/>
+    <mergeCell ref="K86:N86"/>
+    <mergeCell ref="K87:N87"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="K71:N71"/>
+    <mergeCell ref="K72:N72"/>
+    <mergeCell ref="K73:N73"/>
+    <mergeCell ref="K44:N44"/>
     <mergeCell ref="K61:N61"/>
     <mergeCell ref="K57:N57"/>
     <mergeCell ref="K58:N58"/>
@@ -11828,76 +11882,16 @@
     <mergeCell ref="K68:N68"/>
     <mergeCell ref="K69:N69"/>
     <mergeCell ref="K70:N70"/>
-    <mergeCell ref="K96:N96"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K80:N80"/>
-    <mergeCell ref="K81:N81"/>
-    <mergeCell ref="K82:N82"/>
-    <mergeCell ref="K83:N83"/>
-    <mergeCell ref="K84:N84"/>
-    <mergeCell ref="K85:N85"/>
-    <mergeCell ref="K86:N86"/>
-    <mergeCell ref="K87:N87"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="K71:N71"/>
-    <mergeCell ref="K72:N72"/>
-    <mergeCell ref="K73:N73"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="K45:N45"/>
-    <mergeCell ref="K46:N46"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="K48:N48"/>
-    <mergeCell ref="K60:N60"/>
-    <mergeCell ref="K49:N49"/>
-    <mergeCell ref="K50:N50"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="K52:N52"/>
-    <mergeCell ref="K56:N56"/>
-    <mergeCell ref="K53:N53"/>
-    <mergeCell ref="K54:N54"/>
-    <mergeCell ref="K55:N55"/>
-    <mergeCell ref="K39:N39"/>
-    <mergeCell ref="K40:N40"/>
-    <mergeCell ref="K41:N41"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="K43:N43"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="K36:N36"/>
-    <mergeCell ref="K37:N37"/>
-    <mergeCell ref="K38:N38"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="K30:N30"/>
-    <mergeCell ref="K31:N31"/>
-    <mergeCell ref="K32:N32"/>
-    <mergeCell ref="K33:N33"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K76:N76"/>
+    <mergeCell ref="K77:N77"/>
+    <mergeCell ref="K78:N78"/>
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="K91:N91"/>
+    <mergeCell ref="K92:N92"/>
+    <mergeCell ref="K93:N93"/>
+    <mergeCell ref="K94:N94"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="Q1048469:Q1048576 Q5:Q96"/>
@@ -11944,10 +11938,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
+      <c r="B1" s="152"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -11978,8 +11972,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -13074,10 +13068,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
+      <c r="B1" s="152"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -13105,8 +13099,8 @@
       <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
update dữ liệu đã chỉnh sử the review 3
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat dia diem/CF0142_Cap nhat dia diem.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat dia diem/CF0142_Cap nhat dia diem.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Update History" sheetId="4" r:id="rId1"/>
@@ -1389,7 +1389,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="308">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2594,6 +2594,9 @@
 @@IsCommon
 @@LastNodiyUserID
 GETDATE()</t>
+  </si>
+  <si>
+    <t>Tỉnh/ Thành phố</t>
   </si>
 </sst>
 </file>
@@ -3400,6 +3403,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3439,9 +3445,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3509,6 +3512,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3516,12 +3525,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3951,10 +3954,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
+      <c r="B1" s="152"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -3981,8 +3984,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -4021,14 +4024,14 @@
       <c r="D4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="152" t="s">
+      <c r="E4" s="153" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
+      <c r="F4" s="153"/>
+      <c r="G4" s="153"/>
+      <c r="H4" s="153"/>
+      <c r="I4" s="153"/>
+      <c r="J4" s="153"/>
     </row>
     <row r="5" spans="1:10" s="25" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="114">
@@ -4044,14 +4047,14 @@
         <f>H1</f>
         <v>Thị Phượng</v>
       </c>
-      <c r="E5" s="153" t="s">
+      <c r="E5" s="154" t="s">
         <v>280</v>
       </c>
-      <c r="F5" s="154"/>
-      <c r="G5" s="154"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
+      <c r="F5" s="155"/>
+      <c r="G5" s="155"/>
+      <c r="H5" s="155"/>
+      <c r="I5" s="155"/>
+      <c r="J5" s="155"/>
     </row>
     <row r="6" spans="1:10" s="144" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="140">
@@ -4062,12 +4065,12 @@
       </c>
       <c r="C6" s="142"/>
       <c r="D6" s="143"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="156"/>
-      <c r="G6" s="156"/>
-      <c r="H6" s="156"/>
-      <c r="I6" s="156"/>
-      <c r="J6" s="157"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="157"/>
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="158"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="86">
@@ -4078,12 +4081,12 @@
       </c>
       <c r="C7" s="76"/>
       <c r="D7" s="40"/>
-      <c r="E7" s="145"/>
-      <c r="F7" s="146"/>
-      <c r="G7" s="146"/>
-      <c r="H7" s="146"/>
-      <c r="I7" s="146"/>
-      <c r="J7" s="147"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="147"/>
+      <c r="I7" s="147"/>
+      <c r="J7" s="148"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="87">
@@ -4094,12 +4097,12 @@
       </c>
       <c r="C8" s="76"/>
       <c r="D8" s="40"/>
-      <c r="E8" s="148"/>
-      <c r="F8" s="149"/>
-      <c r="G8" s="149"/>
-      <c r="H8" s="149"/>
-      <c r="I8" s="149"/>
-      <c r="J8" s="150"/>
+      <c r="E8" s="149"/>
+      <c r="F8" s="150"/>
+      <c r="G8" s="150"/>
+      <c r="H8" s="150"/>
+      <c r="I8" s="150"/>
+      <c r="J8" s="151"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="88">
@@ -4110,12 +4113,12 @@
       </c>
       <c r="C9" s="76"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="145"/>
-      <c r="F9" s="146"/>
-      <c r="G9" s="146"/>
-      <c r="H9" s="146"/>
-      <c r="I9" s="146"/>
-      <c r="J9" s="147"/>
+      <c r="E9" s="146"/>
+      <c r="F9" s="147"/>
+      <c r="G9" s="147"/>
+      <c r="H9" s="147"/>
+      <c r="I9" s="147"/>
+      <c r="J9" s="148"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="89">
@@ -4126,12 +4129,12 @@
       </c>
       <c r="C10" s="76"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="146"/>
-      <c r="G10" s="146"/>
-      <c r="H10" s="146"/>
-      <c r="I10" s="146"/>
-      <c r="J10" s="147"/>
+      <c r="E10" s="146"/>
+      <c r="F10" s="147"/>
+      <c r="G10" s="147"/>
+      <c r="H10" s="147"/>
+      <c r="I10" s="147"/>
+      <c r="J10" s="148"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="90">
@@ -4142,12 +4145,12 @@
       </c>
       <c r="C11" s="76"/>
       <c r="D11" s="40"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="146"/>
-      <c r="G11" s="146"/>
-      <c r="H11" s="146"/>
-      <c r="I11" s="146"/>
-      <c r="J11" s="147"/>
+      <c r="E11" s="146"/>
+      <c r="F11" s="147"/>
+      <c r="G11" s="147"/>
+      <c r="H11" s="147"/>
+      <c r="I11" s="147"/>
+      <c r="J11" s="148"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="91">
@@ -4158,12 +4161,12 @@
       </c>
       <c r="C12" s="76"/>
       <c r="D12" s="40"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="146"/>
-      <c r="G12" s="146"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="147"/>
+      <c r="E12" s="146"/>
+      <c r="F12" s="147"/>
+      <c r="G12" s="147"/>
+      <c r="H12" s="147"/>
+      <c r="I12" s="147"/>
+      <c r="J12" s="148"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="92">
@@ -4174,12 +4177,12 @@
       </c>
       <c r="C13" s="76"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="145"/>
-      <c r="F13" s="146"/>
-      <c r="G13" s="146"/>
-      <c r="H13" s="146"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="147"/>
+      <c r="E13" s="146"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="147"/>
+      <c r="H13" s="147"/>
+      <c r="I13" s="147"/>
+      <c r="J13" s="148"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="93">
@@ -4190,12 +4193,12 @@
       </c>
       <c r="C14" s="76"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="145"/>
-      <c r="F14" s="146"/>
-      <c r="G14" s="146"/>
-      <c r="H14" s="146"/>
-      <c r="I14" s="146"/>
-      <c r="J14" s="147"/>
+      <c r="E14" s="146"/>
+      <c r="F14" s="147"/>
+      <c r="G14" s="147"/>
+      <c r="H14" s="147"/>
+      <c r="I14" s="147"/>
+      <c r="J14" s="148"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="40">
@@ -4206,12 +4209,12 @@
       </c>
       <c r="C15" s="76"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
-      <c r="H15" s="158"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="158"/>
+      <c r="E15" s="145"/>
+      <c r="F15" s="145"/>
+      <c r="G15" s="145"/>
+      <c r="H15" s="145"/>
+      <c r="I15" s="145"/>
+      <c r="J15" s="145"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="85">
@@ -4222,12 +4225,12 @@
       </c>
       <c r="C16" s="76"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
+      <c r="E16" s="145"/>
+      <c r="F16" s="145"/>
+      <c r="G16" s="145"/>
+      <c r="H16" s="145"/>
+      <c r="I16" s="145"/>
+      <c r="J16" s="145"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="86">
@@ -4238,12 +4241,12 @@
       </c>
       <c r="C17" s="76"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="158"/>
-      <c r="F17" s="158"/>
-      <c r="G17" s="158"/>
-      <c r="H17" s="158"/>
-      <c r="I17" s="158"/>
-      <c r="J17" s="158"/>
+      <c r="E17" s="145"/>
+      <c r="F17" s="145"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="145"/>
+      <c r="I17" s="145"/>
+      <c r="J17" s="145"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="87">
@@ -4254,12 +4257,12 @@
       </c>
       <c r="C18" s="76"/>
       <c r="D18" s="40"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="158"/>
-      <c r="G18" s="158"/>
-      <c r="H18" s="158"/>
-      <c r="I18" s="158"/>
-      <c r="J18" s="158"/>
+      <c r="E18" s="145"/>
+      <c r="F18" s="145"/>
+      <c r="G18" s="145"/>
+      <c r="H18" s="145"/>
+      <c r="I18" s="145"/>
+      <c r="J18" s="145"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="88">
@@ -4270,12 +4273,12 @@
       </c>
       <c r="C19" s="76"/>
       <c r="D19" s="40"/>
-      <c r="E19" s="158"/>
-      <c r="F19" s="158"/>
-      <c r="G19" s="158"/>
-      <c r="H19" s="158"/>
-      <c r="I19" s="158"/>
-      <c r="J19" s="158"/>
+      <c r="E19" s="145"/>
+      <c r="F19" s="145"/>
+      <c r="G19" s="145"/>
+      <c r="H19" s="145"/>
+      <c r="I19" s="145"/>
+      <c r="J19" s="145"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="89">
@@ -4286,12 +4289,12 @@
       </c>
       <c r="C20" s="76"/>
       <c r="D20" s="40"/>
-      <c r="E20" s="158"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158"/>
-      <c r="J20" s="158"/>
+      <c r="E20" s="145"/>
+      <c r="F20" s="145"/>
+      <c r="G20" s="145"/>
+      <c r="H20" s="145"/>
+      <c r="I20" s="145"/>
+      <c r="J20" s="145"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="90">
@@ -4302,12 +4305,12 @@
       </c>
       <c r="C21" s="76"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="158"/>
-      <c r="F21" s="158"/>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158"/>
-      <c r="J21" s="158"/>
+      <c r="E21" s="145"/>
+      <c r="F21" s="145"/>
+      <c r="G21" s="145"/>
+      <c r="H21" s="145"/>
+      <c r="I21" s="145"/>
+      <c r="J21" s="145"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="91">
@@ -4318,12 +4321,12 @@
       </c>
       <c r="C22" s="76"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158"/>
-      <c r="J22" s="158"/>
+      <c r="E22" s="145"/>
+      <c r="F22" s="145"/>
+      <c r="G22" s="145"/>
+      <c r="H22" s="145"/>
+      <c r="I22" s="145"/>
+      <c r="J22" s="145"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="92">
@@ -4334,12 +4337,12 @@
       </c>
       <c r="C23" s="76"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="158"/>
-      <c r="F23" s="158"/>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="158"/>
-      <c r="J23" s="158"/>
+      <c r="E23" s="145"/>
+      <c r="F23" s="145"/>
+      <c r="G23" s="145"/>
+      <c r="H23" s="145"/>
+      <c r="I23" s="145"/>
+      <c r="J23" s="145"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="93">
@@ -4350,12 +4353,12 @@
       </c>
       <c r="C24" s="76"/>
       <c r="D24" s="40"/>
-      <c r="E24" s="158"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="158"/>
-      <c r="H24" s="158"/>
-      <c r="I24" s="158"/>
-      <c r="J24" s="158"/>
+      <c r="E24" s="145"/>
+      <c r="F24" s="145"/>
+      <c r="G24" s="145"/>
+      <c r="H24" s="145"/>
+      <c r="I24" s="145"/>
+      <c r="J24" s="145"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="40">
@@ -4366,12 +4369,12 @@
       </c>
       <c r="C25" s="76"/>
       <c r="D25" s="40"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158"/>
-      <c r="H25" s="158"/>
-      <c r="I25" s="158"/>
-      <c r="J25" s="158"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
+      <c r="H25" s="145"/>
+      <c r="I25" s="145"/>
+      <c r="J25" s="145"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="85">
@@ -4382,12 +4385,12 @@
       </c>
       <c r="C26" s="76"/>
       <c r="D26" s="40"/>
-      <c r="E26" s="158"/>
-      <c r="F26" s="158"/>
-      <c r="G26" s="158"/>
-      <c r="H26" s="158"/>
-      <c r="I26" s="158"/>
-      <c r="J26" s="158"/>
+      <c r="E26" s="145"/>
+      <c r="F26" s="145"/>
+      <c r="G26" s="145"/>
+      <c r="H26" s="145"/>
+      <c r="I26" s="145"/>
+      <c r="J26" s="145"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="86">
@@ -4398,12 +4401,12 @@
       </c>
       <c r="C27" s="76"/>
       <c r="D27" s="40"/>
-      <c r="E27" s="158"/>
-      <c r="F27" s="158"/>
-      <c r="G27" s="158"/>
-      <c r="H27" s="158"/>
-      <c r="I27" s="158"/>
-      <c r="J27" s="158"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
+      <c r="H27" s="145"/>
+      <c r="I27" s="145"/>
+      <c r="J27" s="145"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="87">
@@ -4414,12 +4417,12 @@
       </c>
       <c r="C28" s="76"/>
       <c r="D28" s="40"/>
-      <c r="E28" s="158"/>
-      <c r="F28" s="158"/>
-      <c r="G28" s="158"/>
-      <c r="H28" s="158"/>
-      <c r="I28" s="158"/>
-      <c r="J28" s="158"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="145"/>
+      <c r="H28" s="145"/>
+      <c r="I28" s="145"/>
+      <c r="J28" s="145"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="88">
@@ -4430,12 +4433,12 @@
       </c>
       <c r="C29" s="76"/>
       <c r="D29" s="40"/>
-      <c r="E29" s="158"/>
-      <c r="F29" s="158"/>
-      <c r="G29" s="158"/>
-      <c r="H29" s="158"/>
-      <c r="I29" s="158"/>
-      <c r="J29" s="158"/>
+      <c r="E29" s="145"/>
+      <c r="F29" s="145"/>
+      <c r="G29" s="145"/>
+      <c r="H29" s="145"/>
+      <c r="I29" s="145"/>
+      <c r="J29" s="145"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="89">
@@ -4446,12 +4449,12 @@
       </c>
       <c r="C30" s="76"/>
       <c r="D30" s="40"/>
-      <c r="E30" s="158"/>
-      <c r="F30" s="158"/>
-      <c r="G30" s="158"/>
-      <c r="H30" s="158"/>
-      <c r="I30" s="158"/>
-      <c r="J30" s="158"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
+      <c r="H30" s="145"/>
+      <c r="I30" s="145"/>
+      <c r="J30" s="145"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="90">
@@ -4462,12 +4465,12 @@
       </c>
       <c r="C31" s="76"/>
       <c r="D31" s="40"/>
-      <c r="E31" s="158"/>
-      <c r="F31" s="158"/>
-      <c r="G31" s="158"/>
-      <c r="H31" s="158"/>
-      <c r="I31" s="158"/>
-      <c r="J31" s="158"/>
+      <c r="E31" s="145"/>
+      <c r="F31" s="145"/>
+      <c r="G31" s="145"/>
+      <c r="H31" s="145"/>
+      <c r="I31" s="145"/>
+      <c r="J31" s="145"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="91">
@@ -4478,12 +4481,12 @@
       </c>
       <c r="C32" s="76"/>
       <c r="D32" s="40"/>
-      <c r="E32" s="158"/>
-      <c r="F32" s="158"/>
-      <c r="G32" s="158"/>
-      <c r="H32" s="158"/>
-      <c r="I32" s="158"/>
-      <c r="J32" s="158"/>
+      <c r="E32" s="145"/>
+      <c r="F32" s="145"/>
+      <c r="G32" s="145"/>
+      <c r="H32" s="145"/>
+      <c r="I32" s="145"/>
+      <c r="J32" s="145"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="92">
@@ -4494,12 +4497,12 @@
       </c>
       <c r="C33" s="76"/>
       <c r="D33" s="40"/>
-      <c r="E33" s="158"/>
-      <c r="F33" s="158"/>
-      <c r="G33" s="158"/>
-      <c r="H33" s="158"/>
-      <c r="I33" s="158"/>
-      <c r="J33" s="158"/>
+      <c r="E33" s="145"/>
+      <c r="F33" s="145"/>
+      <c r="G33" s="145"/>
+      <c r="H33" s="145"/>
+      <c r="I33" s="145"/>
+      <c r="J33" s="145"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="93">
@@ -4510,12 +4513,12 @@
       </c>
       <c r="C34" s="76"/>
       <c r="D34" s="40"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="158"/>
-      <c r="H34" s="158"/>
-      <c r="I34" s="158"/>
-      <c r="J34" s="158"/>
+      <c r="E34" s="145"/>
+      <c r="F34" s="145"/>
+      <c r="G34" s="145"/>
+      <c r="H34" s="145"/>
+      <c r="I34" s="145"/>
+      <c r="J34" s="145"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="40">
@@ -4526,12 +4529,12 @@
       </c>
       <c r="C35" s="76"/>
       <c r="D35" s="40"/>
-      <c r="E35" s="158"/>
-      <c r="F35" s="158"/>
-      <c r="G35" s="158"/>
-      <c r="H35" s="158"/>
-      <c r="I35" s="158"/>
-      <c r="J35" s="158"/>
+      <c r="E35" s="145"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="145"/>
+      <c r="H35" s="145"/>
+      <c r="I35" s="145"/>
+      <c r="J35" s="145"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="85">
@@ -4542,12 +4545,12 @@
       </c>
       <c r="C36" s="76"/>
       <c r="D36" s="40"/>
-      <c r="E36" s="158"/>
-      <c r="F36" s="158"/>
-      <c r="G36" s="158"/>
-      <c r="H36" s="158"/>
-      <c r="I36" s="158"/>
-      <c r="J36" s="158"/>
+      <c r="E36" s="145"/>
+      <c r="F36" s="145"/>
+      <c r="G36" s="145"/>
+      <c r="H36" s="145"/>
+      <c r="I36" s="145"/>
+      <c r="J36" s="145"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="86">
@@ -4558,12 +4561,12 @@
       </c>
       <c r="C37" s="76"/>
       <c r="D37" s="40"/>
-      <c r="E37" s="158"/>
-      <c r="F37" s="158"/>
-      <c r="G37" s="158"/>
-      <c r="H37" s="158"/>
-      <c r="I37" s="158"/>
-      <c r="J37" s="158"/>
+      <c r="E37" s="145"/>
+      <c r="F37" s="145"/>
+      <c r="G37" s="145"/>
+      <c r="H37" s="145"/>
+      <c r="I37" s="145"/>
+      <c r="J37" s="145"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="87">
@@ -4574,12 +4577,12 @@
       </c>
       <c r="C38" s="76"/>
       <c r="D38" s="40"/>
-      <c r="E38" s="158"/>
-      <c r="F38" s="158"/>
-      <c r="G38" s="158"/>
-      <c r="H38" s="158"/>
-      <c r="I38" s="158"/>
-      <c r="J38" s="158"/>
+      <c r="E38" s="145"/>
+      <c r="F38" s="145"/>
+      <c r="G38" s="145"/>
+      <c r="H38" s="145"/>
+      <c r="I38" s="145"/>
+      <c r="J38" s="145"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="88">
@@ -4590,12 +4593,12 @@
       </c>
       <c r="C39" s="76"/>
       <c r="D39" s="40"/>
-      <c r="E39" s="158"/>
-      <c r="F39" s="158"/>
-      <c r="G39" s="158"/>
-      <c r="H39" s="158"/>
-      <c r="I39" s="158"/>
-      <c r="J39" s="158"/>
+      <c r="E39" s="145"/>
+      <c r="F39" s="145"/>
+      <c r="G39" s="145"/>
+      <c r="H39" s="145"/>
+      <c r="I39" s="145"/>
+      <c r="J39" s="145"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="89">
@@ -4606,12 +4609,12 @@
       </c>
       <c r="C40" s="76"/>
       <c r="D40" s="40"/>
-      <c r="E40" s="158"/>
-      <c r="F40" s="158"/>
-      <c r="G40" s="158"/>
-      <c r="H40" s="158"/>
-      <c r="I40" s="158"/>
-      <c r="J40" s="158"/>
+      <c r="E40" s="145"/>
+      <c r="F40" s="145"/>
+      <c r="G40" s="145"/>
+      <c r="H40" s="145"/>
+      <c r="I40" s="145"/>
+      <c r="J40" s="145"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="90">
@@ -4622,12 +4625,12 @@
       </c>
       <c r="C41" s="76"/>
       <c r="D41" s="40"/>
-      <c r="E41" s="158"/>
-      <c r="F41" s="158"/>
-      <c r="G41" s="158"/>
-      <c r="H41" s="158"/>
-      <c r="I41" s="158"/>
-      <c r="J41" s="158"/>
+      <c r="E41" s="145"/>
+      <c r="F41" s="145"/>
+      <c r="G41" s="145"/>
+      <c r="H41" s="145"/>
+      <c r="I41" s="145"/>
+      <c r="J41" s="145"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="91">
@@ -4638,32 +4641,23 @@
       </c>
       <c r="C42" s="76"/>
       <c r="D42" s="40"/>
-      <c r="E42" s="158"/>
-      <c r="F42" s="158"/>
-      <c r="G42" s="158"/>
-      <c r="H42" s="158"/>
-      <c r="I42" s="158"/>
-      <c r="J42" s="158"/>
+      <c r="E42" s="145"/>
+      <c r="F42" s="145"/>
+      <c r="G42" s="145"/>
+      <c r="H42" s="145"/>
+      <c r="I42" s="145"/>
+      <c r="J42" s="145"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E25:J25"/>
@@ -4679,14 +4673,23 @@
     <mergeCell ref="E22:J22"/>
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -4901,10 +4904,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
+      <c r="B1" s="152"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -4934,8 +4937,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -5511,13 +5514,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
       <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
@@ -5551,11 +5554,11 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
       <c r="F2" s="30" t="s">
         <v>2</v>
       </c>
@@ -6964,8 +6967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G12:G13"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7190,7 +7193,9 @@
         <v>232</v>
       </c>
       <c r="C8" s="33"/>
-      <c r="D8" s="136"/>
+      <c r="D8" s="136" t="s">
+        <v>307</v>
+      </c>
       <c r="E8" s="136" t="s">
         <v>281</v>
       </c>
@@ -8139,15 +8144,15 @@
       <c r="F4" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="151" t="s">
+      <c r="G4" s="152" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="151"/>
-      <c r="I4" s="151" t="s">
+      <c r="H4" s="152"/>
+      <c r="I4" s="152" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="151"/>
-      <c r="K4" s="151"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="152"/>
     </row>
     <row r="5" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
@@ -8162,15 +8167,15 @@
         <v>135</v>
       </c>
       <c r="F5" s="32"/>
-      <c r="G5" s="184" t="s">
+      <c r="G5" s="181" t="s">
         <v>243</v>
       </c>
-      <c r="H5" s="185"/>
-      <c r="I5" s="181" t="s">
+      <c r="H5" s="182"/>
+      <c r="I5" s="183" t="s">
         <v>288</v>
       </c>
-      <c r="J5" s="182"/>
-      <c r="K5" s="183"/>
+      <c r="J5" s="184"/>
+      <c r="K5" s="185"/>
     </row>
     <row r="6" spans="1:13" s="34" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33">
@@ -8185,15 +8190,15 @@
         <v>242</v>
       </c>
       <c r="F6" s="32"/>
-      <c r="G6" s="184" t="s">
+      <c r="G6" s="181" t="s">
         <v>244</v>
       </c>
-      <c r="H6" s="185"/>
-      <c r="I6" s="181" t="s">
+      <c r="H6" s="182"/>
+      <c r="I6" s="183" t="s">
         <v>289</v>
       </c>
-      <c r="J6" s="182"/>
-      <c r="K6" s="183"/>
+      <c r="J6" s="184"/>
+      <c r="K6" s="185"/>
     </row>
     <row r="7" spans="1:13" s="34" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
@@ -8208,15 +8213,15 @@
         <v>242</v>
       </c>
       <c r="F7" s="32"/>
-      <c r="G7" s="184" t="s">
+      <c r="G7" s="181" t="s">
         <v>244</v>
       </c>
-      <c r="H7" s="185"/>
-      <c r="I7" s="181" t="s">
+      <c r="H7" s="182"/>
+      <c r="I7" s="183" t="s">
         <v>290</v>
       </c>
-      <c r="J7" s="182"/>
-      <c r="K7" s="183"/>
+      <c r="J7" s="184"/>
+      <c r="K7" s="185"/>
     </row>
     <row r="8" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
@@ -8227,11 +8232,11 @@
       <c r="D8" s="33"/>
       <c r="E8" s="33"/>
       <c r="F8" s="32"/>
-      <c r="G8" s="184"/>
-      <c r="H8" s="185"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="182"/>
-      <c r="K8" s="183"/>
+      <c r="G8" s="181"/>
+      <c r="H8" s="182"/>
+      <c r="I8" s="183"/>
+      <c r="J8" s="184"/>
+      <c r="K8" s="185"/>
     </row>
     <row r="9" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33">
@@ -8242,11 +8247,11 @@
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
       <c r="F9" s="32"/>
-      <c r="G9" s="184"/>
-      <c r="H9" s="185"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="182"/>
-      <c r="K9" s="183"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="182"/>
+      <c r="I9" s="183"/>
+      <c r="J9" s="184"/>
+      <c r="K9" s="185"/>
     </row>
     <row r="10" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="33">
@@ -8257,11 +8262,11 @@
       <c r="D10" s="33"/>
       <c r="E10" s="33"/>
       <c r="F10" s="32"/>
-      <c r="G10" s="184"/>
-      <c r="H10" s="185"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="182"/>
-      <c r="K10" s="183"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="182"/>
+      <c r="I10" s="183"/>
+      <c r="J10" s="184"/>
+      <c r="K10" s="185"/>
     </row>
     <row r="11" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33">
@@ -8272,11 +8277,11 @@
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
       <c r="F11" s="32"/>
-      <c r="G11" s="184"/>
-      <c r="H11" s="185"/>
-      <c r="I11" s="181"/>
-      <c r="J11" s="182"/>
-      <c r="K11" s="183"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="182"/>
+      <c r="I11" s="183"/>
+      <c r="J11" s="184"/>
+      <c r="K11" s="185"/>
     </row>
     <row r="12" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="33">
@@ -8287,11 +8292,11 @@
       <c r="D12" s="33"/>
       <c r="E12" s="33"/>
       <c r="F12" s="32"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="185"/>
-      <c r="I12" s="181"/>
-      <c r="J12" s="182"/>
-      <c r="K12" s="183"/>
+      <c r="G12" s="181"/>
+      <c r="H12" s="182"/>
+      <c r="I12" s="183"/>
+      <c r="J12" s="184"/>
+      <c r="K12" s="185"/>
     </row>
     <row r="13" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33">
@@ -8302,11 +8307,11 @@
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
       <c r="F13" s="32"/>
-      <c r="G13" s="184"/>
-      <c r="H13" s="185"/>
-      <c r="I13" s="181"/>
-      <c r="J13" s="182"/>
-      <c r="K13" s="183"/>
+      <c r="G13" s="181"/>
+      <c r="H13" s="182"/>
+      <c r="I13" s="183"/>
+      <c r="J13" s="184"/>
+      <c r="K13" s="185"/>
     </row>
     <row r="14" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
@@ -8317,11 +8322,11 @@
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
       <c r="F14" s="32"/>
-      <c r="G14" s="184"/>
-      <c r="H14" s="185"/>
-      <c r="I14" s="181"/>
-      <c r="J14" s="182"/>
-      <c r="K14" s="183"/>
+      <c r="G14" s="181"/>
+      <c r="H14" s="182"/>
+      <c r="I14" s="183"/>
+      <c r="J14" s="184"/>
+      <c r="K14" s="185"/>
     </row>
     <row r="15" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33">
@@ -8332,11 +8337,11 @@
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
       <c r="F15" s="32"/>
-      <c r="G15" s="184"/>
-      <c r="H15" s="185"/>
-      <c r="I15" s="181"/>
-      <c r="J15" s="182"/>
-      <c r="K15" s="183"/>
+      <c r="G15" s="181"/>
+      <c r="H15" s="182"/>
+      <c r="I15" s="183"/>
+      <c r="J15" s="184"/>
+      <c r="K15" s="185"/>
     </row>
     <row r="16" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33">
@@ -8347,11 +8352,11 @@
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
       <c r="F16" s="32"/>
-      <c r="G16" s="184"/>
-      <c r="H16" s="185"/>
-      <c r="I16" s="181"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="183"/>
+      <c r="G16" s="181"/>
+      <c r="H16" s="182"/>
+      <c r="I16" s="183"/>
+      <c r="J16" s="184"/>
+      <c r="K16" s="185"/>
     </row>
     <row r="17" spans="1:19" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A17" s="33">
@@ -8362,11 +8367,11 @@
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
       <c r="F17" s="32"/>
-      <c r="G17" s="184"/>
-      <c r="H17" s="185"/>
-      <c r="I17" s="181"/>
-      <c r="J17" s="182"/>
-      <c r="K17" s="183"/>
+      <c r="G17" s="181"/>
+      <c r="H17" s="182"/>
+      <c r="I17" s="183"/>
+      <c r="J17" s="184"/>
+      <c r="K17" s="185"/>
     </row>
     <row r="18" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33">
@@ -8377,11 +8382,11 @@
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
       <c r="F18" s="32"/>
-      <c r="G18" s="184"/>
-      <c r="H18" s="185"/>
-      <c r="I18" s="181"/>
-      <c r="J18" s="182"/>
-      <c r="K18" s="183"/>
+      <c r="G18" s="181"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="183"/>
+      <c r="J18" s="184"/>
+      <c r="K18" s="185"/>
     </row>
     <row r="19" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33">
@@ -8392,11 +8397,11 @@
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
       <c r="F19" s="32"/>
-      <c r="G19" s="184"/>
-      <c r="H19" s="185"/>
-      <c r="I19" s="181"/>
-      <c r="J19" s="182"/>
-      <c r="K19" s="183"/>
+      <c r="G19" s="181"/>
+      <c r="H19" s="182"/>
+      <c r="I19" s="183"/>
+      <c r="J19" s="184"/>
+      <c r="K19" s="185"/>
     </row>
     <row r="20" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="33">
@@ -8407,11 +8412,11 @@
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
       <c r="F20" s="32"/>
-      <c r="G20" s="184"/>
-      <c r="H20" s="185"/>
-      <c r="I20" s="181"/>
-      <c r="J20" s="182"/>
-      <c r="K20" s="183"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="183"/>
+      <c r="J20" s="184"/>
+      <c r="K20" s="185"/>
     </row>
     <row r="21" spans="1:19" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A21" s="33">
@@ -8422,11 +8427,11 @@
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
       <c r="F21" s="32"/>
-      <c r="G21" s="184"/>
-      <c r="H21" s="185"/>
-      <c r="I21" s="181"/>
-      <c r="J21" s="182"/>
-      <c r="K21" s="183"/>
+      <c r="G21" s="181"/>
+      <c r="H21" s="182"/>
+      <c r="I21" s="183"/>
+      <c r="J21" s="184"/>
+      <c r="K21" s="185"/>
     </row>
     <row r="22" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="33">
@@ -8437,11 +8442,11 @@
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
       <c r="F22" s="32"/>
-      <c r="G22" s="145"/>
-      <c r="H22" s="147"/>
-      <c r="I22" s="181"/>
-      <c r="J22" s="182"/>
-      <c r="K22" s="183"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="148"/>
+      <c r="I22" s="183"/>
+      <c r="J22" s="184"/>
+      <c r="K22" s="185"/>
     </row>
     <row r="23" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="33">
@@ -8452,11 +8457,11 @@
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
       <c r="F23" s="32"/>
-      <c r="G23" s="145"/>
-      <c r="H23" s="147"/>
-      <c r="I23" s="181"/>
-      <c r="J23" s="182"/>
-      <c r="K23" s="183"/>
+      <c r="G23" s="146"/>
+      <c r="H23" s="148"/>
+      <c r="I23" s="183"/>
+      <c r="J23" s="184"/>
+      <c r="K23" s="185"/>
     </row>
     <row r="24" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="33">
@@ -8467,11 +8472,11 @@
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="32"/>
-      <c r="G24" s="145"/>
-      <c r="H24" s="147"/>
-      <c r="I24" s="181"/>
-      <c r="J24" s="182"/>
-      <c r="K24" s="183"/>
+      <c r="G24" s="146"/>
+      <c r="H24" s="148"/>
+      <c r="I24" s="183"/>
+      <c r="J24" s="184"/>
+      <c r="K24" s="185"/>
     </row>
     <row r="25" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="33">
@@ -8482,11 +8487,11 @@
       <c r="D25" s="33"/>
       <c r="E25" s="33"/>
       <c r="F25" s="32"/>
-      <c r="G25" s="145"/>
-      <c r="H25" s="147"/>
-      <c r="I25" s="181"/>
-      <c r="J25" s="182"/>
-      <c r="K25" s="183"/>
+      <c r="G25" s="146"/>
+      <c r="H25" s="148"/>
+      <c r="I25" s="183"/>
+      <c r="J25" s="184"/>
+      <c r="K25" s="185"/>
     </row>
     <row r="26" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33">
@@ -8497,11 +8502,11 @@
       <c r="D26" s="33"/>
       <c r="E26" s="33"/>
       <c r="F26" s="32"/>
-      <c r="G26" s="145"/>
-      <c r="H26" s="147"/>
-      <c r="I26" s="181"/>
-      <c r="J26" s="182"/>
-      <c r="K26" s="183"/>
+      <c r="G26" s="146"/>
+      <c r="H26" s="148"/>
+      <c r="I26" s="183"/>
+      <c r="J26" s="184"/>
+      <c r="K26" s="185"/>
     </row>
     <row r="27" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33">
@@ -8512,11 +8517,11 @@
       <c r="D27" s="33"/>
       <c r="E27" s="33"/>
       <c r="F27" s="32"/>
-      <c r="G27" s="145"/>
-      <c r="H27" s="147"/>
-      <c r="I27" s="181"/>
-      <c r="J27" s="182"/>
-      <c r="K27" s="183"/>
+      <c r="G27" s="146"/>
+      <c r="H27" s="148"/>
+      <c r="I27" s="183"/>
+      <c r="J27" s="184"/>
+      <c r="K27" s="185"/>
     </row>
     <row r="28" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="33">
@@ -8527,11 +8532,11 @@
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
       <c r="F28" s="32"/>
-      <c r="G28" s="145"/>
-      <c r="H28" s="147"/>
-      <c r="I28" s="181"/>
-      <c r="J28" s="182"/>
-      <c r="K28" s="183"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="148"/>
+      <c r="I28" s="183"/>
+      <c r="J28" s="184"/>
+      <c r="K28" s="185"/>
     </row>
     <row r="29" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="33">
@@ -8542,11 +8547,11 @@
       <c r="D29" s="33"/>
       <c r="E29" s="33"/>
       <c r="F29" s="32"/>
-      <c r="G29" s="145"/>
-      <c r="H29" s="147"/>
-      <c r="I29" s="181"/>
-      <c r="J29" s="182"/>
-      <c r="K29" s="183"/>
+      <c r="G29" s="146"/>
+      <c r="H29" s="148"/>
+      <c r="I29" s="183"/>
+      <c r="J29" s="184"/>
+      <c r="K29" s="185"/>
     </row>
     <row r="30" spans="1:19" s="34" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="33">
@@ -8557,11 +8562,11 @@
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="32"/>
-      <c r="G30" s="145"/>
-      <c r="H30" s="147"/>
-      <c r="I30" s="181"/>
-      <c r="J30" s="182"/>
-      <c r="K30" s="183"/>
+      <c r="G30" s="146"/>
+      <c r="H30" s="148"/>
+      <c r="I30" s="183"/>
+      <c r="J30" s="184"/>
+      <c r="K30" s="185"/>
     </row>
     <row r="31" spans="1:19" s="34" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="33">
@@ -8572,11 +8577,11 @@
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
       <c r="F31" s="32"/>
-      <c r="G31" s="145"/>
-      <c r="H31" s="147"/>
-      <c r="I31" s="181"/>
-      <c r="J31" s="182"/>
-      <c r="K31" s="183"/>
+      <c r="G31" s="146"/>
+      <c r="H31" s="148"/>
+      <c r="I31" s="183"/>
+      <c r="J31" s="184"/>
+      <c r="K31" s="185"/>
     </row>
     <row r="32" spans="1:19" ht="11.25" x14ac:dyDescent="0.15">
       <c r="A32" s="33">
@@ -8587,11 +8592,11 @@
       <c r="D32" s="33"/>
       <c r="E32" s="33"/>
       <c r="F32" s="32"/>
-      <c r="G32" s="145"/>
-      <c r="H32" s="147"/>
-      <c r="I32" s="181"/>
-      <c r="J32" s="182"/>
-      <c r="K32" s="183"/>
+      <c r="G32" s="146"/>
+      <c r="H32" s="148"/>
+      <c r="I32" s="183"/>
+      <c r="J32" s="184"/>
+      <c r="K32" s="185"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
@@ -8609,11 +8614,11 @@
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
       <c r="F33" s="32"/>
-      <c r="G33" s="145"/>
-      <c r="H33" s="147"/>
-      <c r="I33" s="181"/>
-      <c r="J33" s="182"/>
-      <c r="K33" s="183"/>
+      <c r="G33" s="146"/>
+      <c r="H33" s="148"/>
+      <c r="I33" s="183"/>
+      <c r="J33" s="184"/>
+      <c r="K33" s="185"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
       <c r="O33" s="22"/>
@@ -8631,11 +8636,11 @@
       <c r="D34" s="33"/>
       <c r="E34" s="33"/>
       <c r="F34" s="32"/>
-      <c r="G34" s="145"/>
-      <c r="H34" s="147"/>
-      <c r="I34" s="181"/>
-      <c r="J34" s="182"/>
-      <c r="K34" s="183"/>
+      <c r="G34" s="146"/>
+      <c r="H34" s="148"/>
+      <c r="I34" s="183"/>
+      <c r="J34" s="184"/>
+      <c r="K34" s="185"/>
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
       <c r="O34" s="22"/>
@@ -8653,11 +8658,11 @@
       <c r="D35" s="33"/>
       <c r="E35" s="33"/>
       <c r="F35" s="32"/>
-      <c r="G35" s="145"/>
-      <c r="H35" s="147"/>
-      <c r="I35" s="181"/>
-      <c r="J35" s="182"/>
-      <c r="K35" s="183"/>
+      <c r="G35" s="146"/>
+      <c r="H35" s="148"/>
+      <c r="I35" s="183"/>
+      <c r="J35" s="184"/>
+      <c r="K35" s="185"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="22"/>
@@ -8675,11 +8680,11 @@
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
       <c r="F36" s="32"/>
-      <c r="G36" s="145"/>
-      <c r="H36" s="147"/>
-      <c r="I36" s="181"/>
-      <c r="J36" s="182"/>
-      <c r="K36" s="183"/>
+      <c r="G36" s="146"/>
+      <c r="H36" s="148"/>
+      <c r="I36" s="183"/>
+      <c r="J36" s="184"/>
+      <c r="K36" s="185"/>
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
       <c r="O36" s="22"/>
@@ -8697,11 +8702,11 @@
       <c r="D37" s="33"/>
       <c r="E37" s="33"/>
       <c r="F37" s="32"/>
-      <c r="G37" s="145"/>
-      <c r="H37" s="147"/>
-      <c r="I37" s="181"/>
-      <c r="J37" s="182"/>
-      <c r="K37" s="183"/>
+      <c r="G37" s="146"/>
+      <c r="H37" s="148"/>
+      <c r="I37" s="183"/>
+      <c r="J37" s="184"/>
+      <c r="K37" s="185"/>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22"/>
@@ -8719,11 +8724,11 @@
       <c r="D38" s="33"/>
       <c r="E38" s="33"/>
       <c r="F38" s="32"/>
-      <c r="G38" s="145"/>
-      <c r="H38" s="147"/>
-      <c r="I38" s="181"/>
-      <c r="J38" s="182"/>
-      <c r="K38" s="183"/>
+      <c r="G38" s="146"/>
+      <c r="H38" s="148"/>
+      <c r="I38" s="183"/>
+      <c r="J38" s="184"/>
+      <c r="K38" s="185"/>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
       <c r="O38" s="22"/>
@@ -8741,11 +8746,11 @@
       <c r="D39" s="33"/>
       <c r="E39" s="33"/>
       <c r="F39" s="32"/>
-      <c r="G39" s="145"/>
-      <c r="H39" s="147"/>
-      <c r="I39" s="181"/>
-      <c r="J39" s="182"/>
-      <c r="K39" s="183"/>
+      <c r="G39" s="146"/>
+      <c r="H39" s="148"/>
+      <c r="I39" s="183"/>
+      <c r="J39" s="184"/>
+      <c r="K39" s="185"/>
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22"/>
@@ -8763,11 +8768,11 @@
       <c r="D40" s="33"/>
       <c r="E40" s="33"/>
       <c r="F40" s="32"/>
-      <c r="G40" s="145"/>
-      <c r="H40" s="147"/>
-      <c r="I40" s="181"/>
-      <c r="J40" s="182"/>
-      <c r="K40" s="183"/>
+      <c r="G40" s="146"/>
+      <c r="H40" s="148"/>
+      <c r="I40" s="183"/>
+      <c r="J40" s="184"/>
+      <c r="K40" s="185"/>
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
       <c r="O40" s="22"/>
@@ -8785,11 +8790,11 @@
       <c r="D41" s="33"/>
       <c r="E41" s="33"/>
       <c r="F41" s="32"/>
-      <c r="G41" s="145"/>
-      <c r="H41" s="147"/>
-      <c r="I41" s="181"/>
-      <c r="J41" s="182"/>
-      <c r="K41" s="183"/>
+      <c r="G41" s="146"/>
+      <c r="H41" s="148"/>
+      <c r="I41" s="183"/>
+      <c r="J41" s="184"/>
+      <c r="K41" s="185"/>
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22"/>
@@ -8807,11 +8812,11 @@
       <c r="D42" s="33"/>
       <c r="E42" s="33"/>
       <c r="F42" s="32"/>
-      <c r="G42" s="145"/>
-      <c r="H42" s="147"/>
-      <c r="I42" s="181"/>
-      <c r="J42" s="182"/>
-      <c r="K42" s="183"/>
+      <c r="G42" s="146"/>
+      <c r="H42" s="148"/>
+      <c r="I42" s="183"/>
+      <c r="J42" s="184"/>
+      <c r="K42" s="185"/>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
       <c r="O42" s="22"/>
@@ -8829,11 +8834,11 @@
       <c r="D43" s="33"/>
       <c r="E43" s="33"/>
       <c r="F43" s="32"/>
-      <c r="G43" s="145"/>
-      <c r="H43" s="147"/>
-      <c r="I43" s="181"/>
-      <c r="J43" s="182"/>
-      <c r="K43" s="183"/>
+      <c r="G43" s="146"/>
+      <c r="H43" s="148"/>
+      <c r="I43" s="183"/>
+      <c r="J43" s="184"/>
+      <c r="K43" s="185"/>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
       <c r="O43" s="22"/>
@@ -8851,11 +8856,11 @@
       <c r="D44" s="33"/>
       <c r="E44" s="33"/>
       <c r="F44" s="32"/>
-      <c r="G44" s="145"/>
-      <c r="H44" s="147"/>
-      <c r="I44" s="181"/>
-      <c r="J44" s="182"/>
-      <c r="K44" s="183"/>
+      <c r="G44" s="146"/>
+      <c r="H44" s="148"/>
+      <c r="I44" s="183"/>
+      <c r="J44" s="184"/>
+      <c r="K44" s="185"/>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
       <c r="O44" s="22"/>
@@ -8873,11 +8878,11 @@
       <c r="D45" s="33"/>
       <c r="E45" s="33"/>
       <c r="F45" s="32"/>
-      <c r="G45" s="145"/>
-      <c r="H45" s="147"/>
-      <c r="I45" s="181"/>
-      <c r="J45" s="182"/>
-      <c r="K45" s="183"/>
+      <c r="G45" s="146"/>
+      <c r="H45" s="148"/>
+      <c r="I45" s="183"/>
+      <c r="J45" s="184"/>
+      <c r="K45" s="185"/>
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
       <c r="O45" s="22"/>
@@ -8895,11 +8900,11 @@
       <c r="D46" s="33"/>
       <c r="E46" s="33"/>
       <c r="F46" s="32"/>
-      <c r="G46" s="145"/>
-      <c r="H46" s="147"/>
-      <c r="I46" s="181"/>
-      <c r="J46" s="182"/>
-      <c r="K46" s="183"/>
+      <c r="G46" s="146"/>
+      <c r="H46" s="148"/>
+      <c r="I46" s="183"/>
+      <c r="J46" s="184"/>
+      <c r="K46" s="185"/>
       <c r="M46" s="22"/>
       <c r="N46" s="22"/>
       <c r="O46" s="22"/>
@@ -8917,11 +8922,11 @@
       <c r="D47" s="33"/>
       <c r="E47" s="33"/>
       <c r="F47" s="32"/>
-      <c r="G47" s="145"/>
-      <c r="H47" s="147"/>
-      <c r="I47" s="181"/>
-      <c r="J47" s="182"/>
-      <c r="K47" s="183"/>
+      <c r="G47" s="146"/>
+      <c r="H47" s="148"/>
+      <c r="I47" s="183"/>
+      <c r="J47" s="184"/>
+      <c r="K47" s="185"/>
       <c r="M47" s="22"/>
       <c r="N47" s="22"/>
       <c r="O47" s="22"/>
@@ -8939,11 +8944,11 @@
       <c r="D48" s="33"/>
       <c r="E48" s="33"/>
       <c r="F48" s="32"/>
-      <c r="G48" s="145"/>
-      <c r="H48" s="147"/>
-      <c r="I48" s="181"/>
-      <c r="J48" s="182"/>
-      <c r="K48" s="183"/>
+      <c r="G48" s="146"/>
+      <c r="H48" s="148"/>
+      <c r="I48" s="183"/>
+      <c r="J48" s="184"/>
+      <c r="K48" s="185"/>
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
       <c r="O48" s="22"/>
@@ -8961,11 +8966,11 @@
       <c r="D49" s="33"/>
       <c r="E49" s="33"/>
       <c r="F49" s="32"/>
-      <c r="G49" s="145"/>
-      <c r="H49" s="147"/>
-      <c r="I49" s="181"/>
-      <c r="J49" s="182"/>
-      <c r="K49" s="183"/>
+      <c r="G49" s="146"/>
+      <c r="H49" s="148"/>
+      <c r="I49" s="183"/>
+      <c r="J49" s="184"/>
+      <c r="K49" s="185"/>
       <c r="M49" s="22"/>
       <c r="N49" s="22"/>
       <c r="O49" s="22"/>
@@ -8983,11 +8988,11 @@
       <c r="D50" s="33"/>
       <c r="E50" s="33"/>
       <c r="F50" s="32"/>
-      <c r="G50" s="145"/>
-      <c r="H50" s="147"/>
-      <c r="I50" s="181"/>
-      <c r="J50" s="182"/>
-      <c r="K50" s="183"/>
+      <c r="G50" s="146"/>
+      <c r="H50" s="148"/>
+      <c r="I50" s="183"/>
+      <c r="J50" s="184"/>
+      <c r="K50" s="185"/>
       <c r="M50" s="22"/>
       <c r="N50" s="22"/>
       <c r="O50" s="22"/>
@@ -9005,11 +9010,11 @@
       <c r="D51" s="33"/>
       <c r="E51" s="33"/>
       <c r="F51" s="32"/>
-      <c r="G51" s="145"/>
-      <c r="H51" s="147"/>
-      <c r="I51" s="181"/>
-      <c r="J51" s="182"/>
-      <c r="K51" s="183"/>
+      <c r="G51" s="146"/>
+      <c r="H51" s="148"/>
+      <c r="I51" s="183"/>
+      <c r="J51" s="184"/>
+      <c r="K51" s="185"/>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
       <c r="O51" s="22"/>
@@ -9027,11 +9032,11 @@
       <c r="D52" s="33"/>
       <c r="E52" s="33"/>
       <c r="F52" s="32"/>
-      <c r="G52" s="145"/>
-      <c r="H52" s="147"/>
-      <c r="I52" s="181"/>
-      <c r="J52" s="182"/>
-      <c r="K52" s="183"/>
+      <c r="G52" s="146"/>
+      <c r="H52" s="148"/>
+      <c r="I52" s="183"/>
+      <c r="J52" s="184"/>
+      <c r="K52" s="185"/>
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
       <c r="O52" s="22"/>
@@ -9049,11 +9054,11 @@
       <c r="D53" s="33"/>
       <c r="E53" s="33"/>
       <c r="F53" s="32"/>
-      <c r="G53" s="145"/>
-      <c r="H53" s="147"/>
-      <c r="I53" s="181"/>
-      <c r="J53" s="182"/>
-      <c r="K53" s="183"/>
+      <c r="G53" s="146"/>
+      <c r="H53" s="148"/>
+      <c r="I53" s="183"/>
+      <c r="J53" s="184"/>
+      <c r="K53" s="185"/>
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
       <c r="O53" s="22"/>
@@ -9071,11 +9076,11 @@
       <c r="D54" s="33"/>
       <c r="E54" s="33"/>
       <c r="F54" s="32"/>
-      <c r="G54" s="145"/>
-      <c r="H54" s="147"/>
-      <c r="I54" s="181"/>
-      <c r="J54" s="182"/>
-      <c r="K54" s="183"/>
+      <c r="G54" s="146"/>
+      <c r="H54" s="148"/>
+      <c r="I54" s="183"/>
+      <c r="J54" s="184"/>
+      <c r="K54" s="185"/>
       <c r="M54" s="22"/>
       <c r="N54" s="22"/>
       <c r="O54" s="22"/>
@@ -9093,11 +9098,11 @@
       <c r="D55" s="33"/>
       <c r="E55" s="33"/>
       <c r="F55" s="32"/>
-      <c r="G55" s="145"/>
-      <c r="H55" s="147"/>
-      <c r="I55" s="181"/>
-      <c r="J55" s="182"/>
-      <c r="K55" s="183"/>
+      <c r="G55" s="146"/>
+      <c r="H55" s="148"/>
+      <c r="I55" s="183"/>
+      <c r="J55" s="184"/>
+      <c r="K55" s="185"/>
       <c r="M55" s="22"/>
       <c r="N55" s="22"/>
       <c r="O55" s="22"/>
@@ -9115,11 +9120,11 @@
       <c r="D56" s="33"/>
       <c r="E56" s="33"/>
       <c r="F56" s="32"/>
-      <c r="G56" s="145"/>
-      <c r="H56" s="147"/>
-      <c r="I56" s="181"/>
-      <c r="J56" s="182"/>
-      <c r="K56" s="183"/>
+      <c r="G56" s="146"/>
+      <c r="H56" s="148"/>
+      <c r="I56" s="183"/>
+      <c r="J56" s="184"/>
+      <c r="K56" s="185"/>
       <c r="M56" s="22"/>
       <c r="N56" s="22"/>
       <c r="O56" s="22"/>
@@ -9131,25 +9136,80 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="107">
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="I53:K53"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -9164,80 +9224,25 @@
     <mergeCell ref="I17:K17"/>
     <mergeCell ref="I18:K18"/>
     <mergeCell ref="I19:K19"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I49:K49"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="I53:K53"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A1:B2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F56">
@@ -9289,16 +9294,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
+      <c r="H1" s="152"/>
       <c r="I1" s="31" t="s">
         <v>1</v>
       </c>
@@ -9334,14 +9339,14 @@
       <c r="U1" s="52"/>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
       <c r="I2" s="31" t="s">
         <v>2</v>
       </c>
@@ -9454,12 +9459,12 @@
       <c r="J5" s="115" t="s">
         <v>214</v>
       </c>
-      <c r="K5" s="148" t="s">
+      <c r="K5" s="149" t="s">
         <v>284</v>
       </c>
-      <c r="L5" s="149"/>
-      <c r="M5" s="149"/>
-      <c r="N5" s="150"/>
+      <c r="L5" s="150"/>
+      <c r="M5" s="150"/>
+      <c r="N5" s="151"/>
       <c r="O5" s="119" t="s">
         <v>282</v>
       </c>
@@ -9499,12 +9504,12 @@
       <c r="J6" s="115" t="s">
         <v>215</v>
       </c>
-      <c r="K6" s="148" t="s">
+      <c r="K6" s="149" t="s">
         <v>245</v>
       </c>
-      <c r="L6" s="149"/>
-      <c r="M6" s="149"/>
-      <c r="N6" s="150"/>
+      <c r="L6" s="150"/>
+      <c r="M6" s="150"/>
+      <c r="N6" s="151"/>
       <c r="O6" s="119" t="s">
         <v>255</v>
       </c>
@@ -9550,12 +9555,12 @@
       <c r="J7" s="115" t="s">
         <v>216</v>
       </c>
-      <c r="K7" s="148" t="s">
+      <c r="K7" s="149" t="s">
         <v>297</v>
       </c>
-      <c r="L7" s="149"/>
-      <c r="M7" s="149"/>
-      <c r="N7" s="150"/>
+      <c r="L7" s="150"/>
+      <c r="M7" s="150"/>
+      <c r="N7" s="151"/>
       <c r="O7" s="119" t="s">
         <v>298</v>
       </c>
@@ -9603,12 +9608,12 @@
       <c r="J8" s="115" t="s">
         <v>217</v>
       </c>
-      <c r="K8" s="148" t="s">
+      <c r="K8" s="149" t="s">
         <v>302</v>
       </c>
-      <c r="L8" s="149"/>
-      <c r="M8" s="149"/>
-      <c r="N8" s="150"/>
+      <c r="L8" s="150"/>
+      <c r="M8" s="150"/>
+      <c r="N8" s="151"/>
       <c r="O8" s="119" t="s">
         <v>135</v>
       </c>
@@ -9656,12 +9661,12 @@
       <c r="J9" s="115" t="s">
         <v>219</v>
       </c>
-      <c r="K9" s="148" t="s">
+      <c r="K9" s="149" t="s">
         <v>285</v>
       </c>
-      <c r="L9" s="149"/>
-      <c r="M9" s="149"/>
-      <c r="N9" s="150"/>
+      <c r="L9" s="150"/>
+      <c r="M9" s="150"/>
+      <c r="N9" s="151"/>
       <c r="O9" s="119" t="s">
         <v>254</v>
       </c>
@@ -9707,12 +9712,12 @@
       <c r="J10" s="115" t="s">
         <v>269</v>
       </c>
-      <c r="K10" s="148" t="s">
+      <c r="K10" s="149" t="s">
         <v>304</v>
       </c>
-      <c r="L10" s="149"/>
-      <c r="M10" s="149"/>
-      <c r="N10" s="150"/>
+      <c r="L10" s="150"/>
+      <c r="M10" s="150"/>
+      <c r="N10" s="151"/>
       <c r="O10" s="119" t="s">
         <v>305</v>
       </c>
@@ -11825,16 +11830,76 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="96">
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="K91:N91"/>
-    <mergeCell ref="K92:N92"/>
-    <mergeCell ref="K93:N93"/>
-    <mergeCell ref="K94:N94"/>
-    <mergeCell ref="K76:N76"/>
-    <mergeCell ref="K77:N77"/>
-    <mergeCell ref="K78:N78"/>
-    <mergeCell ref="K74:N74"/>
-    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="K31:N31"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="K33:N33"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="K36:N36"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="K38:N38"/>
+    <mergeCell ref="K39:N39"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="K41:N41"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="K45:N45"/>
+    <mergeCell ref="K46:N46"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="K48:N48"/>
+    <mergeCell ref="K60:N60"/>
+    <mergeCell ref="K49:N49"/>
+    <mergeCell ref="K50:N50"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="K52:N52"/>
+    <mergeCell ref="K56:N56"/>
+    <mergeCell ref="K53:N53"/>
+    <mergeCell ref="K54:N54"/>
+    <mergeCell ref="K55:N55"/>
+    <mergeCell ref="K96:N96"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K80:N80"/>
+    <mergeCell ref="K81:N81"/>
+    <mergeCell ref="K82:N82"/>
+    <mergeCell ref="K83:N83"/>
+    <mergeCell ref="K84:N84"/>
+    <mergeCell ref="K85:N85"/>
+    <mergeCell ref="K86:N86"/>
+    <mergeCell ref="K87:N87"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="K71:N71"/>
+    <mergeCell ref="K72:N72"/>
+    <mergeCell ref="K73:N73"/>
+    <mergeCell ref="K44:N44"/>
     <mergeCell ref="K61:N61"/>
     <mergeCell ref="K57:N57"/>
     <mergeCell ref="K58:N58"/>
@@ -11851,76 +11916,16 @@
     <mergeCell ref="K68:N68"/>
     <mergeCell ref="K69:N69"/>
     <mergeCell ref="K70:N70"/>
-    <mergeCell ref="K96:N96"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K80:N80"/>
-    <mergeCell ref="K81:N81"/>
-    <mergeCell ref="K82:N82"/>
-    <mergeCell ref="K83:N83"/>
-    <mergeCell ref="K84:N84"/>
-    <mergeCell ref="K85:N85"/>
-    <mergeCell ref="K86:N86"/>
-    <mergeCell ref="K87:N87"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="K71:N71"/>
-    <mergeCell ref="K72:N72"/>
-    <mergeCell ref="K73:N73"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="K45:N45"/>
-    <mergeCell ref="K46:N46"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="K48:N48"/>
-    <mergeCell ref="K60:N60"/>
-    <mergeCell ref="K49:N49"/>
-    <mergeCell ref="K50:N50"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="K52:N52"/>
-    <mergeCell ref="K56:N56"/>
-    <mergeCell ref="K53:N53"/>
-    <mergeCell ref="K54:N54"/>
-    <mergeCell ref="K55:N55"/>
-    <mergeCell ref="K39:N39"/>
-    <mergeCell ref="K40:N40"/>
-    <mergeCell ref="K41:N41"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="K43:N43"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="K36:N36"/>
-    <mergeCell ref="K37:N37"/>
-    <mergeCell ref="K38:N38"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="K30:N30"/>
-    <mergeCell ref="K31:N31"/>
-    <mergeCell ref="K32:N32"/>
-    <mergeCell ref="K33:N33"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K76:N76"/>
+    <mergeCell ref="K77:N77"/>
+    <mergeCell ref="K78:N78"/>
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="K91:N91"/>
+    <mergeCell ref="K92:N92"/>
+    <mergeCell ref="K93:N93"/>
+    <mergeCell ref="K94:N94"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="Q1048469:Q1048576 Q5:Q96"/>
@@ -11949,7 +11954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A28" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -11967,10 +11972,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
+      <c r="B1" s="152"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -12001,8 +12006,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -13097,10 +13102,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
+      <c r="B1" s="152"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -13128,8 +13133,8 @@
       <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>

</xml_diff>